<commit_message>
First 2 modules completed
Created the dataset to use and ran Decision tree models to predict when to buy and sell.
</commit_message>
<xml_diff>
--- a/notebooks-course/data/BTC-USD.xlsx
+++ b/notebooks-course/data/BTC-USD.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3179"/>
+  <dimension ref="A1:G3383"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -73552,22 +73552,4714 @@
         <v>45076</v>
       </c>
       <c r="B3179" t="n">
-        <v>27751.4609375</v>
+        <v>27745.123046875</v>
       </c>
       <c r="C3179" t="n">
-        <v>27884.162109375</v>
+        <v>28044.759765625</v>
       </c>
       <c r="D3179" t="n">
-        <v>27637.66015625</v>
+        <v>27588.501953125</v>
       </c>
       <c r="E3179" t="n">
-        <v>27871.451171875</v>
+        <v>27702.349609375</v>
       </c>
       <c r="F3179" t="n">
-        <v>27871.451171875</v>
+        <v>27702.349609375</v>
       </c>
       <c r="G3179" t="n">
-        <v>12371207168</v>
+        <v>13251081851</v>
+      </c>
+    </row>
+    <row r="3180">
+      <c r="A3180" s="2" t="n">
+        <v>45077</v>
+      </c>
+      <c r="B3180" t="n">
+        <v>27700.529296875</v>
+      </c>
+      <c r="C3180" t="n">
+        <v>27831.677734375</v>
+      </c>
+      <c r="D3180" t="n">
+        <v>26866.453125</v>
+      </c>
+      <c r="E3180" t="n">
+        <v>27219.658203125</v>
+      </c>
+      <c r="F3180" t="n">
+        <v>27219.658203125</v>
+      </c>
+      <c r="G3180" t="n">
+        <v>15656371534</v>
+      </c>
+    </row>
+    <row r="3181">
+      <c r="A3181" s="2" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B3181" t="n">
+        <v>27218.412109375</v>
+      </c>
+      <c r="C3181" t="n">
+        <v>27346.10546875</v>
+      </c>
+      <c r="D3181" t="n">
+        <v>26671.720703125</v>
+      </c>
+      <c r="E3181" t="n">
+        <v>26819.97265625</v>
+      </c>
+      <c r="F3181" t="n">
+        <v>26819.97265625</v>
+      </c>
+      <c r="G3181" t="n">
+        <v>14678970415</v>
+      </c>
+    </row>
+    <row r="3182">
+      <c r="A3182" s="2" t="n">
+        <v>45079</v>
+      </c>
+      <c r="B3182" t="n">
+        <v>26824.556640625</v>
+      </c>
+      <c r="C3182" t="n">
+        <v>27303.861328125</v>
+      </c>
+      <c r="D3182" t="n">
+        <v>26574.64453125</v>
+      </c>
+      <c r="E3182" t="n">
+        <v>27249.58984375</v>
+      </c>
+      <c r="F3182" t="n">
+        <v>27249.58984375</v>
+      </c>
+      <c r="G3182" t="n">
+        <v>14837415000</v>
+      </c>
+    </row>
+    <row r="3183">
+      <c r="A3183" s="2" t="n">
+        <v>45080</v>
+      </c>
+      <c r="B3183" t="n">
+        <v>27252.32421875</v>
+      </c>
+      <c r="C3183" t="n">
+        <v>27317.052734375</v>
+      </c>
+      <c r="D3183" t="n">
+        <v>26958.00390625</v>
+      </c>
+      <c r="E3183" t="n">
+        <v>27075.12890625</v>
+      </c>
+      <c r="F3183" t="n">
+        <v>27075.12890625</v>
+      </c>
+      <c r="G3183" t="n">
+        <v>8385597470</v>
+      </c>
+    </row>
+    <row r="3184">
+      <c r="A3184" s="2" t="n">
+        <v>45081</v>
+      </c>
+      <c r="B3184" t="n">
+        <v>27075.123046875</v>
+      </c>
+      <c r="C3184" t="n">
+        <v>27407.01953125</v>
+      </c>
+      <c r="D3184" t="n">
+        <v>26968.224609375</v>
+      </c>
+      <c r="E3184" t="n">
+        <v>27119.06640625</v>
+      </c>
+      <c r="F3184" t="n">
+        <v>27119.06640625</v>
+      </c>
+      <c r="G3184" t="n">
+        <v>9360912318</v>
+      </c>
+    </row>
+    <row r="3185">
+      <c r="A3185" s="2" t="n">
+        <v>45082</v>
+      </c>
+      <c r="B3185" t="n">
+        <v>27123.109375</v>
+      </c>
+      <c r="C3185" t="n">
+        <v>27129.982421875</v>
+      </c>
+      <c r="D3185" t="n">
+        <v>25445.16796875</v>
+      </c>
+      <c r="E3185" t="n">
+        <v>25760.09765625</v>
+      </c>
+      <c r="F3185" t="n">
+        <v>25760.09765625</v>
+      </c>
+      <c r="G3185" t="n">
+        <v>21513292646</v>
+      </c>
+    </row>
+    <row r="3186">
+      <c r="A3186" s="2" t="n">
+        <v>45083</v>
+      </c>
+      <c r="B3186" t="n">
+        <v>25732.109375</v>
+      </c>
+      <c r="C3186" t="n">
+        <v>27313.8203125</v>
+      </c>
+      <c r="D3186" t="n">
+        <v>25434.8671875</v>
+      </c>
+      <c r="E3186" t="n">
+        <v>27238.783203125</v>
+      </c>
+      <c r="F3186" t="n">
+        <v>27238.783203125</v>
+      </c>
+      <c r="G3186" t="n">
+        <v>21929670693</v>
+      </c>
+    </row>
+    <row r="3187">
+      <c r="A3187" s="2" t="n">
+        <v>45084</v>
+      </c>
+      <c r="B3187" t="n">
+        <v>27235.650390625</v>
+      </c>
+      <c r="C3187" t="n">
+        <v>27332.181640625</v>
+      </c>
+      <c r="D3187" t="n">
+        <v>26146.98828125</v>
+      </c>
+      <c r="E3187" t="n">
+        <v>26345.998046875</v>
+      </c>
+      <c r="F3187" t="n">
+        <v>26345.998046875</v>
+      </c>
+      <c r="G3187" t="n">
+        <v>19530045082</v>
+      </c>
+    </row>
+    <row r="3188">
+      <c r="A3188" s="2" t="n">
+        <v>45085</v>
+      </c>
+      <c r="B3188" t="n">
+        <v>26347.654296875</v>
+      </c>
+      <c r="C3188" t="n">
+        <v>26797.513671875</v>
+      </c>
+      <c r="D3188" t="n">
+        <v>26246.6640625</v>
+      </c>
+      <c r="E3188" t="n">
+        <v>26508.216796875</v>
+      </c>
+      <c r="F3188" t="n">
+        <v>26508.216796875</v>
+      </c>
+      <c r="G3188" t="n">
+        <v>11904824295</v>
+      </c>
+    </row>
+    <row r="3189">
+      <c r="A3189" s="2" t="n">
+        <v>45086</v>
+      </c>
+      <c r="B3189" t="n">
+        <v>26505.923828125</v>
+      </c>
+      <c r="C3189" t="n">
+        <v>26770.2890625</v>
+      </c>
+      <c r="D3189" t="n">
+        <v>26339.314453125</v>
+      </c>
+      <c r="E3189" t="n">
+        <v>26480.375</v>
+      </c>
+      <c r="F3189" t="n">
+        <v>26480.375</v>
+      </c>
+      <c r="G3189" t="n">
+        <v>11015551640</v>
+      </c>
+    </row>
+    <row r="3190">
+      <c r="A3190" s="2" t="n">
+        <v>45087</v>
+      </c>
+      <c r="B3190" t="n">
+        <v>26481.76171875</v>
+      </c>
+      <c r="C3190" t="n">
+        <v>26531.044921875</v>
+      </c>
+      <c r="D3190" t="n">
+        <v>25501.8359375</v>
+      </c>
+      <c r="E3190" t="n">
+        <v>25851.240234375</v>
+      </c>
+      <c r="F3190" t="n">
+        <v>25851.240234375</v>
+      </c>
+      <c r="G3190" t="n">
+        <v>19872933189</v>
+      </c>
+    </row>
+    <row r="3191">
+      <c r="A3191" s="2" t="n">
+        <v>45088</v>
+      </c>
+      <c r="B3191" t="n">
+        <v>25854.03125</v>
+      </c>
+      <c r="C3191" t="n">
+        <v>26203.439453125</v>
+      </c>
+      <c r="D3191" t="n">
+        <v>25668.986328125</v>
+      </c>
+      <c r="E3191" t="n">
+        <v>25940.16796875</v>
+      </c>
+      <c r="F3191" t="n">
+        <v>25940.16796875</v>
+      </c>
+      <c r="G3191" t="n">
+        <v>10732609603</v>
+      </c>
+    </row>
+    <row r="3192">
+      <c r="A3192" s="2" t="n">
+        <v>45089</v>
+      </c>
+      <c r="B3192" t="n">
+        <v>25934.28515625</v>
+      </c>
+      <c r="C3192" t="n">
+        <v>26087.919921875</v>
+      </c>
+      <c r="D3192" t="n">
+        <v>25675.197265625</v>
+      </c>
+      <c r="E3192" t="n">
+        <v>25902.5</v>
+      </c>
+      <c r="F3192" t="n">
+        <v>25902.5</v>
+      </c>
+      <c r="G3192" t="n">
+        <v>11677889997</v>
+      </c>
+    </row>
+    <row r="3193">
+      <c r="A3193" s="2" t="n">
+        <v>45090</v>
+      </c>
+      <c r="B3193" t="n">
+        <v>25902.94140625</v>
+      </c>
+      <c r="C3193" t="n">
+        <v>26376.3515625</v>
+      </c>
+      <c r="D3193" t="n">
+        <v>25728.365234375</v>
+      </c>
+      <c r="E3193" t="n">
+        <v>25918.728515625</v>
+      </c>
+      <c r="F3193" t="n">
+        <v>25918.728515625</v>
+      </c>
+      <c r="G3193" t="n">
+        <v>14143474486</v>
+      </c>
+    </row>
+    <row r="3194">
+      <c r="A3194" s="2" t="n">
+        <v>45091</v>
+      </c>
+      <c r="B3194" t="n">
+        <v>25920.2578125</v>
+      </c>
+      <c r="C3194" t="n">
+        <v>26041.80078125</v>
+      </c>
+      <c r="D3194" t="n">
+        <v>24902.15234375</v>
+      </c>
+      <c r="E3194" t="n">
+        <v>25124.67578125</v>
+      </c>
+      <c r="F3194" t="n">
+        <v>25124.67578125</v>
+      </c>
+      <c r="G3194" t="n">
+        <v>14265717766</v>
+      </c>
+    </row>
+    <row r="3195">
+      <c r="A3195" s="2" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B3195" t="n">
+        <v>25121.673828125</v>
+      </c>
+      <c r="C3195" t="n">
+        <v>25735.30859375</v>
+      </c>
+      <c r="D3195" t="n">
+        <v>24797.16796875</v>
+      </c>
+      <c r="E3195" t="n">
+        <v>25576.39453125</v>
+      </c>
+      <c r="F3195" t="n">
+        <v>25576.39453125</v>
+      </c>
+      <c r="G3195" t="n">
+        <v>15837384409</v>
+      </c>
+    </row>
+    <row r="3196">
+      <c r="A3196" s="2" t="n">
+        <v>45093</v>
+      </c>
+      <c r="B3196" t="n">
+        <v>25575.283203125</v>
+      </c>
+      <c r="C3196" t="n">
+        <v>26463.173828125</v>
+      </c>
+      <c r="D3196" t="n">
+        <v>25245.357421875</v>
+      </c>
+      <c r="E3196" t="n">
+        <v>26327.462890625</v>
+      </c>
+      <c r="F3196" t="n">
+        <v>26327.462890625</v>
+      </c>
+      <c r="G3196" t="n">
+        <v>16324646965</v>
+      </c>
+    </row>
+    <row r="3197">
+      <c r="A3197" s="2" t="n">
+        <v>45094</v>
+      </c>
+      <c r="B3197" t="n">
+        <v>26328.6796875</v>
+      </c>
+      <c r="C3197" t="n">
+        <v>26769.39453125</v>
+      </c>
+      <c r="D3197" t="n">
+        <v>26174.4921875</v>
+      </c>
+      <c r="E3197" t="n">
+        <v>26510.67578125</v>
+      </c>
+      <c r="F3197" t="n">
+        <v>26510.67578125</v>
+      </c>
+      <c r="G3197" t="n">
+        <v>11090276850</v>
+      </c>
+    </row>
+    <row r="3198">
+      <c r="A3198" s="2" t="n">
+        <v>45095</v>
+      </c>
+      <c r="B3198" t="n">
+        <v>26510.45703125</v>
+      </c>
+      <c r="C3198" t="n">
+        <v>26675.92578125</v>
+      </c>
+      <c r="D3198" t="n">
+        <v>26325.890625</v>
+      </c>
+      <c r="E3198" t="n">
+        <v>26336.212890625</v>
+      </c>
+      <c r="F3198" t="n">
+        <v>26336.212890625</v>
+      </c>
+      <c r="G3198" t="n">
+        <v>9565695129</v>
+      </c>
+    </row>
+    <row r="3199">
+      <c r="A3199" s="2" t="n">
+        <v>45096</v>
+      </c>
+      <c r="B3199" t="n">
+        <v>26335.44140625</v>
+      </c>
+      <c r="C3199" t="n">
+        <v>26984.611328125</v>
+      </c>
+      <c r="D3199" t="n">
+        <v>26312.83203125</v>
+      </c>
+      <c r="E3199" t="n">
+        <v>26851.029296875</v>
+      </c>
+      <c r="F3199" t="n">
+        <v>26851.029296875</v>
+      </c>
+      <c r="G3199" t="n">
+        <v>12826986222</v>
+      </c>
+    </row>
+    <row r="3200">
+      <c r="A3200" s="2" t="n">
+        <v>45097</v>
+      </c>
+      <c r="B3200" t="n">
+        <v>26841.6640625</v>
+      </c>
+      <c r="C3200" t="n">
+        <v>28388.96875</v>
+      </c>
+      <c r="D3200" t="n">
+        <v>26668.791015625</v>
+      </c>
+      <c r="E3200" t="n">
+        <v>28327.48828125</v>
+      </c>
+      <c r="F3200" t="n">
+        <v>28327.48828125</v>
+      </c>
+      <c r="G3200" t="n">
+        <v>22211859147</v>
+      </c>
+    </row>
+    <row r="3201">
+      <c r="A3201" s="2" t="n">
+        <v>45098</v>
+      </c>
+      <c r="B3201" t="n">
+        <v>28311.310546875</v>
+      </c>
+      <c r="C3201" t="n">
+        <v>30737.330078125</v>
+      </c>
+      <c r="D3201" t="n">
+        <v>28283.41015625</v>
+      </c>
+      <c r="E3201" t="n">
+        <v>30027.296875</v>
+      </c>
+      <c r="F3201" t="n">
+        <v>30027.296875</v>
+      </c>
+      <c r="G3201" t="n">
+        <v>33346760979</v>
+      </c>
+    </row>
+    <row r="3202">
+      <c r="A3202" s="2" t="n">
+        <v>45099</v>
+      </c>
+      <c r="B3202" t="n">
+        <v>29995.935546875</v>
+      </c>
+      <c r="C3202" t="n">
+        <v>30495.998046875</v>
+      </c>
+      <c r="D3202" t="n">
+        <v>29679.158203125</v>
+      </c>
+      <c r="E3202" t="n">
+        <v>29912.28125</v>
+      </c>
+      <c r="F3202" t="n">
+        <v>29912.28125</v>
+      </c>
+      <c r="G3202" t="n">
+        <v>20653160491</v>
+      </c>
+    </row>
+    <row r="3203">
+      <c r="A3203" s="2" t="n">
+        <v>45100</v>
+      </c>
+      <c r="B3203" t="n">
+        <v>29896.3828125</v>
+      </c>
+      <c r="C3203" t="n">
+        <v>31389.5390625</v>
+      </c>
+      <c r="D3203" t="n">
+        <v>29845.21484375</v>
+      </c>
+      <c r="E3203" t="n">
+        <v>30695.46875</v>
+      </c>
+      <c r="F3203" t="n">
+        <v>30695.46875</v>
+      </c>
+      <c r="G3203" t="n">
+        <v>24115570085</v>
+      </c>
+    </row>
+    <row r="3204">
+      <c r="A3204" s="2" t="n">
+        <v>45101</v>
+      </c>
+      <c r="B3204" t="n">
+        <v>30708.73828125</v>
+      </c>
+      <c r="C3204" t="n">
+        <v>30804.1484375</v>
+      </c>
+      <c r="D3204" t="n">
+        <v>30290.146484375</v>
+      </c>
+      <c r="E3204" t="n">
+        <v>30548.6953125</v>
+      </c>
+      <c r="F3204" t="n">
+        <v>30548.6953125</v>
+      </c>
+      <c r="G3204" t="n">
+        <v>12147822496</v>
+      </c>
+    </row>
+    <row r="3205">
+      <c r="A3205" s="2" t="n">
+        <v>45102</v>
+      </c>
+      <c r="B3205" t="n">
+        <v>30545.150390625</v>
+      </c>
+      <c r="C3205" t="n">
+        <v>31041.271484375</v>
+      </c>
+      <c r="D3205" t="n">
+        <v>30327.943359375</v>
+      </c>
+      <c r="E3205" t="n">
+        <v>30480.26171875</v>
+      </c>
+      <c r="F3205" t="n">
+        <v>30480.26171875</v>
+      </c>
+      <c r="G3205" t="n">
+        <v>12703464114</v>
+      </c>
+    </row>
+    <row r="3206">
+      <c r="A3206" s="2" t="n">
+        <v>45103</v>
+      </c>
+      <c r="B3206" t="n">
+        <v>30480.5234375</v>
+      </c>
+      <c r="C3206" t="n">
+        <v>30636.029296875</v>
+      </c>
+      <c r="D3206" t="n">
+        <v>29955.744140625</v>
+      </c>
+      <c r="E3206" t="n">
+        <v>30271.130859375</v>
+      </c>
+      <c r="F3206" t="n">
+        <v>30271.130859375</v>
+      </c>
+      <c r="G3206" t="n">
+        <v>16493186997</v>
+      </c>
+    </row>
+    <row r="3207">
+      <c r="A3207" s="2" t="n">
+        <v>45104</v>
+      </c>
+      <c r="B3207" t="n">
+        <v>30274.3203125</v>
+      </c>
+      <c r="C3207" t="n">
+        <v>31006.787109375</v>
+      </c>
+      <c r="D3207" t="n">
+        <v>30236.650390625</v>
+      </c>
+      <c r="E3207" t="n">
+        <v>30688.1640625</v>
+      </c>
+      <c r="F3207" t="n">
+        <v>30688.1640625</v>
+      </c>
+      <c r="G3207" t="n">
+        <v>16428827944</v>
+      </c>
+    </row>
+    <row r="3208">
+      <c r="A3208" s="2" t="n">
+        <v>45105</v>
+      </c>
+      <c r="B3208" t="n">
+        <v>30696.560546875</v>
+      </c>
+      <c r="C3208" t="n">
+        <v>30703.279296875</v>
+      </c>
+      <c r="D3208" t="n">
+        <v>29921.822265625</v>
+      </c>
+      <c r="E3208" t="n">
+        <v>30086.24609375</v>
+      </c>
+      <c r="F3208" t="n">
+        <v>30086.24609375</v>
+      </c>
+      <c r="G3208" t="n">
+        <v>14571500779</v>
+      </c>
+    </row>
+    <row r="3209">
+      <c r="A3209" s="2" t="n">
+        <v>45106</v>
+      </c>
+      <c r="B3209" t="n">
+        <v>30086.1875</v>
+      </c>
+      <c r="C3209" t="n">
+        <v>30796.25</v>
+      </c>
+      <c r="D3209" t="n">
+        <v>30057.203125</v>
+      </c>
+      <c r="E3209" t="n">
+        <v>30445.3515625</v>
+      </c>
+      <c r="F3209" t="n">
+        <v>30445.3515625</v>
+      </c>
+      <c r="G3209" t="n">
+        <v>13180860821</v>
+      </c>
+    </row>
+    <row r="3210">
+      <c r="A3210" s="2" t="n">
+        <v>45107</v>
+      </c>
+      <c r="B3210" t="n">
+        <v>30441.353515625</v>
+      </c>
+      <c r="C3210" t="n">
+        <v>31256.86328125</v>
+      </c>
+      <c r="D3210" t="n">
+        <v>29600.275390625</v>
+      </c>
+      <c r="E3210" t="n">
+        <v>30477.251953125</v>
+      </c>
+      <c r="F3210" t="n">
+        <v>30477.251953125</v>
+      </c>
+      <c r="G3210" t="n">
+        <v>26387306197</v>
+      </c>
+    </row>
+    <row r="3211">
+      <c r="A3211" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B3211" t="n">
+        <v>30471.84765625</v>
+      </c>
+      <c r="C3211" t="n">
+        <v>30641.2890625</v>
+      </c>
+      <c r="D3211" t="n">
+        <v>30328.865234375</v>
+      </c>
+      <c r="E3211" t="n">
+        <v>30590.078125</v>
+      </c>
+      <c r="F3211" t="n">
+        <v>30590.078125</v>
+      </c>
+      <c r="G3211" t="n">
+        <v>9086606733</v>
+      </c>
+    </row>
+    <row r="3212">
+      <c r="A3212" s="2" t="n">
+        <v>45109</v>
+      </c>
+      <c r="B3212" t="n">
+        <v>30587.26953125</v>
+      </c>
+      <c r="C3212" t="n">
+        <v>30766.140625</v>
+      </c>
+      <c r="D3212" t="n">
+        <v>30264.01953125</v>
+      </c>
+      <c r="E3212" t="n">
+        <v>30620.76953125</v>
+      </c>
+      <c r="F3212" t="n">
+        <v>30620.76953125</v>
+      </c>
+      <c r="G3212" t="n">
+        <v>10533418042</v>
+      </c>
+    </row>
+    <row r="3213">
+      <c r="A3213" s="2" t="n">
+        <v>45110</v>
+      </c>
+      <c r="B3213" t="n">
+        <v>30624.515625</v>
+      </c>
+      <c r="C3213" t="n">
+        <v>31375.61328125</v>
+      </c>
+      <c r="D3213" t="n">
+        <v>30586.513671875</v>
+      </c>
+      <c r="E3213" t="n">
+        <v>31156.439453125</v>
+      </c>
+      <c r="F3213" t="n">
+        <v>31156.439453125</v>
+      </c>
+      <c r="G3213" t="n">
+        <v>15271884873</v>
+      </c>
+    </row>
+    <row r="3214">
+      <c r="A3214" s="2" t="n">
+        <v>45111</v>
+      </c>
+      <c r="B3214" t="n">
+        <v>31156.865234375</v>
+      </c>
+      <c r="C3214" t="n">
+        <v>31325.197265625</v>
+      </c>
+      <c r="D3214" t="n">
+        <v>30659.35546875</v>
+      </c>
+      <c r="E3214" t="n">
+        <v>30777.58203125</v>
+      </c>
+      <c r="F3214" t="n">
+        <v>30777.58203125</v>
+      </c>
+      <c r="G3214" t="n">
+        <v>12810828427</v>
+      </c>
+    </row>
+    <row r="3215">
+      <c r="A3215" s="2" t="n">
+        <v>45112</v>
+      </c>
+      <c r="B3215" t="n">
+        <v>30778.724609375</v>
+      </c>
+      <c r="C3215" t="n">
+        <v>30877.330078125</v>
+      </c>
+      <c r="D3215" t="n">
+        <v>30225.61328125</v>
+      </c>
+      <c r="E3215" t="n">
+        <v>30514.166015625</v>
+      </c>
+      <c r="F3215" t="n">
+        <v>30514.166015625</v>
+      </c>
+      <c r="G3215" t="n">
+        <v>12481622280</v>
+      </c>
+    </row>
+    <row r="3216">
+      <c r="A3216" s="2" t="n">
+        <v>45113</v>
+      </c>
+      <c r="B3216" t="n">
+        <v>30507.150390625</v>
+      </c>
+      <c r="C3216" t="n">
+        <v>31460.052734375</v>
+      </c>
+      <c r="D3216" t="n">
+        <v>29892.2265625</v>
+      </c>
+      <c r="E3216" t="n">
+        <v>29909.337890625</v>
+      </c>
+      <c r="F3216" t="n">
+        <v>29909.337890625</v>
+      </c>
+      <c r="G3216" t="n">
+        <v>21129219509</v>
+      </c>
+    </row>
+    <row r="3217">
+      <c r="A3217" s="2" t="n">
+        <v>45114</v>
+      </c>
+      <c r="B3217" t="n">
+        <v>29907.998046875</v>
+      </c>
+      <c r="C3217" t="n">
+        <v>30434.64453125</v>
+      </c>
+      <c r="D3217" t="n">
+        <v>29777.28515625</v>
+      </c>
+      <c r="E3217" t="n">
+        <v>30342.265625</v>
+      </c>
+      <c r="F3217" t="n">
+        <v>30342.265625</v>
+      </c>
+      <c r="G3217" t="n">
+        <v>13384770155</v>
+      </c>
+    </row>
+    <row r="3218">
+      <c r="A3218" s="2" t="n">
+        <v>45115</v>
+      </c>
+      <c r="B3218" t="n">
+        <v>30346.921875</v>
+      </c>
+      <c r="C3218" t="n">
+        <v>30374.4375</v>
+      </c>
+      <c r="D3218" t="n">
+        <v>30080.16015625</v>
+      </c>
+      <c r="E3218" t="n">
+        <v>30292.541015625</v>
+      </c>
+      <c r="F3218" t="n">
+        <v>30292.541015625</v>
+      </c>
+      <c r="G3218" t="n">
+        <v>7509378699</v>
+      </c>
+    </row>
+    <row r="3219">
+      <c r="A3219" s="2" t="n">
+        <v>45116</v>
+      </c>
+      <c r="B3219" t="n">
+        <v>30291.611328125</v>
+      </c>
+      <c r="C3219" t="n">
+        <v>30427.58984375</v>
+      </c>
+      <c r="D3219" t="n">
+        <v>30085.591796875</v>
+      </c>
+      <c r="E3219" t="n">
+        <v>30171.234375</v>
+      </c>
+      <c r="F3219" t="n">
+        <v>30171.234375</v>
+      </c>
+      <c r="G3219" t="n">
+        <v>7903327692</v>
+      </c>
+    </row>
+    <row r="3220">
+      <c r="A3220" s="2" t="n">
+        <v>45117</v>
+      </c>
+      <c r="B3220" t="n">
+        <v>30172.423828125</v>
+      </c>
+      <c r="C3220" t="n">
+        <v>31026.083984375</v>
+      </c>
+      <c r="D3220" t="n">
+        <v>29985.39453125</v>
+      </c>
+      <c r="E3220" t="n">
+        <v>30414.470703125</v>
+      </c>
+      <c r="F3220" t="n">
+        <v>30414.470703125</v>
+      </c>
+      <c r="G3220" t="n">
+        <v>14828209155</v>
+      </c>
+    </row>
+    <row r="3221">
+      <c r="A3221" s="2" t="n">
+        <v>45118</v>
+      </c>
+      <c r="B3221" t="n">
+        <v>30417.6328125</v>
+      </c>
+      <c r="C3221" t="n">
+        <v>30788.314453125</v>
+      </c>
+      <c r="D3221" t="n">
+        <v>30358.09765625</v>
+      </c>
+      <c r="E3221" t="n">
+        <v>30620.951171875</v>
+      </c>
+      <c r="F3221" t="n">
+        <v>30620.951171875</v>
+      </c>
+      <c r="G3221" t="n">
+        <v>12151839152</v>
+      </c>
+    </row>
+    <row r="3222">
+      <c r="A3222" s="2" t="n">
+        <v>45119</v>
+      </c>
+      <c r="B3222" t="n">
+        <v>30622.24609375</v>
+      </c>
+      <c r="C3222" t="n">
+        <v>30959.96484375</v>
+      </c>
+      <c r="D3222" t="n">
+        <v>30228.8359375</v>
+      </c>
+      <c r="E3222" t="n">
+        <v>30391.646484375</v>
+      </c>
+      <c r="F3222" t="n">
+        <v>30391.646484375</v>
+      </c>
+      <c r="G3222" t="n">
+        <v>14805659717</v>
+      </c>
+    </row>
+    <row r="3223">
+      <c r="A3223" s="2" t="n">
+        <v>45120</v>
+      </c>
+      <c r="B3223" t="n">
+        <v>30387.48828125</v>
+      </c>
+      <c r="C3223" t="n">
+        <v>31814.515625</v>
+      </c>
+      <c r="D3223" t="n">
+        <v>30268.3515625</v>
+      </c>
+      <c r="E3223" t="n">
+        <v>31476.048828125</v>
+      </c>
+      <c r="F3223" t="n">
+        <v>31476.048828125</v>
+      </c>
+      <c r="G3223" t="n">
+        <v>23686079548</v>
+      </c>
+    </row>
+    <row r="3224">
+      <c r="A3224" s="2" t="n">
+        <v>45121</v>
+      </c>
+      <c r="B3224" t="n">
+        <v>31474.720703125</v>
+      </c>
+      <c r="C3224" t="n">
+        <v>31582.25390625</v>
+      </c>
+      <c r="D3224" t="n">
+        <v>29966.38671875</v>
+      </c>
+      <c r="E3224" t="n">
+        <v>30334.068359375</v>
+      </c>
+      <c r="F3224" t="n">
+        <v>30334.068359375</v>
+      </c>
+      <c r="G3224" t="n">
+        <v>20917902660</v>
+      </c>
+    </row>
+    <row r="3225">
+      <c r="A3225" s="2" t="n">
+        <v>45122</v>
+      </c>
+      <c r="B3225" t="n">
+        <v>30331.783203125</v>
+      </c>
+      <c r="C3225" t="n">
+        <v>30407.78125</v>
+      </c>
+      <c r="D3225" t="n">
+        <v>30263.462890625</v>
+      </c>
+      <c r="E3225" t="n">
+        <v>30295.806640625</v>
+      </c>
+      <c r="F3225" t="n">
+        <v>30295.806640625</v>
+      </c>
+      <c r="G3225" t="n">
+        <v>8011667756</v>
+      </c>
+    </row>
+    <row r="3226">
+      <c r="A3226" s="2" t="n">
+        <v>45123</v>
+      </c>
+      <c r="B3226" t="n">
+        <v>30297.47265625</v>
+      </c>
+      <c r="C3226" t="n">
+        <v>30437.560546875</v>
+      </c>
+      <c r="D3226" t="n">
+        <v>30089.669921875</v>
+      </c>
+      <c r="E3226" t="n">
+        <v>30249.1328125</v>
+      </c>
+      <c r="F3226" t="n">
+        <v>30249.1328125</v>
+      </c>
+      <c r="G3226" t="n">
+        <v>8516564470</v>
+      </c>
+    </row>
+    <row r="3227">
+      <c r="A3227" s="2" t="n">
+        <v>45124</v>
+      </c>
+      <c r="B3227" t="n">
+        <v>30249.626953125</v>
+      </c>
+      <c r="C3227" t="n">
+        <v>30336.400390625</v>
+      </c>
+      <c r="D3227" t="n">
+        <v>29685.783203125</v>
+      </c>
+      <c r="E3227" t="n">
+        <v>30145.888671875</v>
+      </c>
+      <c r="F3227" t="n">
+        <v>30145.888671875</v>
+      </c>
+      <c r="G3227" t="n">
+        <v>13240156074</v>
+      </c>
+    </row>
+    <row r="3228">
+      <c r="A3228" s="2" t="n">
+        <v>45125</v>
+      </c>
+      <c r="B3228" t="n">
+        <v>30147.0703125</v>
+      </c>
+      <c r="C3228" t="n">
+        <v>30233.65625</v>
+      </c>
+      <c r="D3228" t="n">
+        <v>29556.427734375</v>
+      </c>
+      <c r="E3228" t="n">
+        <v>29856.5625</v>
+      </c>
+      <c r="F3228" t="n">
+        <v>29856.5625</v>
+      </c>
+      <c r="G3228" t="n">
+        <v>13138897269</v>
+      </c>
+    </row>
+    <row r="3229">
+      <c r="A3229" s="2" t="n">
+        <v>45126</v>
+      </c>
+      <c r="B3229" t="n">
+        <v>29862.046875</v>
+      </c>
+      <c r="C3229" t="n">
+        <v>30184.181640625</v>
+      </c>
+      <c r="D3229" t="n">
+        <v>29794.26953125</v>
+      </c>
+      <c r="E3229" t="n">
+        <v>29913.923828125</v>
+      </c>
+      <c r="F3229" t="n">
+        <v>29913.923828125</v>
+      </c>
+      <c r="G3229" t="n">
+        <v>12128602812</v>
+      </c>
+    </row>
+    <row r="3230">
+      <c r="A3230" s="2" t="n">
+        <v>45127</v>
+      </c>
+      <c r="B3230" t="n">
+        <v>29915.25</v>
+      </c>
+      <c r="C3230" t="n">
+        <v>30195.53125</v>
+      </c>
+      <c r="D3230" t="n">
+        <v>29638.095703125</v>
+      </c>
+      <c r="E3230" t="n">
+        <v>29792.015625</v>
+      </c>
+      <c r="F3230" t="n">
+        <v>29792.015625</v>
+      </c>
+      <c r="G3230" t="n">
+        <v>14655207121</v>
+      </c>
+    </row>
+    <row r="3231">
+      <c r="A3231" s="2" t="n">
+        <v>45128</v>
+      </c>
+      <c r="B3231" t="n">
+        <v>29805.111328125</v>
+      </c>
+      <c r="C3231" t="n">
+        <v>30045.998046875</v>
+      </c>
+      <c r="D3231" t="n">
+        <v>29733.8515625</v>
+      </c>
+      <c r="E3231" t="n">
+        <v>29908.744140625</v>
+      </c>
+      <c r="F3231" t="n">
+        <v>29908.744140625</v>
+      </c>
+      <c r="G3231" t="n">
+        <v>10972789818</v>
+      </c>
+    </row>
+    <row r="3232">
+      <c r="A3232" s="2" t="n">
+        <v>45129</v>
+      </c>
+      <c r="B3232" t="n">
+        <v>29908.697265625</v>
+      </c>
+      <c r="C3232" t="n">
+        <v>29991.615234375</v>
+      </c>
+      <c r="D3232" t="n">
+        <v>29664.12109375</v>
+      </c>
+      <c r="E3232" t="n">
+        <v>29771.802734375</v>
+      </c>
+      <c r="F3232" t="n">
+        <v>29771.802734375</v>
+      </c>
+      <c r="G3232" t="n">
+        <v>7873300598</v>
+      </c>
+    </row>
+    <row r="3233">
+      <c r="A3233" s="2" t="n">
+        <v>45130</v>
+      </c>
+      <c r="B3233" t="n">
+        <v>29790.111328125</v>
+      </c>
+      <c r="C3233" t="n">
+        <v>30330.640625</v>
+      </c>
+      <c r="D3233" t="n">
+        <v>29741.52734375</v>
+      </c>
+      <c r="E3233" t="n">
+        <v>30084.5390625</v>
+      </c>
+      <c r="F3233" t="n">
+        <v>30084.5390625</v>
+      </c>
+      <c r="G3233" t="n">
+        <v>9220145050</v>
+      </c>
+    </row>
+    <row r="3234">
+      <c r="A3234" s="2" t="n">
+        <v>45131</v>
+      </c>
+      <c r="B3234" t="n">
+        <v>30081.662109375</v>
+      </c>
+      <c r="C3234" t="n">
+        <v>30093.39453125</v>
+      </c>
+      <c r="D3234" t="n">
+        <v>28934.294921875</v>
+      </c>
+      <c r="E3234" t="n">
+        <v>29176.916015625</v>
+      </c>
+      <c r="F3234" t="n">
+        <v>29176.916015625</v>
+      </c>
+      <c r="G3234" t="n">
+        <v>15395817395</v>
+      </c>
+    </row>
+    <row r="3235">
+      <c r="A3235" s="2" t="n">
+        <v>45132</v>
+      </c>
+      <c r="B3235" t="n">
+        <v>29178.970703125</v>
+      </c>
+      <c r="C3235" t="n">
+        <v>29353.16015625</v>
+      </c>
+      <c r="D3235" t="n">
+        <v>29062.43359375</v>
+      </c>
+      <c r="E3235" t="n">
+        <v>29227.390625</v>
+      </c>
+      <c r="F3235" t="n">
+        <v>29227.390625</v>
+      </c>
+      <c r="G3235" t="n">
+        <v>10266772793</v>
+      </c>
+    </row>
+    <row r="3236">
+      <c r="A3236" s="2" t="n">
+        <v>45133</v>
+      </c>
+      <c r="B3236" t="n">
+        <v>29225.759765625</v>
+      </c>
+      <c r="C3236" t="n">
+        <v>29675.552734375</v>
+      </c>
+      <c r="D3236" t="n">
+        <v>29113.912109375</v>
+      </c>
+      <c r="E3236" t="n">
+        <v>29354.97265625</v>
+      </c>
+      <c r="F3236" t="n">
+        <v>29354.97265625</v>
+      </c>
+      <c r="G3236" t="n">
+        <v>13497554655</v>
+      </c>
+    </row>
+    <row r="3237">
+      <c r="A3237" s="2" t="n">
+        <v>45134</v>
+      </c>
+      <c r="B3237" t="n">
+        <v>29353.798828125</v>
+      </c>
+      <c r="C3237" t="n">
+        <v>29560.966796875</v>
+      </c>
+      <c r="D3237" t="n">
+        <v>29099.3515625</v>
+      </c>
+      <c r="E3237" t="n">
+        <v>29210.689453125</v>
+      </c>
+      <c r="F3237" t="n">
+        <v>29210.689453125</v>
+      </c>
+      <c r="G3237" t="n">
+        <v>10770779217</v>
+      </c>
+    </row>
+    <row r="3238">
+      <c r="A3238" s="2" t="n">
+        <v>45135</v>
+      </c>
+      <c r="B3238" t="n">
+        <v>29212.1640625</v>
+      </c>
+      <c r="C3238" t="n">
+        <v>29521.513671875</v>
+      </c>
+      <c r="D3238" t="n">
+        <v>29125.845703125</v>
+      </c>
+      <c r="E3238" t="n">
+        <v>29319.24609375</v>
+      </c>
+      <c r="F3238" t="n">
+        <v>29319.24609375</v>
+      </c>
+      <c r="G3238" t="n">
+        <v>11218474952</v>
+      </c>
+    </row>
+    <row r="3239">
+      <c r="A3239" s="2" t="n">
+        <v>45136</v>
+      </c>
+      <c r="B3239" t="n">
+        <v>29319.4453125</v>
+      </c>
+      <c r="C3239" t="n">
+        <v>29396.84375</v>
+      </c>
+      <c r="D3239" t="n">
+        <v>29264.166015625</v>
+      </c>
+      <c r="E3239" t="n">
+        <v>29356.91796875</v>
+      </c>
+      <c r="F3239" t="n">
+        <v>29356.91796875</v>
+      </c>
+      <c r="G3239" t="n">
+        <v>6481775959</v>
+      </c>
+    </row>
+    <row r="3240">
+      <c r="A3240" s="2" t="n">
+        <v>45137</v>
+      </c>
+      <c r="B3240" t="n">
+        <v>29357.09375</v>
+      </c>
+      <c r="C3240" t="n">
+        <v>29443.169921875</v>
+      </c>
+      <c r="D3240" t="n">
+        <v>29059.501953125</v>
+      </c>
+      <c r="E3240" t="n">
+        <v>29275.30859375</v>
+      </c>
+      <c r="F3240" t="n">
+        <v>29275.30859375</v>
+      </c>
+      <c r="G3240" t="n">
+        <v>8678454527</v>
+      </c>
+    </row>
+    <row r="3241">
+      <c r="A3241" s="2" t="n">
+        <v>45138</v>
+      </c>
+      <c r="B3241" t="n">
+        <v>29278.314453125</v>
+      </c>
+      <c r="C3241" t="n">
+        <v>29489.873046875</v>
+      </c>
+      <c r="D3241" t="n">
+        <v>29131.578125</v>
+      </c>
+      <c r="E3241" t="n">
+        <v>29230.111328125</v>
+      </c>
+      <c r="F3241" t="n">
+        <v>29230.111328125</v>
+      </c>
+      <c r="G3241" t="n">
+        <v>11656781982</v>
+      </c>
+    </row>
+    <row r="3242">
+      <c r="A3242" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B3242" t="n">
+        <v>29230.873046875</v>
+      </c>
+      <c r="C3242" t="n">
+        <v>29675.732421875</v>
+      </c>
+      <c r="D3242" t="n">
+        <v>28657.0234375</v>
+      </c>
+      <c r="E3242" t="n">
+        <v>29675.732421875</v>
+      </c>
+      <c r="F3242" t="n">
+        <v>29675.732421875</v>
+      </c>
+      <c r="G3242" t="n">
+        <v>18272392391</v>
+      </c>
+    </row>
+    <row r="3243">
+      <c r="A3243" s="2" t="n">
+        <v>45140</v>
+      </c>
+      <c r="B3243" t="n">
+        <v>29704.146484375</v>
+      </c>
+      <c r="C3243" t="n">
+        <v>29987.998046875</v>
+      </c>
+      <c r="D3243" t="n">
+        <v>28946.509765625</v>
+      </c>
+      <c r="E3243" t="n">
+        <v>29151.958984375</v>
+      </c>
+      <c r="F3243" t="n">
+        <v>29151.958984375</v>
+      </c>
+      <c r="G3243" t="n">
+        <v>19212655598</v>
+      </c>
+    </row>
+    <row r="3244">
+      <c r="A3244" s="2" t="n">
+        <v>45141</v>
+      </c>
+      <c r="B3244" t="n">
+        <v>29161.8125</v>
+      </c>
+      <c r="C3244" t="n">
+        <v>29375.70703125</v>
+      </c>
+      <c r="D3244" t="n">
+        <v>28959.48828125</v>
+      </c>
+      <c r="E3244" t="n">
+        <v>29178.6796875</v>
+      </c>
+      <c r="F3244" t="n">
+        <v>29178.6796875</v>
+      </c>
+      <c r="G3244" t="n">
+        <v>12780357746</v>
+      </c>
+    </row>
+    <row r="3245">
+      <c r="A3245" s="2" t="n">
+        <v>45142</v>
+      </c>
+      <c r="B3245" t="n">
+        <v>29174.3828125</v>
+      </c>
+      <c r="C3245" t="n">
+        <v>29302.078125</v>
+      </c>
+      <c r="D3245" t="n">
+        <v>28885.3359375</v>
+      </c>
+      <c r="E3245" t="n">
+        <v>29074.091796875</v>
+      </c>
+      <c r="F3245" t="n">
+        <v>29074.091796875</v>
+      </c>
+      <c r="G3245" t="n">
+        <v>12036639988</v>
+      </c>
+    </row>
+    <row r="3246">
+      <c r="A3246" s="2" t="n">
+        <v>45143</v>
+      </c>
+      <c r="B3246" t="n">
+        <v>29075.388671875</v>
+      </c>
+      <c r="C3246" t="n">
+        <v>29102.46484375</v>
+      </c>
+      <c r="D3246" t="n">
+        <v>28957.796875</v>
+      </c>
+      <c r="E3246" t="n">
+        <v>29042.126953125</v>
+      </c>
+      <c r="F3246" t="n">
+        <v>29042.126953125</v>
+      </c>
+      <c r="G3246" t="n">
+        <v>6598366353</v>
+      </c>
+    </row>
+    <row r="3247">
+      <c r="A3247" s="2" t="n">
+        <v>45144</v>
+      </c>
+      <c r="B3247" t="n">
+        <v>29043.701171875</v>
+      </c>
+      <c r="C3247" t="n">
+        <v>29160.822265625</v>
+      </c>
+      <c r="D3247" t="n">
+        <v>28963.833984375</v>
+      </c>
+      <c r="E3247" t="n">
+        <v>29041.85546875</v>
+      </c>
+      <c r="F3247" t="n">
+        <v>29041.85546875</v>
+      </c>
+      <c r="G3247" t="n">
+        <v>7269806994</v>
+      </c>
+    </row>
+    <row r="3248">
+      <c r="A3248" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="B3248" t="n">
+        <v>29038.513671875</v>
+      </c>
+      <c r="C3248" t="n">
+        <v>29244.28125</v>
+      </c>
+      <c r="D3248" t="n">
+        <v>28724.140625</v>
+      </c>
+      <c r="E3248" t="n">
+        <v>29180.578125</v>
+      </c>
+      <c r="F3248" t="n">
+        <v>29180.578125</v>
+      </c>
+      <c r="G3248" t="n">
+        <v>13618163710</v>
+      </c>
+    </row>
+    <row r="3249">
+      <c r="A3249" s="2" t="n">
+        <v>45146</v>
+      </c>
+      <c r="B3249" t="n">
+        <v>29180.01953125</v>
+      </c>
+      <c r="C3249" t="n">
+        <v>30176.796875</v>
+      </c>
+      <c r="D3249" t="n">
+        <v>29113.814453125</v>
+      </c>
+      <c r="E3249" t="n">
+        <v>29765.4921875</v>
+      </c>
+      <c r="F3249" t="n">
+        <v>29765.4921875</v>
+      </c>
+      <c r="G3249" t="n">
+        <v>17570561357</v>
+      </c>
+    </row>
+    <row r="3250">
+      <c r="A3250" s="2" t="n">
+        <v>45147</v>
+      </c>
+      <c r="B3250" t="n">
+        <v>29766.6953125</v>
+      </c>
+      <c r="C3250" t="n">
+        <v>30093.435546875</v>
+      </c>
+      <c r="D3250" t="n">
+        <v>29376.80078125</v>
+      </c>
+      <c r="E3250" t="n">
+        <v>29561.494140625</v>
+      </c>
+      <c r="F3250" t="n">
+        <v>29561.494140625</v>
+      </c>
+      <c r="G3250" t="n">
+        <v>18379521213</v>
+      </c>
+    </row>
+    <row r="3251">
+      <c r="A3251" s="2" t="n">
+        <v>45148</v>
+      </c>
+      <c r="B3251" t="n">
+        <v>29563.97265625</v>
+      </c>
+      <c r="C3251" t="n">
+        <v>29688.564453125</v>
+      </c>
+      <c r="D3251" t="n">
+        <v>29354.447265625</v>
+      </c>
+      <c r="E3251" t="n">
+        <v>29429.591796875</v>
+      </c>
+      <c r="F3251" t="n">
+        <v>29429.591796875</v>
+      </c>
+      <c r="G3251" t="n">
+        <v>11865344789</v>
+      </c>
+    </row>
+    <row r="3252">
+      <c r="A3252" s="2" t="n">
+        <v>45149</v>
+      </c>
+      <c r="B3252" t="n">
+        <v>29424.90234375</v>
+      </c>
+      <c r="C3252" t="n">
+        <v>29517.7734375</v>
+      </c>
+      <c r="D3252" t="n">
+        <v>29253.517578125</v>
+      </c>
+      <c r="E3252" t="n">
+        <v>29397.71484375</v>
+      </c>
+      <c r="F3252" t="n">
+        <v>29397.71484375</v>
+      </c>
+      <c r="G3252" t="n">
+        <v>10195168197</v>
+      </c>
+    </row>
+    <row r="3253">
+      <c r="A3253" s="2" t="n">
+        <v>45150</v>
+      </c>
+      <c r="B3253" t="n">
+        <v>29399.787109375</v>
+      </c>
+      <c r="C3253" t="n">
+        <v>29465.11328125</v>
+      </c>
+      <c r="D3253" t="n">
+        <v>29357.587890625</v>
+      </c>
+      <c r="E3253" t="n">
+        <v>29415.96484375</v>
+      </c>
+      <c r="F3253" t="n">
+        <v>29415.96484375</v>
+      </c>
+      <c r="G3253" t="n">
+        <v>6194358008</v>
+      </c>
+    </row>
+    <row r="3254">
+      <c r="A3254" s="2" t="n">
+        <v>45151</v>
+      </c>
+      <c r="B3254" t="n">
+        <v>29416.59375</v>
+      </c>
+      <c r="C3254" t="n">
+        <v>29441.43359375</v>
+      </c>
+      <c r="D3254" t="n">
+        <v>29265.806640625</v>
+      </c>
+      <c r="E3254" t="n">
+        <v>29282.9140625</v>
+      </c>
+      <c r="F3254" t="n">
+        <v>29282.9140625</v>
+      </c>
+      <c r="G3254" t="n">
+        <v>7329897180</v>
+      </c>
+    </row>
+    <row r="3255">
+      <c r="A3255" s="2" t="n">
+        <v>45152</v>
+      </c>
+      <c r="B3255" t="n">
+        <v>29283.263671875</v>
+      </c>
+      <c r="C3255" t="n">
+        <v>29660.25390625</v>
+      </c>
+      <c r="D3255" t="n">
+        <v>29124.10546875</v>
+      </c>
+      <c r="E3255" t="n">
+        <v>29408.443359375</v>
+      </c>
+      <c r="F3255" t="n">
+        <v>29408.443359375</v>
+      </c>
+      <c r="G3255" t="n">
+        <v>14013695304</v>
+      </c>
+    </row>
+    <row r="3256">
+      <c r="A3256" s="2" t="n">
+        <v>45153</v>
+      </c>
+      <c r="B3256" t="n">
+        <v>29408.048828125</v>
+      </c>
+      <c r="C3256" t="n">
+        <v>29439.12109375</v>
+      </c>
+      <c r="D3256" t="n">
+        <v>29088.853515625</v>
+      </c>
+      <c r="E3256" t="n">
+        <v>29170.34765625</v>
+      </c>
+      <c r="F3256" t="n">
+        <v>29170.34765625</v>
+      </c>
+      <c r="G3256" t="n">
+        <v>12640195779</v>
+      </c>
+    </row>
+    <row r="3257">
+      <c r="A3257" s="2" t="n">
+        <v>45154</v>
+      </c>
+      <c r="B3257" t="n">
+        <v>29169.07421875</v>
+      </c>
+      <c r="C3257" t="n">
+        <v>29221.9765625</v>
+      </c>
+      <c r="D3257" t="n">
+        <v>28701.779296875</v>
+      </c>
+      <c r="E3257" t="n">
+        <v>28701.779296875</v>
+      </c>
+      <c r="F3257" t="n">
+        <v>28701.779296875</v>
+      </c>
+      <c r="G3257" t="n">
+        <v>14949271904</v>
+      </c>
+    </row>
+    <row r="3258">
+      <c r="A3258" s="2" t="n">
+        <v>45155</v>
+      </c>
+      <c r="B3258" t="n">
+        <v>28699.802734375</v>
+      </c>
+      <c r="C3258" t="n">
+        <v>28745.947265625</v>
+      </c>
+      <c r="D3258" t="n">
+        <v>25409.111328125</v>
+      </c>
+      <c r="E3258" t="n">
+        <v>26664.55078125</v>
+      </c>
+      <c r="F3258" t="n">
+        <v>26664.55078125</v>
+      </c>
+      <c r="G3258" t="n">
+        <v>31120851211</v>
+      </c>
+    </row>
+    <row r="3259">
+      <c r="A3259" s="2" t="n">
+        <v>45156</v>
+      </c>
+      <c r="B3259" t="n">
+        <v>26636.078125</v>
+      </c>
+      <c r="C3259" t="n">
+        <v>26808.1953125</v>
+      </c>
+      <c r="D3259" t="n">
+        <v>25668.921875</v>
+      </c>
+      <c r="E3259" t="n">
+        <v>26049.556640625</v>
+      </c>
+      <c r="F3259" t="n">
+        <v>26049.556640625</v>
+      </c>
+      <c r="G3259" t="n">
+        <v>24026236529</v>
+      </c>
+    </row>
+    <row r="3260">
+      <c r="A3260" s="2" t="n">
+        <v>45157</v>
+      </c>
+      <c r="B3260" t="n">
+        <v>26047.83203125</v>
+      </c>
+      <c r="C3260" t="n">
+        <v>26249.44921875</v>
+      </c>
+      <c r="D3260" t="n">
+        <v>25802.408203125</v>
+      </c>
+      <c r="E3260" t="n">
+        <v>26096.205078125</v>
+      </c>
+      <c r="F3260" t="n">
+        <v>26096.205078125</v>
+      </c>
+      <c r="G3260" t="n">
+        <v>10631443812</v>
+      </c>
+    </row>
+    <row r="3261">
+      <c r="A3261" s="2" t="n">
+        <v>45158</v>
+      </c>
+      <c r="B3261" t="n">
+        <v>26096.861328125</v>
+      </c>
+      <c r="C3261" t="n">
+        <v>26260.681640625</v>
+      </c>
+      <c r="D3261" t="n">
+        <v>26004.314453125</v>
+      </c>
+      <c r="E3261" t="n">
+        <v>26189.583984375</v>
+      </c>
+      <c r="F3261" t="n">
+        <v>26189.583984375</v>
+      </c>
+      <c r="G3261" t="n">
+        <v>9036580420</v>
+      </c>
+    </row>
+    <row r="3262">
+      <c r="A3262" s="2" t="n">
+        <v>45159</v>
+      </c>
+      <c r="B3262" t="n">
+        <v>26188.69140625</v>
+      </c>
+      <c r="C3262" t="n">
+        <v>26220.201171875</v>
+      </c>
+      <c r="D3262" t="n">
+        <v>25846.087890625</v>
+      </c>
+      <c r="E3262" t="n">
+        <v>26124.140625</v>
+      </c>
+      <c r="F3262" t="n">
+        <v>26124.140625</v>
+      </c>
+      <c r="G3262" t="n">
+        <v>13371557893</v>
+      </c>
+    </row>
+    <row r="3263">
+      <c r="A3263" s="2" t="n">
+        <v>45160</v>
+      </c>
+      <c r="B3263" t="n">
+        <v>26130.748046875</v>
+      </c>
+      <c r="C3263" t="n">
+        <v>26135.5078125</v>
+      </c>
+      <c r="D3263" t="n">
+        <v>25520.728515625</v>
+      </c>
+      <c r="E3263" t="n">
+        <v>26031.65625</v>
+      </c>
+      <c r="F3263" t="n">
+        <v>26031.65625</v>
+      </c>
+      <c r="G3263" t="n">
+        <v>14503820706</v>
+      </c>
+    </row>
+    <row r="3264">
+      <c r="A3264" s="2" t="n">
+        <v>45161</v>
+      </c>
+      <c r="B3264" t="n">
+        <v>26040.474609375</v>
+      </c>
+      <c r="C3264" t="n">
+        <v>26786.8984375</v>
+      </c>
+      <c r="D3264" t="n">
+        <v>25804.998046875</v>
+      </c>
+      <c r="E3264" t="n">
+        <v>26431.640625</v>
+      </c>
+      <c r="F3264" t="n">
+        <v>26431.640625</v>
+      </c>
+      <c r="G3264" t="n">
+        <v>16985265785</v>
+      </c>
+    </row>
+    <row r="3265">
+      <c r="A3265" s="2" t="n">
+        <v>45162</v>
+      </c>
+      <c r="B3265" t="n">
+        <v>26431.51953125</v>
+      </c>
+      <c r="C3265" t="n">
+        <v>26554.91015625</v>
+      </c>
+      <c r="D3265" t="n">
+        <v>25914.92578125</v>
+      </c>
+      <c r="E3265" t="n">
+        <v>26162.373046875</v>
+      </c>
+      <c r="F3265" t="n">
+        <v>26162.373046875</v>
+      </c>
+      <c r="G3265" t="n">
+        <v>12871532023</v>
+      </c>
+    </row>
+    <row r="3266">
+      <c r="A3266" s="2" t="n">
+        <v>45163</v>
+      </c>
+      <c r="B3266" t="n">
+        <v>26163.6796875</v>
+      </c>
+      <c r="C3266" t="n">
+        <v>26248.103515625</v>
+      </c>
+      <c r="D3266" t="n">
+        <v>25786.8125</v>
+      </c>
+      <c r="E3266" t="n">
+        <v>26047.66796875</v>
+      </c>
+      <c r="F3266" t="n">
+        <v>26047.66796875</v>
+      </c>
+      <c r="G3266" t="n">
+        <v>12406045118</v>
+      </c>
+    </row>
+    <row r="3267">
+      <c r="A3267" s="2" t="n">
+        <v>45164</v>
+      </c>
+      <c r="B3267" t="n">
+        <v>26047.234375</v>
+      </c>
+      <c r="C3267" t="n">
+        <v>26107.384765625</v>
+      </c>
+      <c r="D3267" t="n">
+        <v>25983.87890625</v>
+      </c>
+      <c r="E3267" t="n">
+        <v>26008.462890625</v>
+      </c>
+      <c r="F3267" t="n">
+        <v>26008.462890625</v>
+      </c>
+      <c r="G3267" t="n">
+        <v>6034817316</v>
+      </c>
+    </row>
+    <row r="3268">
+      <c r="A3268" s="2" t="n">
+        <v>45165</v>
+      </c>
+      <c r="B3268" t="n">
+        <v>26008.2421875</v>
+      </c>
+      <c r="C3268" t="n">
+        <v>26165.373046875</v>
+      </c>
+      <c r="D3268" t="n">
+        <v>25965.09765625</v>
+      </c>
+      <c r="E3268" t="n">
+        <v>26089.693359375</v>
+      </c>
+      <c r="F3268" t="n">
+        <v>26089.693359375</v>
+      </c>
+      <c r="G3268" t="n">
+        <v>6913768611</v>
+      </c>
+    </row>
+    <row r="3269">
+      <c r="A3269" s="2" t="n">
+        <v>45166</v>
+      </c>
+      <c r="B3269" t="n">
+        <v>26089.615234375</v>
+      </c>
+      <c r="C3269" t="n">
+        <v>26198.578125</v>
+      </c>
+      <c r="D3269" t="n">
+        <v>25880.599609375</v>
+      </c>
+      <c r="E3269" t="n">
+        <v>26106.150390625</v>
+      </c>
+      <c r="F3269" t="n">
+        <v>26106.150390625</v>
+      </c>
+      <c r="G3269" t="n">
+        <v>11002805166</v>
+      </c>
+    </row>
+    <row r="3270">
+      <c r="A3270" s="2" t="n">
+        <v>45167</v>
+      </c>
+      <c r="B3270" t="n">
+        <v>26102.486328125</v>
+      </c>
+      <c r="C3270" t="n">
+        <v>28089.337890625</v>
+      </c>
+      <c r="D3270" t="n">
+        <v>25912.62890625</v>
+      </c>
+      <c r="E3270" t="n">
+        <v>27727.392578125</v>
+      </c>
+      <c r="F3270" t="n">
+        <v>27727.392578125</v>
+      </c>
+      <c r="G3270" t="n">
+        <v>29368391712</v>
+      </c>
+    </row>
+    <row r="3271">
+      <c r="A3271" s="2" t="n">
+        <v>45168</v>
+      </c>
+      <c r="B3271" t="n">
+        <v>27726.083984375</v>
+      </c>
+      <c r="C3271" t="n">
+        <v>27760.16015625</v>
+      </c>
+      <c r="D3271" t="n">
+        <v>27069.20703125</v>
+      </c>
+      <c r="E3271" t="n">
+        <v>27297.265625</v>
+      </c>
+      <c r="F3271" t="n">
+        <v>27297.265625</v>
+      </c>
+      <c r="G3271" t="n">
+        <v>16343655235</v>
+      </c>
+    </row>
+    <row r="3272">
+      <c r="A3272" s="2" t="n">
+        <v>45169</v>
+      </c>
+      <c r="B3272" t="n">
+        <v>27301.9296875</v>
+      </c>
+      <c r="C3272" t="n">
+        <v>27456.078125</v>
+      </c>
+      <c r="D3272" t="n">
+        <v>25752.9296875</v>
+      </c>
+      <c r="E3272" t="n">
+        <v>25931.47265625</v>
+      </c>
+      <c r="F3272" t="n">
+        <v>25931.47265625</v>
+      </c>
+      <c r="G3272" t="n">
+        <v>20181001451</v>
+      </c>
+    </row>
+    <row r="3273">
+      <c r="A3273" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B3273" t="n">
+        <v>25934.021484375</v>
+      </c>
+      <c r="C3273" t="n">
+        <v>26125.869140625</v>
+      </c>
+      <c r="D3273" t="n">
+        <v>25362.609375</v>
+      </c>
+      <c r="E3273" t="n">
+        <v>25800.724609375</v>
+      </c>
+      <c r="F3273" t="n">
+        <v>25800.724609375</v>
+      </c>
+      <c r="G3273" t="n">
+        <v>17202862221</v>
+      </c>
+    </row>
+    <row r="3274">
+      <c r="A3274" s="2" t="n">
+        <v>45171</v>
+      </c>
+      <c r="B3274" t="n">
+        <v>25800.91015625</v>
+      </c>
+      <c r="C3274" t="n">
+        <v>25970.28515625</v>
+      </c>
+      <c r="D3274" t="n">
+        <v>25753.09375</v>
+      </c>
+      <c r="E3274" t="n">
+        <v>25868.798828125</v>
+      </c>
+      <c r="F3274" t="n">
+        <v>25868.798828125</v>
+      </c>
+      <c r="G3274" t="n">
+        <v>10100387473</v>
+      </c>
+    </row>
+    <row r="3275">
+      <c r="A3275" s="2" t="n">
+        <v>45172</v>
+      </c>
+      <c r="B3275" t="n">
+        <v>25869.47265625</v>
+      </c>
+      <c r="C3275" t="n">
+        <v>26087.1484375</v>
+      </c>
+      <c r="D3275" t="n">
+        <v>25817.03125</v>
+      </c>
+      <c r="E3275" t="n">
+        <v>25969.56640625</v>
+      </c>
+      <c r="F3275" t="n">
+        <v>25969.56640625</v>
+      </c>
+      <c r="G3275" t="n">
+        <v>8962524523</v>
+      </c>
+    </row>
+    <row r="3276">
+      <c r="A3276" s="2" t="n">
+        <v>45173</v>
+      </c>
+      <c r="B3276" t="n">
+        <v>25968.169921875</v>
+      </c>
+      <c r="C3276" t="n">
+        <v>26081.525390625</v>
+      </c>
+      <c r="D3276" t="n">
+        <v>25657.025390625</v>
+      </c>
+      <c r="E3276" t="n">
+        <v>25812.416015625</v>
+      </c>
+      <c r="F3276" t="n">
+        <v>25812.416015625</v>
+      </c>
+      <c r="G3276" t="n">
+        <v>10680635106</v>
+      </c>
+    </row>
+    <row r="3277">
+      <c r="A3277" s="2" t="n">
+        <v>45174</v>
+      </c>
+      <c r="B3277" t="n">
+        <v>25814.95703125</v>
+      </c>
+      <c r="C3277" t="n">
+        <v>25858.375</v>
+      </c>
+      <c r="D3277" t="n">
+        <v>25589.98828125</v>
+      </c>
+      <c r="E3277" t="n">
+        <v>25779.982421875</v>
+      </c>
+      <c r="F3277" t="n">
+        <v>25779.982421875</v>
+      </c>
+      <c r="G3277" t="n">
+        <v>11094740040</v>
+      </c>
+    </row>
+    <row r="3278">
+      <c r="A3278" s="2" t="n">
+        <v>45175</v>
+      </c>
+      <c r="B3278" t="n">
+        <v>25783.931640625</v>
+      </c>
+      <c r="C3278" t="n">
+        <v>25953.015625</v>
+      </c>
+      <c r="D3278" t="n">
+        <v>25404.359375</v>
+      </c>
+      <c r="E3278" t="n">
+        <v>25753.236328125</v>
+      </c>
+      <c r="F3278" t="n">
+        <v>25753.236328125</v>
+      </c>
+      <c r="G3278" t="n">
+        <v>12752705327</v>
+      </c>
+    </row>
+    <row r="3279">
+      <c r="A3279" s="2" t="n">
+        <v>45176</v>
+      </c>
+      <c r="B3279" t="n">
+        <v>25748.3125</v>
+      </c>
+      <c r="C3279" t="n">
+        <v>26409.302734375</v>
+      </c>
+      <c r="D3279" t="n">
+        <v>25608.201171875</v>
+      </c>
+      <c r="E3279" t="n">
+        <v>26240.1953125</v>
+      </c>
+      <c r="F3279" t="n">
+        <v>26240.1953125</v>
+      </c>
+      <c r="G3279" t="n">
+        <v>11088307100</v>
+      </c>
+    </row>
+    <row r="3280">
+      <c r="A3280" s="2" t="n">
+        <v>45177</v>
+      </c>
+      <c r="B3280" t="n">
+        <v>26245.208984375</v>
+      </c>
+      <c r="C3280" t="n">
+        <v>26414.005859375</v>
+      </c>
+      <c r="D3280" t="n">
+        <v>25677.48046875</v>
+      </c>
+      <c r="E3280" t="n">
+        <v>25905.654296875</v>
+      </c>
+      <c r="F3280" t="n">
+        <v>25905.654296875</v>
+      </c>
+      <c r="G3280" t="n">
+        <v>10817356400</v>
+      </c>
+    </row>
+    <row r="3281">
+      <c r="A3281" s="2" t="n">
+        <v>45178</v>
+      </c>
+      <c r="B3281" t="n">
+        <v>25905.42578125</v>
+      </c>
+      <c r="C3281" t="n">
+        <v>25921.9765625</v>
+      </c>
+      <c r="D3281" t="n">
+        <v>25810.494140625</v>
+      </c>
+      <c r="E3281" t="n">
+        <v>25895.677734375</v>
+      </c>
+      <c r="F3281" t="n">
+        <v>25895.677734375</v>
+      </c>
+      <c r="G3281" t="n">
+        <v>5481314132</v>
+      </c>
+    </row>
+    <row r="3282">
+      <c r="A3282" s="2" t="n">
+        <v>45179</v>
+      </c>
+      <c r="B3282" t="n">
+        <v>25895.2109375</v>
+      </c>
+      <c r="C3282" t="n">
+        <v>25978.130859375</v>
+      </c>
+      <c r="D3282" t="n">
+        <v>25640.26171875</v>
+      </c>
+      <c r="E3282" t="n">
+        <v>25832.2265625</v>
+      </c>
+      <c r="F3282" t="n">
+        <v>25832.2265625</v>
+      </c>
+      <c r="G3282" t="n">
+        <v>7899553047</v>
+      </c>
+    </row>
+    <row r="3283">
+      <c r="A3283" s="2" t="n">
+        <v>45180</v>
+      </c>
+      <c r="B3283" t="n">
+        <v>25831.71484375</v>
+      </c>
+      <c r="C3283" t="n">
+        <v>25883.947265625</v>
+      </c>
+      <c r="D3283" t="n">
+        <v>24930.296875</v>
+      </c>
+      <c r="E3283" t="n">
+        <v>25162.654296875</v>
+      </c>
+      <c r="F3283" t="n">
+        <v>25162.654296875</v>
+      </c>
+      <c r="G3283" t="n">
+        <v>14600006467</v>
+      </c>
+    </row>
+    <row r="3284">
+      <c r="A3284" s="2" t="n">
+        <v>45181</v>
+      </c>
+      <c r="B3284" t="n">
+        <v>25160.658203125</v>
+      </c>
+      <c r="C3284" t="n">
+        <v>26451.939453125</v>
+      </c>
+      <c r="D3284" t="n">
+        <v>25133.078125</v>
+      </c>
+      <c r="E3284" t="n">
+        <v>25833.34375</v>
+      </c>
+      <c r="F3284" t="n">
+        <v>25833.34375</v>
+      </c>
+      <c r="G3284" t="n">
+        <v>18657279324</v>
+      </c>
+    </row>
+    <row r="3285">
+      <c r="A3285" s="2" t="n">
+        <v>45182</v>
+      </c>
+      <c r="B3285" t="n">
+        <v>25837.5546875</v>
+      </c>
+      <c r="C3285" t="n">
+        <v>26376.11328125</v>
+      </c>
+      <c r="D3285" t="n">
+        <v>25781.123046875</v>
+      </c>
+      <c r="E3285" t="n">
+        <v>26228.32421875</v>
+      </c>
+      <c r="F3285" t="n">
+        <v>26228.32421875</v>
+      </c>
+      <c r="G3285" t="n">
+        <v>13072077070</v>
+      </c>
+    </row>
+    <row r="3286">
+      <c r="A3286" s="2" t="n">
+        <v>45183</v>
+      </c>
+      <c r="B3286" t="n">
+        <v>26228.27734375</v>
+      </c>
+      <c r="C3286" t="n">
+        <v>26774.623046875</v>
+      </c>
+      <c r="D3286" t="n">
+        <v>26171.451171875</v>
+      </c>
+      <c r="E3286" t="n">
+        <v>26539.673828125</v>
+      </c>
+      <c r="F3286" t="n">
+        <v>26539.673828125</v>
+      </c>
+      <c r="G3286" t="n">
+        <v>13811359124</v>
+      </c>
+    </row>
+    <row r="3287">
+      <c r="A3287" s="2" t="n">
+        <v>45184</v>
+      </c>
+      <c r="B3287" t="n">
+        <v>26533.818359375</v>
+      </c>
+      <c r="C3287" t="n">
+        <v>26840.498046875</v>
+      </c>
+      <c r="D3287" t="n">
+        <v>26240.701171875</v>
+      </c>
+      <c r="E3287" t="n">
+        <v>26608.693359375</v>
+      </c>
+      <c r="F3287" t="n">
+        <v>26608.693359375</v>
+      </c>
+      <c r="G3287" t="n">
+        <v>11479735788</v>
+      </c>
+    </row>
+    <row r="3288">
+      <c r="A3288" s="2" t="n">
+        <v>45185</v>
+      </c>
+      <c r="B3288" t="n">
+        <v>26606.19921875</v>
+      </c>
+      <c r="C3288" t="n">
+        <v>26754.76953125</v>
+      </c>
+      <c r="D3288" t="n">
+        <v>26473.890625</v>
+      </c>
+      <c r="E3288" t="n">
+        <v>26568.28125</v>
+      </c>
+      <c r="F3288" t="n">
+        <v>26568.28125</v>
+      </c>
+      <c r="G3288" t="n">
+        <v>7402031417</v>
+      </c>
+    </row>
+    <row r="3289">
+      <c r="A3289" s="2" t="n">
+        <v>45186</v>
+      </c>
+      <c r="B3289" t="n">
+        <v>26567.927734375</v>
+      </c>
+      <c r="C3289" t="n">
+        <v>26617.998046875</v>
+      </c>
+      <c r="D3289" t="n">
+        <v>26445.07421875</v>
+      </c>
+      <c r="E3289" t="n">
+        <v>26534.1875</v>
+      </c>
+      <c r="F3289" t="n">
+        <v>26534.1875</v>
+      </c>
+      <c r="G3289" t="n">
+        <v>6774210670</v>
+      </c>
+    </row>
+    <row r="3290">
+      <c r="A3290" s="2" t="n">
+        <v>45187</v>
+      </c>
+      <c r="B3290" t="n">
+        <v>26532.994140625</v>
+      </c>
+      <c r="C3290" t="n">
+        <v>27414.734375</v>
+      </c>
+      <c r="D3290" t="n">
+        <v>26415.515625</v>
+      </c>
+      <c r="E3290" t="n">
+        <v>26754.28125</v>
+      </c>
+      <c r="F3290" t="n">
+        <v>26754.28125</v>
+      </c>
+      <c r="G3290" t="n">
+        <v>15615339655</v>
+      </c>
+    </row>
+    <row r="3291">
+      <c r="A3291" s="2" t="n">
+        <v>45188</v>
+      </c>
+      <c r="B3291" t="n">
+        <v>26760.8515625</v>
+      </c>
+      <c r="C3291" t="n">
+        <v>27488.763671875</v>
+      </c>
+      <c r="D3291" t="n">
+        <v>26681.60546875</v>
+      </c>
+      <c r="E3291" t="n">
+        <v>27211.1171875</v>
+      </c>
+      <c r="F3291" t="n">
+        <v>27211.1171875</v>
+      </c>
+      <c r="G3291" t="n">
+        <v>13807690550</v>
+      </c>
+    </row>
+    <row r="3292">
+      <c r="A3292" s="2" t="n">
+        <v>45189</v>
+      </c>
+      <c r="B3292" t="n">
+        <v>27210.228515625</v>
+      </c>
+      <c r="C3292" t="n">
+        <v>27379.505859375</v>
+      </c>
+      <c r="D3292" t="n">
+        <v>26864.08203125</v>
+      </c>
+      <c r="E3292" t="n">
+        <v>27132.0078125</v>
+      </c>
+      <c r="F3292" t="n">
+        <v>27132.0078125</v>
+      </c>
+      <c r="G3292" t="n">
+        <v>13281116604</v>
+      </c>
+    </row>
+    <row r="3293">
+      <c r="A3293" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="B3293" t="n">
+        <v>27129.83984375</v>
+      </c>
+      <c r="C3293" t="n">
+        <v>27152.939453125</v>
+      </c>
+      <c r="D3293" t="n">
+        <v>26389.30078125</v>
+      </c>
+      <c r="E3293" t="n">
+        <v>26567.6328125</v>
+      </c>
+      <c r="F3293" t="n">
+        <v>26567.6328125</v>
+      </c>
+      <c r="G3293" t="n">
+        <v>13371443708</v>
+      </c>
+    </row>
+    <row r="3294">
+      <c r="A3294" s="2" t="n">
+        <v>45191</v>
+      </c>
+      <c r="B3294" t="n">
+        <v>26564.056640625</v>
+      </c>
+      <c r="C3294" t="n">
+        <v>26726.078125</v>
+      </c>
+      <c r="D3294" t="n">
+        <v>26495.533203125</v>
+      </c>
+      <c r="E3294" t="n">
+        <v>26579.568359375</v>
+      </c>
+      <c r="F3294" t="n">
+        <v>26579.568359375</v>
+      </c>
+      <c r="G3294" t="n">
+        <v>10578746709</v>
+      </c>
+    </row>
+    <row r="3295">
+      <c r="A3295" s="2" t="n">
+        <v>45192</v>
+      </c>
+      <c r="B3295" t="n">
+        <v>26578.556640625</v>
+      </c>
+      <c r="C3295" t="n">
+        <v>26634.185546875</v>
+      </c>
+      <c r="D3295" t="n">
+        <v>26520.51953125</v>
+      </c>
+      <c r="E3295" t="n">
+        <v>26579.390625</v>
+      </c>
+      <c r="F3295" t="n">
+        <v>26579.390625</v>
+      </c>
+      <c r="G3295" t="n">
+        <v>7404700301</v>
+      </c>
+    </row>
+    <row r="3296">
+      <c r="A3296" s="2" t="n">
+        <v>45193</v>
+      </c>
+      <c r="B3296" t="n">
+        <v>26579.373046875</v>
+      </c>
+      <c r="C3296" t="n">
+        <v>26716.05859375</v>
+      </c>
+      <c r="D3296" t="n">
+        <v>26221.05078125</v>
+      </c>
+      <c r="E3296" t="n">
+        <v>26256.826171875</v>
+      </c>
+      <c r="F3296" t="n">
+        <v>26256.826171875</v>
+      </c>
+      <c r="G3296" t="n">
+        <v>8192867686</v>
+      </c>
+    </row>
+    <row r="3297">
+      <c r="A3297" s="2" t="n">
+        <v>45194</v>
+      </c>
+      <c r="B3297" t="n">
+        <v>26253.775390625</v>
+      </c>
+      <c r="C3297" t="n">
+        <v>26421.5078125</v>
+      </c>
+      <c r="D3297" t="n">
+        <v>26011.46875</v>
+      </c>
+      <c r="E3297" t="n">
+        <v>26298.48046875</v>
+      </c>
+      <c r="F3297" t="n">
+        <v>26298.48046875</v>
+      </c>
+      <c r="G3297" t="n">
+        <v>11997833257</v>
+      </c>
+    </row>
+    <row r="3298">
+      <c r="A3298" s="2" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3298" t="n">
+        <v>26294.7578125</v>
+      </c>
+      <c r="C3298" t="n">
+        <v>26389.884765625</v>
+      </c>
+      <c r="D3298" t="n">
+        <v>26090.712890625</v>
+      </c>
+      <c r="E3298" t="n">
+        <v>26217.25</v>
+      </c>
+      <c r="F3298" t="n">
+        <v>26217.25</v>
+      </c>
+      <c r="G3298" t="n">
+        <v>9985498161</v>
+      </c>
+    </row>
+    <row r="3299">
+      <c r="A3299" s="2" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B3299" t="n">
+        <v>26209.498046875</v>
+      </c>
+      <c r="C3299" t="n">
+        <v>26817.841796875</v>
+      </c>
+      <c r="D3299" t="n">
+        <v>26111.46484375</v>
+      </c>
+      <c r="E3299" t="n">
+        <v>26352.716796875</v>
+      </c>
+      <c r="F3299" t="n">
+        <v>26352.716796875</v>
+      </c>
+      <c r="G3299" t="n">
+        <v>11718380997</v>
+      </c>
+    </row>
+    <row r="3300">
+      <c r="A3300" s="2" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B3300" t="n">
+        <v>26355.8125</v>
+      </c>
+      <c r="C3300" t="n">
+        <v>27259.5</v>
+      </c>
+      <c r="D3300" t="n">
+        <v>26327.322265625</v>
+      </c>
+      <c r="E3300" t="n">
+        <v>27021.546875</v>
+      </c>
+      <c r="F3300" t="n">
+        <v>27021.546875</v>
+      </c>
+      <c r="G3300" t="n">
+        <v>14079002707</v>
+      </c>
+    </row>
+    <row r="3301">
+      <c r="A3301" s="2" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B3301" t="n">
+        <v>27024.841796875</v>
+      </c>
+      <c r="C3301" t="n">
+        <v>27225.9375</v>
+      </c>
+      <c r="D3301" t="n">
+        <v>26721.763671875</v>
+      </c>
+      <c r="E3301" t="n">
+        <v>26911.720703125</v>
+      </c>
+      <c r="F3301" t="n">
+        <v>26911.720703125</v>
+      </c>
+      <c r="G3301" t="n">
+        <v>10396435377</v>
+      </c>
+    </row>
+    <row r="3302">
+      <c r="A3302" s="2" t="n">
+        <v>45199</v>
+      </c>
+      <c r="B3302" t="n">
+        <v>26911.689453125</v>
+      </c>
+      <c r="C3302" t="n">
+        <v>27091.794921875</v>
+      </c>
+      <c r="D3302" t="n">
+        <v>26888.96875</v>
+      </c>
+      <c r="E3302" t="n">
+        <v>26967.916015625</v>
+      </c>
+      <c r="F3302" t="n">
+        <v>26967.916015625</v>
+      </c>
+      <c r="G3302" t="n">
+        <v>5331172801</v>
+      </c>
+    </row>
+    <row r="3303">
+      <c r="A3303" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B3303" t="n">
+        <v>26967.396484375</v>
+      </c>
+      <c r="C3303" t="n">
+        <v>28047.23828125</v>
+      </c>
+      <c r="D3303" t="n">
+        <v>26965.09375</v>
+      </c>
+      <c r="E3303" t="n">
+        <v>27983.75</v>
+      </c>
+      <c r="F3303" t="n">
+        <v>27983.75</v>
+      </c>
+      <c r="G3303" t="n">
+        <v>9503917434</v>
+      </c>
+    </row>
+    <row r="3304">
+      <c r="A3304" s="2" t="n">
+        <v>45201</v>
+      </c>
+      <c r="B3304" t="n">
+        <v>27976.798828125</v>
+      </c>
+      <c r="C3304" t="n">
+        <v>28494.458984375</v>
+      </c>
+      <c r="D3304" t="n">
+        <v>27347.787109375</v>
+      </c>
+      <c r="E3304" t="n">
+        <v>27530.78515625</v>
+      </c>
+      <c r="F3304" t="n">
+        <v>27530.78515625</v>
+      </c>
+      <c r="G3304" t="n">
+        <v>19793041322</v>
+      </c>
+    </row>
+    <row r="3305">
+      <c r="A3305" s="2" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B3305" t="n">
+        <v>27508.251953125</v>
+      </c>
+      <c r="C3305" t="n">
+        <v>27667.19140625</v>
+      </c>
+      <c r="D3305" t="n">
+        <v>27216.001953125</v>
+      </c>
+      <c r="E3305" t="n">
+        <v>27429.978515625</v>
+      </c>
+      <c r="F3305" t="n">
+        <v>27429.978515625</v>
+      </c>
+      <c r="G3305" t="n">
+        <v>11407814187</v>
+      </c>
+    </row>
+    <row r="3306">
+      <c r="A3306" s="2" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B3306" t="n">
+        <v>27429.07421875</v>
+      </c>
+      <c r="C3306" t="n">
+        <v>27826.658203125</v>
+      </c>
+      <c r="D3306" t="n">
+        <v>27248.10546875</v>
+      </c>
+      <c r="E3306" t="n">
+        <v>27799.39453125</v>
+      </c>
+      <c r="F3306" t="n">
+        <v>27799.39453125</v>
+      </c>
+      <c r="G3306" t="n">
+        <v>11143355314</v>
+      </c>
+    </row>
+    <row r="3307">
+      <c r="A3307" s="2" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B3307" t="n">
+        <v>27798.646484375</v>
+      </c>
+      <c r="C3307" t="n">
+        <v>28091.861328125</v>
+      </c>
+      <c r="D3307" t="n">
+        <v>27375.6015625</v>
+      </c>
+      <c r="E3307" t="n">
+        <v>27415.912109375</v>
+      </c>
+      <c r="F3307" t="n">
+        <v>27415.912109375</v>
+      </c>
+      <c r="G3307" t="n">
+        <v>11877253670</v>
+      </c>
+    </row>
+    <row r="3308">
+      <c r="A3308" s="2" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B3308" t="n">
+        <v>27412.123046875</v>
+      </c>
+      <c r="C3308" t="n">
+        <v>28252.537109375</v>
+      </c>
+      <c r="D3308" t="n">
+        <v>27215.552734375</v>
+      </c>
+      <c r="E3308" t="n">
+        <v>27946.59765625</v>
+      </c>
+      <c r="F3308" t="n">
+        <v>27946.59765625</v>
+      </c>
+      <c r="G3308" t="n">
+        <v>13492391599</v>
+      </c>
+    </row>
+    <row r="3309">
+      <c r="A3309" s="2" t="n">
+        <v>45206</v>
+      </c>
+      <c r="B3309" t="n">
+        <v>27946.78125</v>
+      </c>
+      <c r="C3309" t="n">
+        <v>28028.091796875</v>
+      </c>
+      <c r="D3309" t="n">
+        <v>27870.423828125</v>
+      </c>
+      <c r="E3309" t="n">
+        <v>27968.83984375</v>
+      </c>
+      <c r="F3309" t="n">
+        <v>27968.83984375</v>
+      </c>
+      <c r="G3309" t="n">
+        <v>6553044316</v>
+      </c>
+    </row>
+    <row r="3310">
+      <c r="A3310" s="2" t="n">
+        <v>45207</v>
+      </c>
+      <c r="B3310" t="n">
+        <v>27971.677734375</v>
+      </c>
+      <c r="C3310" t="n">
+        <v>28102.169921875</v>
+      </c>
+      <c r="D3310" t="n">
+        <v>27740.662109375</v>
+      </c>
+      <c r="E3310" t="n">
+        <v>27935.08984375</v>
+      </c>
+      <c r="F3310" t="n">
+        <v>27935.08984375</v>
+      </c>
+      <c r="G3310" t="n">
+        <v>7916875290</v>
+      </c>
+    </row>
+    <row r="3311">
+      <c r="A3311" s="2" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B3311" t="n">
+        <v>27934.47265625</v>
+      </c>
+      <c r="C3311" t="n">
+        <v>27989.470703125</v>
+      </c>
+      <c r="D3311" t="n">
+        <v>27302.5625</v>
+      </c>
+      <c r="E3311" t="n">
+        <v>27583.677734375</v>
+      </c>
+      <c r="F3311" t="n">
+        <v>27583.677734375</v>
+      </c>
+      <c r="G3311" t="n">
+        <v>12007668568</v>
+      </c>
+    </row>
+    <row r="3312">
+      <c r="A3312" s="2" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B3312" t="n">
+        <v>27589.201171875</v>
+      </c>
+      <c r="C3312" t="n">
+        <v>27715.84765625</v>
+      </c>
+      <c r="D3312" t="n">
+        <v>27301.654296875</v>
+      </c>
+      <c r="E3312" t="n">
+        <v>27391.01953125</v>
+      </c>
+      <c r="F3312" t="n">
+        <v>27391.01953125</v>
+      </c>
+      <c r="G3312" t="n">
+        <v>9973350678</v>
+      </c>
+    </row>
+    <row r="3313">
+      <c r="A3313" s="2" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B3313" t="n">
+        <v>27392.076171875</v>
+      </c>
+      <c r="C3313" t="n">
+        <v>27474.115234375</v>
+      </c>
+      <c r="D3313" t="n">
+        <v>26561.099609375</v>
+      </c>
+      <c r="E3313" t="n">
+        <v>26873.3203125</v>
+      </c>
+      <c r="F3313" t="n">
+        <v>26873.3203125</v>
+      </c>
+      <c r="G3313" t="n">
+        <v>13648094333</v>
+      </c>
+    </row>
+    <row r="3314">
+      <c r="A3314" s="2" t="n">
+        <v>45211</v>
+      </c>
+      <c r="B3314" t="n">
+        <v>26873.29296875</v>
+      </c>
+      <c r="C3314" t="n">
+        <v>26921.439453125</v>
+      </c>
+      <c r="D3314" t="n">
+        <v>26558.3203125</v>
+      </c>
+      <c r="E3314" t="n">
+        <v>26756.798828125</v>
+      </c>
+      <c r="F3314" t="n">
+        <v>26756.798828125</v>
+      </c>
+      <c r="G3314" t="n">
+        <v>9392909295</v>
+      </c>
+    </row>
+    <row r="3315">
+      <c r="A3315" s="2" t="n">
+        <v>45212</v>
+      </c>
+      <c r="B3315" t="n">
+        <v>26752.87890625</v>
+      </c>
+      <c r="C3315" t="n">
+        <v>27092.697265625</v>
+      </c>
+      <c r="D3315" t="n">
+        <v>26686.322265625</v>
+      </c>
+      <c r="E3315" t="n">
+        <v>26862.375</v>
+      </c>
+      <c r="F3315" t="n">
+        <v>26862.375</v>
+      </c>
+      <c r="G3315" t="n">
+        <v>15165312851</v>
+      </c>
+    </row>
+    <row r="3316">
+      <c r="A3316" s="2" t="n">
+        <v>45213</v>
+      </c>
+      <c r="B3316" t="n">
+        <v>26866.203125</v>
+      </c>
+      <c r="C3316" t="n">
+        <v>26969</v>
+      </c>
+      <c r="D3316" t="n">
+        <v>26814.5859375</v>
+      </c>
+      <c r="E3316" t="n">
+        <v>26861.70703125</v>
+      </c>
+      <c r="F3316" t="n">
+        <v>26861.70703125</v>
+      </c>
+      <c r="G3316" t="n">
+        <v>5388116782</v>
+      </c>
+    </row>
+    <row r="3317">
+      <c r="A3317" s="2" t="n">
+        <v>45214</v>
+      </c>
+      <c r="B3317" t="n">
+        <v>26858.01171875</v>
+      </c>
+      <c r="C3317" t="n">
+        <v>27289.169921875</v>
+      </c>
+      <c r="D3317" t="n">
+        <v>26817.89453125</v>
+      </c>
+      <c r="E3317" t="n">
+        <v>27159.65234375</v>
+      </c>
+      <c r="F3317" t="n">
+        <v>27159.65234375</v>
+      </c>
+      <c r="G3317" t="n">
+        <v>7098201980</v>
+      </c>
+    </row>
+    <row r="3318">
+      <c r="A3318" s="2" t="n">
+        <v>45215</v>
+      </c>
+      <c r="B3318" t="n">
+        <v>27162.62890625</v>
+      </c>
+      <c r="C3318" t="n">
+        <v>29448.138671875</v>
+      </c>
+      <c r="D3318" t="n">
+        <v>27130.47265625</v>
+      </c>
+      <c r="E3318" t="n">
+        <v>28519.466796875</v>
+      </c>
+      <c r="F3318" t="n">
+        <v>28519.466796875</v>
+      </c>
+      <c r="G3318" t="n">
+        <v>27833876539</v>
+      </c>
+    </row>
+    <row r="3319">
+      <c r="A3319" s="2" t="n">
+        <v>45216</v>
+      </c>
+      <c r="B3319" t="n">
+        <v>28522.09765625</v>
+      </c>
+      <c r="C3319" t="n">
+        <v>28618.751953125</v>
+      </c>
+      <c r="D3319" t="n">
+        <v>28110.185546875</v>
+      </c>
+      <c r="E3319" t="n">
+        <v>28415.748046875</v>
+      </c>
+      <c r="F3319" t="n">
+        <v>28415.748046875</v>
+      </c>
+      <c r="G3319" t="n">
+        <v>14872527508</v>
+      </c>
+    </row>
+    <row r="3320">
+      <c r="A3320" s="2" t="n">
+        <v>45217</v>
+      </c>
+      <c r="B3320" t="n">
+        <v>28413.53125</v>
+      </c>
+      <c r="C3320" t="n">
+        <v>28889.009765625</v>
+      </c>
+      <c r="D3320" t="n">
+        <v>28174.251953125</v>
+      </c>
+      <c r="E3320" t="n">
+        <v>28328.341796875</v>
+      </c>
+      <c r="F3320" t="n">
+        <v>28328.341796875</v>
+      </c>
+      <c r="G3320" t="n">
+        <v>12724128586</v>
+      </c>
+    </row>
+    <row r="3321">
+      <c r="A3321" s="2" t="n">
+        <v>45218</v>
+      </c>
+      <c r="B3321" t="n">
+        <v>28332.416015625</v>
+      </c>
+      <c r="C3321" t="n">
+        <v>28892.474609375</v>
+      </c>
+      <c r="D3321" t="n">
+        <v>28177.98828125</v>
+      </c>
+      <c r="E3321" t="n">
+        <v>28719.806640625</v>
+      </c>
+      <c r="F3321" t="n">
+        <v>28719.806640625</v>
+      </c>
+      <c r="G3321" t="n">
+        <v>14448058195</v>
+      </c>
+    </row>
+    <row r="3322">
+      <c r="A3322" s="2" t="n">
+        <v>45219</v>
+      </c>
+      <c r="B3322" t="n">
+        <v>28732.8125</v>
+      </c>
+      <c r="C3322" t="n">
+        <v>30104.0859375</v>
+      </c>
+      <c r="D3322" t="n">
+        <v>28601.669921875</v>
+      </c>
+      <c r="E3322" t="n">
+        <v>29682.94921875</v>
+      </c>
+      <c r="F3322" t="n">
+        <v>29682.94921875</v>
+      </c>
+      <c r="G3322" t="n">
+        <v>21536125230</v>
+      </c>
+    </row>
+    <row r="3323">
+      <c r="A3323" s="2" t="n">
+        <v>45220</v>
+      </c>
+      <c r="B3323" t="n">
+        <v>29683.380859375</v>
+      </c>
+      <c r="C3323" t="n">
+        <v>30287.482421875</v>
+      </c>
+      <c r="D3323" t="n">
+        <v>29481.751953125</v>
+      </c>
+      <c r="E3323" t="n">
+        <v>29918.412109375</v>
+      </c>
+      <c r="F3323" t="n">
+        <v>29918.412109375</v>
+      </c>
+      <c r="G3323" t="n">
+        <v>11541146996</v>
+      </c>
+    </row>
+    <row r="3324">
+      <c r="A3324" s="2" t="n">
+        <v>45221</v>
+      </c>
+      <c r="B3324" t="n">
+        <v>29918.654296875</v>
+      </c>
+      <c r="C3324" t="n">
+        <v>30199.43359375</v>
+      </c>
+      <c r="D3324" t="n">
+        <v>29720.3125</v>
+      </c>
+      <c r="E3324" t="n">
+        <v>29993.896484375</v>
+      </c>
+      <c r="F3324" t="n">
+        <v>29993.896484375</v>
+      </c>
+      <c r="G3324" t="n">
+        <v>10446520040</v>
+      </c>
+    </row>
+    <row r="3325">
+      <c r="A3325" s="2" t="n">
+        <v>45222</v>
+      </c>
+      <c r="B3325" t="n">
+        <v>30140.685546875</v>
+      </c>
+      <c r="C3325" t="n">
+        <v>34370.4375</v>
+      </c>
+      <c r="D3325" t="n">
+        <v>30097.828125</v>
+      </c>
+      <c r="E3325" t="n">
+        <v>33086.234375</v>
+      </c>
+      <c r="F3325" t="n">
+        <v>33086.234375</v>
+      </c>
+      <c r="G3325" t="n">
+        <v>38363572311</v>
+      </c>
+    </row>
+    <row r="3326">
+      <c r="A3326" s="2" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B3326" t="n">
+        <v>33077.3046875</v>
+      </c>
+      <c r="C3326" t="n">
+        <v>35150.43359375</v>
+      </c>
+      <c r="D3326" t="n">
+        <v>32880.76171875</v>
+      </c>
+      <c r="E3326" t="n">
+        <v>33901.52734375</v>
+      </c>
+      <c r="F3326" t="n">
+        <v>33901.52734375</v>
+      </c>
+      <c r="G3326" t="n">
+        <v>44934999645</v>
+      </c>
+    </row>
+    <row r="3327">
+      <c r="A3327" s="2" t="n">
+        <v>45224</v>
+      </c>
+      <c r="B3327" t="n">
+        <v>33916.04296875</v>
+      </c>
+      <c r="C3327" t="n">
+        <v>35133.7578125</v>
+      </c>
+      <c r="D3327" t="n">
+        <v>33709.109375</v>
+      </c>
+      <c r="E3327" t="n">
+        <v>34502.8203125</v>
+      </c>
+      <c r="F3327" t="n">
+        <v>34502.8203125</v>
+      </c>
+      <c r="G3327" t="n">
+        <v>25254318008</v>
+      </c>
+    </row>
+    <row r="3328">
+      <c r="A3328" s="2" t="n">
+        <v>45225</v>
+      </c>
+      <c r="B3328" t="n">
+        <v>34504.2890625</v>
+      </c>
+      <c r="C3328" t="n">
+        <v>34832.91015625</v>
+      </c>
+      <c r="D3328" t="n">
+        <v>33762.32421875</v>
+      </c>
+      <c r="E3328" t="n">
+        <v>34156.6484375</v>
+      </c>
+      <c r="F3328" t="n">
+        <v>34156.6484375</v>
+      </c>
+      <c r="G3328" t="n">
+        <v>19427195376</v>
+      </c>
+    </row>
+    <row r="3329">
+      <c r="A3329" s="2" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B3329" t="n">
+        <v>34156.5</v>
+      </c>
+      <c r="C3329" t="n">
+        <v>34238.2109375</v>
+      </c>
+      <c r="D3329" t="n">
+        <v>33416.88671875</v>
+      </c>
+      <c r="E3329" t="n">
+        <v>33909.80078125</v>
+      </c>
+      <c r="F3329" t="n">
+        <v>33909.80078125</v>
+      </c>
+      <c r="G3329" t="n">
+        <v>16418032871</v>
+      </c>
+    </row>
+    <row r="3330">
+      <c r="A3330" s="2" t="n">
+        <v>45227</v>
+      </c>
+      <c r="B3330" t="n">
+        <v>33907.72265625</v>
+      </c>
+      <c r="C3330" t="n">
+        <v>34399.390625</v>
+      </c>
+      <c r="D3330" t="n">
+        <v>33874.8046875</v>
+      </c>
+      <c r="E3330" t="n">
+        <v>34089.57421875</v>
+      </c>
+      <c r="F3330" t="n">
+        <v>34089.57421875</v>
+      </c>
+      <c r="G3330" t="n">
+        <v>10160330825</v>
+      </c>
+    </row>
+    <row r="3331">
+      <c r="A3331" s="2" t="n">
+        <v>45228</v>
+      </c>
+      <c r="B3331" t="n">
+        <v>34089.37109375</v>
+      </c>
+      <c r="C3331" t="n">
+        <v>34743.26171875</v>
+      </c>
+      <c r="D3331" t="n">
+        <v>33947.56640625</v>
+      </c>
+      <c r="E3331" t="n">
+        <v>34538.48046875</v>
+      </c>
+      <c r="F3331" t="n">
+        <v>34538.48046875</v>
+      </c>
+      <c r="G3331" t="n">
+        <v>11160323986</v>
+      </c>
+    </row>
+    <row r="3332">
+      <c r="A3332" s="2" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B3332" t="n">
+        <v>34531.7421875</v>
+      </c>
+      <c r="C3332" t="n">
+        <v>34843.93359375</v>
+      </c>
+      <c r="D3332" t="n">
+        <v>34110.97265625</v>
+      </c>
+      <c r="E3332" t="n">
+        <v>34502.36328125</v>
+      </c>
+      <c r="F3332" t="n">
+        <v>34502.36328125</v>
+      </c>
+      <c r="G3332" t="n">
+        <v>17184860315</v>
+      </c>
+    </row>
+    <row r="3333">
+      <c r="A3333" s="2" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B3333" t="n">
+        <v>34500.078125</v>
+      </c>
+      <c r="C3333" t="n">
+        <v>34719.25390625</v>
+      </c>
+      <c r="D3333" t="n">
+        <v>34083.30859375</v>
+      </c>
+      <c r="E3333" t="n">
+        <v>34667.78125</v>
+      </c>
+      <c r="F3333" t="n">
+        <v>34667.78125</v>
+      </c>
+      <c r="G3333" t="n">
+        <v>15758270810</v>
+      </c>
+    </row>
+    <row r="3334">
+      <c r="A3334" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B3334" t="n">
+        <v>34657.2734375</v>
+      </c>
+      <c r="C3334" t="n">
+        <v>35527.9296875</v>
+      </c>
+      <c r="D3334" t="n">
+        <v>34170.69140625</v>
+      </c>
+      <c r="E3334" t="n">
+        <v>35437.25390625</v>
+      </c>
+      <c r="F3334" t="n">
+        <v>35437.25390625</v>
+      </c>
+      <c r="G3334" t="n">
+        <v>22446272005</v>
+      </c>
+    </row>
+    <row r="3335">
+      <c r="A3335" s="2" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B3335" t="n">
+        <v>35441.578125</v>
+      </c>
+      <c r="C3335" t="n">
+        <v>35919.84375</v>
+      </c>
+      <c r="D3335" t="n">
+        <v>34401.57421875</v>
+      </c>
+      <c r="E3335" t="n">
+        <v>34938.2421875</v>
+      </c>
+      <c r="F3335" t="n">
+        <v>34938.2421875</v>
+      </c>
+      <c r="G3335" t="n">
+        <v>20998158544</v>
+      </c>
+    </row>
+    <row r="3336">
+      <c r="A3336" s="2" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B3336" t="n">
+        <v>34942.47265625</v>
+      </c>
+      <c r="C3336" t="n">
+        <v>34942.47265625</v>
+      </c>
+      <c r="D3336" t="n">
+        <v>34133.44140625</v>
+      </c>
+      <c r="E3336" t="n">
+        <v>34732.32421875</v>
+      </c>
+      <c r="F3336" t="n">
+        <v>34732.32421875</v>
+      </c>
+      <c r="G3336" t="n">
+        <v>17158456701</v>
+      </c>
+    </row>
+    <row r="3337">
+      <c r="A3337" s="2" t="n">
+        <v>45234</v>
+      </c>
+      <c r="B3337" t="n">
+        <v>34736.32421875</v>
+      </c>
+      <c r="C3337" t="n">
+        <v>35256.03125</v>
+      </c>
+      <c r="D3337" t="n">
+        <v>34616.69140625</v>
+      </c>
+      <c r="E3337" t="n">
+        <v>35082.1953125</v>
+      </c>
+      <c r="F3337" t="n">
+        <v>35082.1953125</v>
+      </c>
+      <c r="G3337" t="n">
+        <v>9561294264</v>
+      </c>
+    </row>
+    <row r="3338">
+      <c r="A3338" s="2" t="n">
+        <v>45235</v>
+      </c>
+      <c r="B3338" t="n">
+        <v>35090.01171875</v>
+      </c>
+      <c r="C3338" t="n">
+        <v>35340.33984375</v>
+      </c>
+      <c r="D3338" t="n">
+        <v>34594.2421875</v>
+      </c>
+      <c r="E3338" t="n">
+        <v>35049.35546875</v>
+      </c>
+      <c r="F3338" t="n">
+        <v>35049.35546875</v>
+      </c>
+      <c r="G3338" t="n">
+        <v>12412743996</v>
+      </c>
+    </row>
+    <row r="3339">
+      <c r="A3339" s="2" t="n">
+        <v>45236</v>
+      </c>
+      <c r="B3339" t="n">
+        <v>35044.7890625</v>
+      </c>
+      <c r="C3339" t="n">
+        <v>35286.02734375</v>
+      </c>
+      <c r="D3339" t="n">
+        <v>34765.36328125</v>
+      </c>
+      <c r="E3339" t="n">
+        <v>35037.37109375</v>
+      </c>
+      <c r="F3339" t="n">
+        <v>35037.37109375</v>
+      </c>
+      <c r="G3339" t="n">
+        <v>12693436420</v>
+      </c>
+    </row>
+    <row r="3340">
+      <c r="A3340" s="2" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B3340" t="n">
+        <v>35047.79296875</v>
+      </c>
+      <c r="C3340" t="n">
+        <v>35892.41796875</v>
+      </c>
+      <c r="D3340" t="n">
+        <v>34545.81640625</v>
+      </c>
+      <c r="E3340" t="n">
+        <v>35443.5625</v>
+      </c>
+      <c r="F3340" t="n">
+        <v>35443.5625</v>
+      </c>
+      <c r="G3340" t="n">
+        <v>18834737789</v>
+      </c>
+    </row>
+    <row r="3341">
+      <c r="A3341" s="2" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B3341" t="n">
+        <v>35419.4765625</v>
+      </c>
+      <c r="C3341" t="n">
+        <v>35994.41796875</v>
+      </c>
+      <c r="D3341" t="n">
+        <v>35147.80078125</v>
+      </c>
+      <c r="E3341" t="n">
+        <v>35655.27734375</v>
+      </c>
+      <c r="F3341" t="n">
+        <v>35655.27734375</v>
+      </c>
+      <c r="G3341" t="n">
+        <v>17295394918</v>
+      </c>
+    </row>
+    <row r="3342">
+      <c r="A3342" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B3342" t="n">
+        <v>35633.6328125</v>
+      </c>
+      <c r="C3342" t="n">
+        <v>37926.2578125</v>
+      </c>
+      <c r="D3342" t="n">
+        <v>35592.1015625</v>
+      </c>
+      <c r="E3342" t="n">
+        <v>36693.125</v>
+      </c>
+      <c r="F3342" t="n">
+        <v>36693.125</v>
+      </c>
+      <c r="G3342" t="n">
+        <v>37762672382</v>
+      </c>
+    </row>
+    <row r="3343">
+      <c r="A3343" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="B3343" t="n">
+        <v>36702.25</v>
+      </c>
+      <c r="C3343" t="n">
+        <v>37493.80078125</v>
+      </c>
+      <c r="D3343" t="n">
+        <v>36362.75390625</v>
+      </c>
+      <c r="E3343" t="n">
+        <v>37313.96875</v>
+      </c>
+      <c r="F3343" t="n">
+        <v>37313.96875</v>
+      </c>
+      <c r="G3343" t="n">
+        <v>22711265155</v>
+      </c>
+    </row>
+    <row r="3344">
+      <c r="A3344" s="2" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B3344" t="n">
+        <v>37310.0703125</v>
+      </c>
+      <c r="C3344" t="n">
+        <v>37407.09375</v>
+      </c>
+      <c r="D3344" t="n">
+        <v>36773.66796875</v>
+      </c>
+      <c r="E3344" t="n">
+        <v>37138.05078125</v>
+      </c>
+      <c r="F3344" t="n">
+        <v>37138.05078125</v>
+      </c>
+      <c r="G3344" t="n">
+        <v>13924272142</v>
+      </c>
+    </row>
+    <row r="3345">
+      <c r="A3345" s="2" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B3345" t="n">
+        <v>37133.9921875</v>
+      </c>
+      <c r="C3345" t="n">
+        <v>37227.69140625</v>
+      </c>
+      <c r="D3345" t="n">
+        <v>36779.1171875</v>
+      </c>
+      <c r="E3345" t="n">
+        <v>37054.51953125</v>
+      </c>
+      <c r="F3345" t="n">
+        <v>37054.51953125</v>
+      </c>
+      <c r="G3345" t="n">
+        <v>11545715999</v>
+      </c>
+    </row>
+    <row r="3346">
+      <c r="A3346" s="2" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B3346" t="n">
+        <v>37070.3046875</v>
+      </c>
+      <c r="C3346" t="n">
+        <v>37405.1171875</v>
+      </c>
+      <c r="D3346" t="n">
+        <v>36399.60546875</v>
+      </c>
+      <c r="E3346" t="n">
+        <v>36502.35546875</v>
+      </c>
+      <c r="F3346" t="n">
+        <v>36502.35546875</v>
+      </c>
+      <c r="G3346" t="n">
+        <v>19057712790</v>
+      </c>
+    </row>
+    <row r="3347">
+      <c r="A3347" s="2" t="n">
+        <v>45244</v>
+      </c>
+      <c r="B3347" t="n">
+        <v>36491.7890625</v>
+      </c>
+      <c r="C3347" t="n">
+        <v>36753.3515625</v>
+      </c>
+      <c r="D3347" t="n">
+        <v>34948.5</v>
+      </c>
+      <c r="E3347" t="n">
+        <v>35537.640625</v>
+      </c>
+      <c r="F3347" t="n">
+        <v>35537.640625</v>
+      </c>
+      <c r="G3347" t="n">
+        <v>23857403554</v>
+      </c>
+    </row>
+    <row r="3348">
+      <c r="A3348" s="2" t="n">
+        <v>45245</v>
+      </c>
+      <c r="B3348" t="n">
+        <v>35548.11328125</v>
+      </c>
+      <c r="C3348" t="n">
+        <v>37964.89453125</v>
+      </c>
+      <c r="D3348" t="n">
+        <v>35383.78125</v>
+      </c>
+      <c r="E3348" t="n">
+        <v>37880.58203125</v>
+      </c>
+      <c r="F3348" t="n">
+        <v>37880.58203125</v>
+      </c>
+      <c r="G3348" t="n">
+        <v>27365821679</v>
+      </c>
+    </row>
+    <row r="3349">
+      <c r="A3349" s="2" t="n">
+        <v>45246</v>
+      </c>
+      <c r="B3349" t="n">
+        <v>37879.98046875</v>
+      </c>
+      <c r="C3349" t="n">
+        <v>37934.625</v>
+      </c>
+      <c r="D3349" t="n">
+        <v>35545.47265625</v>
+      </c>
+      <c r="E3349" t="n">
+        <v>36154.76953125</v>
+      </c>
+      <c r="F3349" t="n">
+        <v>36154.76953125</v>
+      </c>
+      <c r="G3349" t="n">
+        <v>26007385366</v>
+      </c>
+    </row>
+    <row r="3350">
+      <c r="A3350" s="2" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B3350" t="n">
+        <v>36164.82421875</v>
+      </c>
+      <c r="C3350" t="n">
+        <v>36704.484375</v>
+      </c>
+      <c r="D3350" t="n">
+        <v>35901.234375</v>
+      </c>
+      <c r="E3350" t="n">
+        <v>36596.68359375</v>
+      </c>
+      <c r="F3350" t="n">
+        <v>36596.68359375</v>
+      </c>
+      <c r="G3350" t="n">
+        <v>22445028430</v>
+      </c>
+    </row>
+    <row r="3351">
+      <c r="A3351" s="2" t="n">
+        <v>45248</v>
+      </c>
+      <c r="B3351" t="n">
+        <v>36625.37109375</v>
+      </c>
+      <c r="C3351" t="n">
+        <v>36839.28125</v>
+      </c>
+      <c r="D3351" t="n">
+        <v>36233.3125</v>
+      </c>
+      <c r="E3351" t="n">
+        <v>36585.703125</v>
+      </c>
+      <c r="F3351" t="n">
+        <v>36585.703125</v>
+      </c>
+      <c r="G3351" t="n">
+        <v>11886022717</v>
+      </c>
+    </row>
+    <row r="3352">
+      <c r="A3352" s="2" t="n">
+        <v>45249</v>
+      </c>
+      <c r="B3352" t="n">
+        <v>36585.765625</v>
+      </c>
+      <c r="C3352" t="n">
+        <v>37509.35546875</v>
+      </c>
+      <c r="D3352" t="n">
+        <v>36414.59765625</v>
+      </c>
+      <c r="E3352" t="n">
+        <v>37386.546875</v>
+      </c>
+      <c r="F3352" t="n">
+        <v>37386.546875</v>
+      </c>
+      <c r="G3352" t="n">
+        <v>12915986553</v>
+      </c>
+    </row>
+    <row r="3353">
+      <c r="A3353" s="2" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B3353" t="n">
+        <v>37374.07421875</v>
+      </c>
+      <c r="C3353" t="n">
+        <v>37756.8203125</v>
+      </c>
+      <c r="D3353" t="n">
+        <v>36882.53125</v>
+      </c>
+      <c r="E3353" t="n">
+        <v>37476.95703125</v>
+      </c>
+      <c r="F3353" t="n">
+        <v>37476.95703125</v>
+      </c>
+      <c r="G3353" t="n">
+        <v>20888209068</v>
+      </c>
+    </row>
+    <row r="3354">
+      <c r="A3354" s="2" t="n">
+        <v>45251</v>
+      </c>
+      <c r="B3354" t="n">
+        <v>37469.16015625</v>
+      </c>
+      <c r="C3354" t="n">
+        <v>37631.140625</v>
+      </c>
+      <c r="D3354" t="n">
+        <v>35813.8125</v>
+      </c>
+      <c r="E3354" t="n">
+        <v>35813.8125</v>
+      </c>
+      <c r="F3354" t="n">
+        <v>35813.8125</v>
+      </c>
+      <c r="G3354" t="n">
+        <v>25172163756</v>
+      </c>
+    </row>
+    <row r="3355">
+      <c r="A3355" s="2" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B3355" t="n">
+        <v>35756.5546875</v>
+      </c>
+      <c r="C3355" t="n">
+        <v>37856.98046875</v>
+      </c>
+      <c r="D3355" t="n">
+        <v>35670.97265625</v>
+      </c>
+      <c r="E3355" t="n">
+        <v>37432.33984375</v>
+      </c>
+      <c r="F3355" t="n">
+        <v>37432.33984375</v>
+      </c>
+      <c r="G3355" t="n">
+        <v>24397247860</v>
+      </c>
+    </row>
+    <row r="3356">
+      <c r="A3356" s="2" t="n">
+        <v>45253</v>
+      </c>
+      <c r="B3356" t="n">
+        <v>37420.43359375</v>
+      </c>
+      <c r="C3356" t="n">
+        <v>37643.91796875</v>
+      </c>
+      <c r="D3356" t="n">
+        <v>36923.86328125</v>
+      </c>
+      <c r="E3356" t="n">
+        <v>37289.62109375</v>
+      </c>
+      <c r="F3356" t="n">
+        <v>37289.62109375</v>
+      </c>
+      <c r="G3356" t="n">
+        <v>14214948217</v>
+      </c>
+    </row>
+    <row r="3357">
+      <c r="A3357" s="2" t="n">
+        <v>45254</v>
+      </c>
+      <c r="B3357" t="n">
+        <v>37296.31640625</v>
+      </c>
+      <c r="C3357" t="n">
+        <v>38415.33984375</v>
+      </c>
+      <c r="D3357" t="n">
+        <v>37261.60546875</v>
+      </c>
+      <c r="E3357" t="n">
+        <v>37720.28125</v>
+      </c>
+      <c r="F3357" t="n">
+        <v>37720.28125</v>
+      </c>
+      <c r="G3357" t="n">
+        <v>22922957823</v>
+      </c>
+    </row>
+    <row r="3358">
+      <c r="A3358" s="2" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B3358" t="n">
+        <v>37721.4140625</v>
+      </c>
+      <c r="C3358" t="n">
+        <v>37892.4296875</v>
+      </c>
+      <c r="D3358" t="n">
+        <v>37617.41796875</v>
+      </c>
+      <c r="E3358" t="n">
+        <v>37796.79296875</v>
+      </c>
+      <c r="F3358" t="n">
+        <v>37796.79296875</v>
+      </c>
+      <c r="G3358" t="n">
+        <v>9099571165</v>
+      </c>
+    </row>
+    <row r="3359">
+      <c r="A3359" s="2" t="n">
+        <v>45256</v>
+      </c>
+      <c r="B3359" t="n">
+        <v>37796.828125</v>
+      </c>
+      <c r="C3359" t="n">
+        <v>37820.30078125</v>
+      </c>
+      <c r="D3359" t="n">
+        <v>37162.75</v>
+      </c>
+      <c r="E3359" t="n">
+        <v>37479.12109375</v>
+      </c>
+      <c r="F3359" t="n">
+        <v>37479.12109375</v>
+      </c>
+      <c r="G3359" t="n">
+        <v>13744796068</v>
+      </c>
+    </row>
+    <row r="3360">
+      <c r="A3360" s="2" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B3360" t="n">
+        <v>37454.19140625</v>
+      </c>
+      <c r="C3360" t="n">
+        <v>37559.35546875</v>
+      </c>
+      <c r="D3360" t="n">
+        <v>36750.12890625</v>
+      </c>
+      <c r="E3360" t="n">
+        <v>37254.16796875</v>
+      </c>
+      <c r="F3360" t="n">
+        <v>37254.16796875</v>
+      </c>
+      <c r="G3360" t="n">
+        <v>19002925720</v>
+      </c>
+    </row>
+    <row r="3361">
+      <c r="A3361" s="2" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B3361" t="n">
+        <v>37247.9921875</v>
+      </c>
+      <c r="C3361" t="n">
+        <v>38368.48046875</v>
+      </c>
+      <c r="D3361" t="n">
+        <v>36891.08984375</v>
+      </c>
+      <c r="E3361" t="n">
+        <v>37831.0859375</v>
+      </c>
+      <c r="F3361" t="n">
+        <v>37831.0859375</v>
+      </c>
+      <c r="G3361" t="n">
+        <v>21696137014</v>
+      </c>
+    </row>
+    <row r="3362">
+      <c r="A3362" s="2" t="n">
+        <v>45259</v>
+      </c>
+      <c r="B3362" t="n">
+        <v>37826.10546875</v>
+      </c>
+      <c r="C3362" t="n">
+        <v>38366.11328125</v>
+      </c>
+      <c r="D3362" t="n">
+        <v>37612.6328125</v>
+      </c>
+      <c r="E3362" t="n">
+        <v>37858.4921875</v>
+      </c>
+      <c r="F3362" t="n">
+        <v>37858.4921875</v>
+      </c>
+      <c r="G3362" t="n">
+        <v>20728546658</v>
+      </c>
+    </row>
+    <row r="3363">
+      <c r="A3363" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B3363" t="n">
+        <v>37861.1171875</v>
+      </c>
+      <c r="C3363" t="n">
+        <v>38141.75390625</v>
+      </c>
+      <c r="D3363" t="n">
+        <v>37531.140625</v>
+      </c>
+      <c r="E3363" t="n">
+        <v>37712.74609375</v>
+      </c>
+      <c r="F3363" t="n">
+        <v>37712.74609375</v>
+      </c>
+      <c r="G3363" t="n">
+        <v>18115982627</v>
+      </c>
+    </row>
+    <row r="3364">
+      <c r="A3364" s="2" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B3364" t="n">
+        <v>37718.0078125</v>
+      </c>
+      <c r="C3364" t="n">
+        <v>38954.109375</v>
+      </c>
+      <c r="D3364" t="n">
+        <v>37629.359375</v>
+      </c>
+      <c r="E3364" t="n">
+        <v>38688.75</v>
+      </c>
+      <c r="F3364" t="n">
+        <v>38688.75</v>
+      </c>
+      <c r="G3364" t="n">
+        <v>23512784002</v>
+      </c>
+    </row>
+    <row r="3365">
+      <c r="A3365" s="2" t="n">
+        <v>45262</v>
+      </c>
+      <c r="B3365" t="n">
+        <v>38689.27734375</v>
+      </c>
+      <c r="C3365" t="n">
+        <v>39678.9375</v>
+      </c>
+      <c r="D3365" t="n">
+        <v>38652.59375</v>
+      </c>
+      <c r="E3365" t="n">
+        <v>39476.33203125</v>
+      </c>
+      <c r="F3365" t="n">
+        <v>39476.33203125</v>
+      </c>
+      <c r="G3365" t="n">
+        <v>15534035612</v>
+      </c>
+    </row>
+    <row r="3366">
+      <c r="A3366" s="2" t="n">
+        <v>45263</v>
+      </c>
+      <c r="B3366" t="n">
+        <v>39472.20703125</v>
+      </c>
+      <c r="C3366" t="n">
+        <v>40135.60546875</v>
+      </c>
+      <c r="D3366" t="n">
+        <v>39298.1640625</v>
+      </c>
+      <c r="E3366" t="n">
+        <v>39978.390625</v>
+      </c>
+      <c r="F3366" t="n">
+        <v>39978.390625</v>
+      </c>
+      <c r="G3366" t="n">
+        <v>15769696322</v>
+      </c>
+    </row>
+    <row r="3367">
+      <c r="A3367" s="2" t="n">
+        <v>45264</v>
+      </c>
+      <c r="B3367" t="n">
+        <v>39978.62890625</v>
+      </c>
+      <c r="C3367" t="n">
+        <v>42371.75</v>
+      </c>
+      <c r="D3367" t="n">
+        <v>39978.62890625</v>
+      </c>
+      <c r="E3367" t="n">
+        <v>41980.09765625</v>
+      </c>
+      <c r="F3367" t="n">
+        <v>41980.09765625</v>
+      </c>
+      <c r="G3367" t="n">
+        <v>39856129827</v>
+      </c>
+    </row>
+    <row r="3368">
+      <c r="A3368" s="2" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B3368" t="n">
+        <v>41986.265625</v>
+      </c>
+      <c r="C3368" t="n">
+        <v>44408.6640625</v>
+      </c>
+      <c r="D3368" t="n">
+        <v>41421.1484375</v>
+      </c>
+      <c r="E3368" t="n">
+        <v>44080.6484375</v>
+      </c>
+      <c r="F3368" t="n">
+        <v>44080.6484375</v>
+      </c>
+      <c r="G3368" t="n">
+        <v>36312154535</v>
+      </c>
+    </row>
+    <row r="3369">
+      <c r="A3369" s="2" t="n">
+        <v>45266</v>
+      </c>
+      <c r="B3369" t="n">
+        <v>44080.0234375</v>
+      </c>
+      <c r="C3369" t="n">
+        <v>44265.76953125</v>
+      </c>
+      <c r="D3369" t="n">
+        <v>43478.08203125</v>
+      </c>
+      <c r="E3369" t="n">
+        <v>43746.4453125</v>
+      </c>
+      <c r="F3369" t="n">
+        <v>43746.4453125</v>
+      </c>
+      <c r="G3369" t="n">
+        <v>29909761586</v>
+      </c>
+    </row>
+    <row r="3370">
+      <c r="A3370" s="2" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B3370" t="n">
+        <v>43769.1328125</v>
+      </c>
+      <c r="C3370" t="n">
+        <v>44042.58984375</v>
+      </c>
+      <c r="D3370" t="n">
+        <v>42880.6484375</v>
+      </c>
+      <c r="E3370" t="n">
+        <v>43292.6640625</v>
+      </c>
+      <c r="F3370" t="n">
+        <v>43292.6640625</v>
+      </c>
+      <c r="G3370" t="n">
+        <v>27635760671</v>
+      </c>
+    </row>
+    <row r="3371">
+      <c r="A3371" s="2" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B3371" t="n">
+        <v>43293.13671875</v>
+      </c>
+      <c r="C3371" t="n">
+        <v>44705.515625</v>
+      </c>
+      <c r="D3371" t="n">
+        <v>43125.296875</v>
+      </c>
+      <c r="E3371" t="n">
+        <v>44166.6015625</v>
+      </c>
+      <c r="F3371" t="n">
+        <v>44166.6015625</v>
+      </c>
+      <c r="G3371" t="n">
+        <v>24421116687</v>
+      </c>
+    </row>
+    <row r="3372">
+      <c r="A3372" s="2" t="n">
+        <v>45269</v>
+      </c>
+      <c r="B3372" t="n">
+        <v>44180.01953125</v>
+      </c>
+      <c r="C3372" t="n">
+        <v>44361.2578125</v>
+      </c>
+      <c r="D3372" t="n">
+        <v>43627.59765625</v>
+      </c>
+      <c r="E3372" t="n">
+        <v>43725.984375</v>
+      </c>
+      <c r="F3372" t="n">
+        <v>43725.984375</v>
+      </c>
+      <c r="G3372" t="n">
+        <v>17368210171</v>
+      </c>
+    </row>
+    <row r="3373">
+      <c r="A3373" s="2" t="n">
+        <v>45270</v>
+      </c>
+      <c r="B3373" t="n">
+        <v>43728.3828125</v>
+      </c>
+      <c r="C3373" t="n">
+        <v>44034.625</v>
+      </c>
+      <c r="D3373" t="n">
+        <v>43593.28515625</v>
+      </c>
+      <c r="E3373" t="n">
+        <v>43779.69921875</v>
+      </c>
+      <c r="F3373" t="n">
+        <v>43779.69921875</v>
+      </c>
+      <c r="G3373" t="n">
+        <v>13000481418</v>
+      </c>
+    </row>
+    <row r="3374">
+      <c r="A3374" s="2" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B3374" t="n">
+        <v>43792.01953125</v>
+      </c>
+      <c r="C3374" t="n">
+        <v>43808.375</v>
+      </c>
+      <c r="D3374" t="n">
+        <v>40234.578125</v>
+      </c>
+      <c r="E3374" t="n">
+        <v>41243.83203125</v>
+      </c>
+      <c r="F3374" t="n">
+        <v>41243.83203125</v>
+      </c>
+      <c r="G3374" t="n">
+        <v>40632672038</v>
+      </c>
+    </row>
+    <row r="3375">
+      <c r="A3375" s="2" t="n">
+        <v>45272</v>
+      </c>
+      <c r="B3375" t="n">
+        <v>41238.734375</v>
+      </c>
+      <c r="C3375" t="n">
+        <v>42048.3046875</v>
+      </c>
+      <c r="D3375" t="n">
+        <v>40667.5625</v>
+      </c>
+      <c r="E3375" t="n">
+        <v>41450.22265625</v>
+      </c>
+      <c r="F3375" t="n">
+        <v>41450.22265625</v>
+      </c>
+      <c r="G3375" t="n">
+        <v>24779520132</v>
+      </c>
+    </row>
+    <row r="3376">
+      <c r="A3376" s="2" t="n">
+        <v>45273</v>
+      </c>
+      <c r="B3376" t="n">
+        <v>41468.46484375</v>
+      </c>
+      <c r="C3376" t="n">
+        <v>43429.78125</v>
+      </c>
+      <c r="D3376" t="n">
+        <v>40676.8671875</v>
+      </c>
+      <c r="E3376" t="n">
+        <v>42890.7421875</v>
+      </c>
+      <c r="F3376" t="n">
+        <v>42890.7421875</v>
+      </c>
+      <c r="G3376" t="n">
+        <v>26797884674</v>
+      </c>
+    </row>
+    <row r="3377">
+      <c r="A3377" s="2" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B3377" t="n">
+        <v>42884.26171875</v>
+      </c>
+      <c r="C3377" t="n">
+        <v>43390.859375</v>
+      </c>
+      <c r="D3377" t="n">
+        <v>41767.08984375</v>
+      </c>
+      <c r="E3377" t="n">
+        <v>43023.97265625</v>
+      </c>
+      <c r="F3377" t="n">
+        <v>43023.97265625</v>
+      </c>
+      <c r="G3377" t="n">
+        <v>25578530178</v>
+      </c>
+    </row>
+    <row r="3378">
+      <c r="A3378" s="2" t="n">
+        <v>45275</v>
+      </c>
+      <c r="B3378" t="n">
+        <v>43028.25</v>
+      </c>
+      <c r="C3378" t="n">
+        <v>43087.82421875</v>
+      </c>
+      <c r="D3378" t="n">
+        <v>41692.96875</v>
+      </c>
+      <c r="E3378" t="n">
+        <v>41929.7578125</v>
+      </c>
+      <c r="F3378" t="n">
+        <v>41929.7578125</v>
+      </c>
+      <c r="G3378" t="n">
+        <v>19639442462</v>
+      </c>
+    </row>
+    <row r="3379">
+      <c r="A3379" s="2" t="n">
+        <v>45276</v>
+      </c>
+      <c r="B3379" t="n">
+        <v>41937.7421875</v>
+      </c>
+      <c r="C3379" t="n">
+        <v>42664.9453125</v>
+      </c>
+      <c r="D3379" t="n">
+        <v>41723.11328125</v>
+      </c>
+      <c r="E3379" t="n">
+        <v>42240.1171875</v>
+      </c>
+      <c r="F3379" t="n">
+        <v>42240.1171875</v>
+      </c>
+      <c r="G3379" t="n">
+        <v>14386729590</v>
+      </c>
+    </row>
+    <row r="3380">
+      <c r="A3380" s="2" t="n">
+        <v>45277</v>
+      </c>
+      <c r="B3380" t="n">
+        <v>42236.109375</v>
+      </c>
+      <c r="C3380" t="n">
+        <v>42359.49609375</v>
+      </c>
+      <c r="D3380" t="n">
+        <v>41274.54296875</v>
+      </c>
+      <c r="E3380" t="n">
+        <v>41364.6640625</v>
+      </c>
+      <c r="F3380" t="n">
+        <v>41364.6640625</v>
+      </c>
+      <c r="G3380" t="n">
+        <v>16678702876</v>
+      </c>
+    </row>
+    <row r="3381">
+      <c r="A3381" s="2" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B3381" t="n">
+        <v>41348.203125</v>
+      </c>
+      <c r="C3381" t="n">
+        <v>42720.296875</v>
+      </c>
+      <c r="D3381" t="n">
+        <v>40530.2578125</v>
+      </c>
+      <c r="E3381" t="n">
+        <v>42623.5390625</v>
+      </c>
+      <c r="F3381" t="n">
+        <v>42623.5390625</v>
+      </c>
+      <c r="G3381" t="n">
+        <v>25224642008</v>
+      </c>
+    </row>
+    <row r="3382">
+      <c r="A3382" s="2" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B3382" t="n">
+        <v>42641.51171875</v>
+      </c>
+      <c r="C3382" t="n">
+        <v>43354.296875</v>
+      </c>
+      <c r="D3382" t="n">
+        <v>41826.3359375</v>
+      </c>
+      <c r="E3382" t="n">
+        <v>42270.52734375</v>
+      </c>
+      <c r="F3382" t="n">
+        <v>42270.52734375</v>
+      </c>
+      <c r="G3382" t="n">
+        <v>23171001281</v>
+      </c>
+    </row>
+    <row r="3383">
+      <c r="A3383" s="2" t="n">
+        <v>45281</v>
+      </c>
+      <c r="B3383" t="n">
+        <v>43648.125</v>
+      </c>
+      <c r="C3383" t="n">
+        <v>43725.05078125</v>
+      </c>
+      <c r="D3383" t="n">
+        <v>43559.04296875</v>
+      </c>
+      <c r="E3383" t="n">
+        <v>43588.48828125</v>
+      </c>
+      <c r="F3383" t="n">
+        <v>43588.48828125</v>
+      </c>
+      <c r="G3383" t="n">
+        <v>28905066496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pending changes exported from your codespace
</commit_message>
<xml_diff>
--- a/notebooks-course/data/BTC-USD.xlsx
+++ b/notebooks-course/data/BTC-USD.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3179"/>
+  <dimension ref="A1:G3388"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -73552,22 +73552,4829 @@
         <v>45076</v>
       </c>
       <c r="B3179" t="n">
-        <v>27751.4609375</v>
+        <v>27745.123046875</v>
       </c>
       <c r="C3179" t="n">
-        <v>27884.162109375</v>
+        <v>28044.759765625</v>
       </c>
       <c r="D3179" t="n">
-        <v>27637.66015625</v>
+        <v>27588.501953125</v>
       </c>
       <c r="E3179" t="n">
-        <v>27871.451171875</v>
+        <v>27702.349609375</v>
       </c>
       <c r="F3179" t="n">
-        <v>27871.451171875</v>
+        <v>27702.349609375</v>
       </c>
       <c r="G3179" t="n">
-        <v>12371207168</v>
+        <v>13251081851</v>
+      </c>
+    </row>
+    <row r="3180">
+      <c r="A3180" s="2" t="n">
+        <v>45077</v>
+      </c>
+      <c r="B3180" t="n">
+        <v>27700.529296875</v>
+      </c>
+      <c r="C3180" t="n">
+        <v>27831.677734375</v>
+      </c>
+      <c r="D3180" t="n">
+        <v>26866.453125</v>
+      </c>
+      <c r="E3180" t="n">
+        <v>27219.658203125</v>
+      </c>
+      <c r="F3180" t="n">
+        <v>27219.658203125</v>
+      </c>
+      <c r="G3180" t="n">
+        <v>15656371534</v>
+      </c>
+    </row>
+    <row r="3181">
+      <c r="A3181" s="2" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B3181" t="n">
+        <v>27218.412109375</v>
+      </c>
+      <c r="C3181" t="n">
+        <v>27346.10546875</v>
+      </c>
+      <c r="D3181" t="n">
+        <v>26671.720703125</v>
+      </c>
+      <c r="E3181" t="n">
+        <v>26819.97265625</v>
+      </c>
+      <c r="F3181" t="n">
+        <v>26819.97265625</v>
+      </c>
+      <c r="G3181" t="n">
+        <v>14678970415</v>
+      </c>
+    </row>
+    <row r="3182">
+      <c r="A3182" s="2" t="n">
+        <v>45079</v>
+      </c>
+      <c r="B3182" t="n">
+        <v>26824.556640625</v>
+      </c>
+      <c r="C3182" t="n">
+        <v>27303.861328125</v>
+      </c>
+      <c r="D3182" t="n">
+        <v>26574.64453125</v>
+      </c>
+      <c r="E3182" t="n">
+        <v>27249.58984375</v>
+      </c>
+      <c r="F3182" t="n">
+        <v>27249.58984375</v>
+      </c>
+      <c r="G3182" t="n">
+        <v>14837415000</v>
+      </c>
+    </row>
+    <row r="3183">
+      <c r="A3183" s="2" t="n">
+        <v>45080</v>
+      </c>
+      <c r="B3183" t="n">
+        <v>27252.32421875</v>
+      </c>
+      <c r="C3183" t="n">
+        <v>27317.052734375</v>
+      </c>
+      <c r="D3183" t="n">
+        <v>26958.00390625</v>
+      </c>
+      <c r="E3183" t="n">
+        <v>27075.12890625</v>
+      </c>
+      <c r="F3183" t="n">
+        <v>27075.12890625</v>
+      </c>
+      <c r="G3183" t="n">
+        <v>8385597470</v>
+      </c>
+    </row>
+    <row r="3184">
+      <c r="A3184" s="2" t="n">
+        <v>45081</v>
+      </c>
+      <c r="B3184" t="n">
+        <v>27075.123046875</v>
+      </c>
+      <c r="C3184" t="n">
+        <v>27407.01953125</v>
+      </c>
+      <c r="D3184" t="n">
+        <v>26968.224609375</v>
+      </c>
+      <c r="E3184" t="n">
+        <v>27119.06640625</v>
+      </c>
+      <c r="F3184" t="n">
+        <v>27119.06640625</v>
+      </c>
+      <c r="G3184" t="n">
+        <v>9360912318</v>
+      </c>
+    </row>
+    <row r="3185">
+      <c r="A3185" s="2" t="n">
+        <v>45082</v>
+      </c>
+      <c r="B3185" t="n">
+        <v>27123.109375</v>
+      </c>
+      <c r="C3185" t="n">
+        <v>27129.982421875</v>
+      </c>
+      <c r="D3185" t="n">
+        <v>25445.16796875</v>
+      </c>
+      <c r="E3185" t="n">
+        <v>25760.09765625</v>
+      </c>
+      <c r="F3185" t="n">
+        <v>25760.09765625</v>
+      </c>
+      <c r="G3185" t="n">
+        <v>21513292646</v>
+      </c>
+    </row>
+    <row r="3186">
+      <c r="A3186" s="2" t="n">
+        <v>45083</v>
+      </c>
+      <c r="B3186" t="n">
+        <v>25732.109375</v>
+      </c>
+      <c r="C3186" t="n">
+        <v>27313.8203125</v>
+      </c>
+      <c r="D3186" t="n">
+        <v>25434.8671875</v>
+      </c>
+      <c r="E3186" t="n">
+        <v>27238.783203125</v>
+      </c>
+      <c r="F3186" t="n">
+        <v>27238.783203125</v>
+      </c>
+      <c r="G3186" t="n">
+        <v>21929670693</v>
+      </c>
+    </row>
+    <row r="3187">
+      <c r="A3187" s="2" t="n">
+        <v>45084</v>
+      </c>
+      <c r="B3187" t="n">
+        <v>27235.650390625</v>
+      </c>
+      <c r="C3187" t="n">
+        <v>27332.181640625</v>
+      </c>
+      <c r="D3187" t="n">
+        <v>26146.98828125</v>
+      </c>
+      <c r="E3187" t="n">
+        <v>26345.998046875</v>
+      </c>
+      <c r="F3187" t="n">
+        <v>26345.998046875</v>
+      </c>
+      <c r="G3187" t="n">
+        <v>19530045082</v>
+      </c>
+    </row>
+    <row r="3188">
+      <c r="A3188" s="2" t="n">
+        <v>45085</v>
+      </c>
+      <c r="B3188" t="n">
+        <v>26347.654296875</v>
+      </c>
+      <c r="C3188" t="n">
+        <v>26797.513671875</v>
+      </c>
+      <c r="D3188" t="n">
+        <v>26246.6640625</v>
+      </c>
+      <c r="E3188" t="n">
+        <v>26508.216796875</v>
+      </c>
+      <c r="F3188" t="n">
+        <v>26508.216796875</v>
+      </c>
+      <c r="G3188" t="n">
+        <v>11904824295</v>
+      </c>
+    </row>
+    <row r="3189">
+      <c r="A3189" s="2" t="n">
+        <v>45086</v>
+      </c>
+      <c r="B3189" t="n">
+        <v>26505.923828125</v>
+      </c>
+      <c r="C3189" t="n">
+        <v>26770.2890625</v>
+      </c>
+      <c r="D3189" t="n">
+        <v>26339.314453125</v>
+      </c>
+      <c r="E3189" t="n">
+        <v>26480.375</v>
+      </c>
+      <c r="F3189" t="n">
+        <v>26480.375</v>
+      </c>
+      <c r="G3189" t="n">
+        <v>11015551640</v>
+      </c>
+    </row>
+    <row r="3190">
+      <c r="A3190" s="2" t="n">
+        <v>45087</v>
+      </c>
+      <c r="B3190" t="n">
+        <v>26481.76171875</v>
+      </c>
+      <c r="C3190" t="n">
+        <v>26531.044921875</v>
+      </c>
+      <c r="D3190" t="n">
+        <v>25501.8359375</v>
+      </c>
+      <c r="E3190" t="n">
+        <v>25851.240234375</v>
+      </c>
+      <c r="F3190" t="n">
+        <v>25851.240234375</v>
+      </c>
+      <c r="G3190" t="n">
+        <v>19872933189</v>
+      </c>
+    </row>
+    <row r="3191">
+      <c r="A3191" s="2" t="n">
+        <v>45088</v>
+      </c>
+      <c r="B3191" t="n">
+        <v>25854.03125</v>
+      </c>
+      <c r="C3191" t="n">
+        <v>26203.439453125</v>
+      </c>
+      <c r="D3191" t="n">
+        <v>25668.986328125</v>
+      </c>
+      <c r="E3191" t="n">
+        <v>25940.16796875</v>
+      </c>
+      <c r="F3191" t="n">
+        <v>25940.16796875</v>
+      </c>
+      <c r="G3191" t="n">
+        <v>10732609603</v>
+      </c>
+    </row>
+    <row r="3192">
+      <c r="A3192" s="2" t="n">
+        <v>45089</v>
+      </c>
+      <c r="B3192" t="n">
+        <v>25934.28515625</v>
+      </c>
+      <c r="C3192" t="n">
+        <v>26087.919921875</v>
+      </c>
+      <c r="D3192" t="n">
+        <v>25675.197265625</v>
+      </c>
+      <c r="E3192" t="n">
+        <v>25902.5</v>
+      </c>
+      <c r="F3192" t="n">
+        <v>25902.5</v>
+      </c>
+      <c r="G3192" t="n">
+        <v>11677889997</v>
+      </c>
+    </row>
+    <row r="3193">
+      <c r="A3193" s="2" t="n">
+        <v>45090</v>
+      </c>
+      <c r="B3193" t="n">
+        <v>25902.94140625</v>
+      </c>
+      <c r="C3193" t="n">
+        <v>26376.3515625</v>
+      </c>
+      <c r="D3193" t="n">
+        <v>25728.365234375</v>
+      </c>
+      <c r="E3193" t="n">
+        <v>25918.728515625</v>
+      </c>
+      <c r="F3193" t="n">
+        <v>25918.728515625</v>
+      </c>
+      <c r="G3193" t="n">
+        <v>14143474486</v>
+      </c>
+    </row>
+    <row r="3194">
+      <c r="A3194" s="2" t="n">
+        <v>45091</v>
+      </c>
+      <c r="B3194" t="n">
+        <v>25920.2578125</v>
+      </c>
+      <c r="C3194" t="n">
+        <v>26041.80078125</v>
+      </c>
+      <c r="D3194" t="n">
+        <v>24902.15234375</v>
+      </c>
+      <c r="E3194" t="n">
+        <v>25124.67578125</v>
+      </c>
+      <c r="F3194" t="n">
+        <v>25124.67578125</v>
+      </c>
+      <c r="G3194" t="n">
+        <v>14265717766</v>
+      </c>
+    </row>
+    <row r="3195">
+      <c r="A3195" s="2" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B3195" t="n">
+        <v>25121.673828125</v>
+      </c>
+      <c r="C3195" t="n">
+        <v>25735.30859375</v>
+      </c>
+      <c r="D3195" t="n">
+        <v>24797.16796875</v>
+      </c>
+      <c r="E3195" t="n">
+        <v>25576.39453125</v>
+      </c>
+      <c r="F3195" t="n">
+        <v>25576.39453125</v>
+      </c>
+      <c r="G3195" t="n">
+        <v>15837384409</v>
+      </c>
+    </row>
+    <row r="3196">
+      <c r="A3196" s="2" t="n">
+        <v>45093</v>
+      </c>
+      <c r="B3196" t="n">
+        <v>25575.283203125</v>
+      </c>
+      <c r="C3196" t="n">
+        <v>26463.173828125</v>
+      </c>
+      <c r="D3196" t="n">
+        <v>25245.357421875</v>
+      </c>
+      <c r="E3196" t="n">
+        <v>26327.462890625</v>
+      </c>
+      <c r="F3196" t="n">
+        <v>26327.462890625</v>
+      </c>
+      <c r="G3196" t="n">
+        <v>16324646965</v>
+      </c>
+    </row>
+    <row r="3197">
+      <c r="A3197" s="2" t="n">
+        <v>45094</v>
+      </c>
+      <c r="B3197" t="n">
+        <v>26328.6796875</v>
+      </c>
+      <c r="C3197" t="n">
+        <v>26769.39453125</v>
+      </c>
+      <c r="D3197" t="n">
+        <v>26174.4921875</v>
+      </c>
+      <c r="E3197" t="n">
+        <v>26510.67578125</v>
+      </c>
+      <c r="F3197" t="n">
+        <v>26510.67578125</v>
+      </c>
+      <c r="G3197" t="n">
+        <v>11090276850</v>
+      </c>
+    </row>
+    <row r="3198">
+      <c r="A3198" s="2" t="n">
+        <v>45095</v>
+      </c>
+      <c r="B3198" t="n">
+        <v>26510.45703125</v>
+      </c>
+      <c r="C3198" t="n">
+        <v>26675.92578125</v>
+      </c>
+      <c r="D3198" t="n">
+        <v>26325.890625</v>
+      </c>
+      <c r="E3198" t="n">
+        <v>26336.212890625</v>
+      </c>
+      <c r="F3198" t="n">
+        <v>26336.212890625</v>
+      </c>
+      <c r="G3198" t="n">
+        <v>9565695129</v>
+      </c>
+    </row>
+    <row r="3199">
+      <c r="A3199" s="2" t="n">
+        <v>45096</v>
+      </c>
+      <c r="B3199" t="n">
+        <v>26335.44140625</v>
+      </c>
+      <c r="C3199" t="n">
+        <v>26984.611328125</v>
+      </c>
+      <c r="D3199" t="n">
+        <v>26312.83203125</v>
+      </c>
+      <c r="E3199" t="n">
+        <v>26851.029296875</v>
+      </c>
+      <c r="F3199" t="n">
+        <v>26851.029296875</v>
+      </c>
+      <c r="G3199" t="n">
+        <v>12826986222</v>
+      </c>
+    </row>
+    <row r="3200">
+      <c r="A3200" s="2" t="n">
+        <v>45097</v>
+      </c>
+      <c r="B3200" t="n">
+        <v>26841.6640625</v>
+      </c>
+      <c r="C3200" t="n">
+        <v>28388.96875</v>
+      </c>
+      <c r="D3200" t="n">
+        <v>26668.791015625</v>
+      </c>
+      <c r="E3200" t="n">
+        <v>28327.48828125</v>
+      </c>
+      <c r="F3200" t="n">
+        <v>28327.48828125</v>
+      </c>
+      <c r="G3200" t="n">
+        <v>22211859147</v>
+      </c>
+    </row>
+    <row r="3201">
+      <c r="A3201" s="2" t="n">
+        <v>45098</v>
+      </c>
+      <c r="B3201" t="n">
+        <v>28311.310546875</v>
+      </c>
+      <c r="C3201" t="n">
+        <v>30737.330078125</v>
+      </c>
+      <c r="D3201" t="n">
+        <v>28283.41015625</v>
+      </c>
+      <c r="E3201" t="n">
+        <v>30027.296875</v>
+      </c>
+      <c r="F3201" t="n">
+        <v>30027.296875</v>
+      </c>
+      <c r="G3201" t="n">
+        <v>33346760979</v>
+      </c>
+    </row>
+    <row r="3202">
+      <c r="A3202" s="2" t="n">
+        <v>45099</v>
+      </c>
+      <c r="B3202" t="n">
+        <v>29995.935546875</v>
+      </c>
+      <c r="C3202" t="n">
+        <v>30495.998046875</v>
+      </c>
+      <c r="D3202" t="n">
+        <v>29679.158203125</v>
+      </c>
+      <c r="E3202" t="n">
+        <v>29912.28125</v>
+      </c>
+      <c r="F3202" t="n">
+        <v>29912.28125</v>
+      </c>
+      <c r="G3202" t="n">
+        <v>20653160491</v>
+      </c>
+    </row>
+    <row r="3203">
+      <c r="A3203" s="2" t="n">
+        <v>45100</v>
+      </c>
+      <c r="B3203" t="n">
+        <v>29896.3828125</v>
+      </c>
+      <c r="C3203" t="n">
+        <v>31389.5390625</v>
+      </c>
+      <c r="D3203" t="n">
+        <v>29845.21484375</v>
+      </c>
+      <c r="E3203" t="n">
+        <v>30695.46875</v>
+      </c>
+      <c r="F3203" t="n">
+        <v>30695.46875</v>
+      </c>
+      <c r="G3203" t="n">
+        <v>24115570085</v>
+      </c>
+    </row>
+    <row r="3204">
+      <c r="A3204" s="2" t="n">
+        <v>45101</v>
+      </c>
+      <c r="B3204" t="n">
+        <v>30708.73828125</v>
+      </c>
+      <c r="C3204" t="n">
+        <v>30804.1484375</v>
+      </c>
+      <c r="D3204" t="n">
+        <v>30290.146484375</v>
+      </c>
+      <c r="E3204" t="n">
+        <v>30548.6953125</v>
+      </c>
+      <c r="F3204" t="n">
+        <v>30548.6953125</v>
+      </c>
+      <c r="G3204" t="n">
+        <v>12147822496</v>
+      </c>
+    </row>
+    <row r="3205">
+      <c r="A3205" s="2" t="n">
+        <v>45102</v>
+      </c>
+      <c r="B3205" t="n">
+        <v>30545.150390625</v>
+      </c>
+      <c r="C3205" t="n">
+        <v>31041.271484375</v>
+      </c>
+      <c r="D3205" t="n">
+        <v>30327.943359375</v>
+      </c>
+      <c r="E3205" t="n">
+        <v>30480.26171875</v>
+      </c>
+      <c r="F3205" t="n">
+        <v>30480.26171875</v>
+      </c>
+      <c r="G3205" t="n">
+        <v>12703464114</v>
+      </c>
+    </row>
+    <row r="3206">
+      <c r="A3206" s="2" t="n">
+        <v>45103</v>
+      </c>
+      <c r="B3206" t="n">
+        <v>30480.5234375</v>
+      </c>
+      <c r="C3206" t="n">
+        <v>30636.029296875</v>
+      </c>
+      <c r="D3206" t="n">
+        <v>29955.744140625</v>
+      </c>
+      <c r="E3206" t="n">
+        <v>30271.130859375</v>
+      </c>
+      <c r="F3206" t="n">
+        <v>30271.130859375</v>
+      </c>
+      <c r="G3206" t="n">
+        <v>16493186997</v>
+      </c>
+    </row>
+    <row r="3207">
+      <c r="A3207" s="2" t="n">
+        <v>45104</v>
+      </c>
+      <c r="B3207" t="n">
+        <v>30274.3203125</v>
+      </c>
+      <c r="C3207" t="n">
+        <v>31006.787109375</v>
+      </c>
+      <c r="D3207" t="n">
+        <v>30236.650390625</v>
+      </c>
+      <c r="E3207" t="n">
+        <v>30688.1640625</v>
+      </c>
+      <c r="F3207" t="n">
+        <v>30688.1640625</v>
+      </c>
+      <c r="G3207" t="n">
+        <v>16428827944</v>
+      </c>
+    </row>
+    <row r="3208">
+      <c r="A3208" s="2" t="n">
+        <v>45105</v>
+      </c>
+      <c r="B3208" t="n">
+        <v>30696.560546875</v>
+      </c>
+      <c r="C3208" t="n">
+        <v>30703.279296875</v>
+      </c>
+      <c r="D3208" t="n">
+        <v>29921.822265625</v>
+      </c>
+      <c r="E3208" t="n">
+        <v>30086.24609375</v>
+      </c>
+      <c r="F3208" t="n">
+        <v>30086.24609375</v>
+      </c>
+      <c r="G3208" t="n">
+        <v>14571500779</v>
+      </c>
+    </row>
+    <row r="3209">
+      <c r="A3209" s="2" t="n">
+        <v>45106</v>
+      </c>
+      <c r="B3209" t="n">
+        <v>30086.1875</v>
+      </c>
+      <c r="C3209" t="n">
+        <v>30796.25</v>
+      </c>
+      <c r="D3209" t="n">
+        <v>30057.203125</v>
+      </c>
+      <c r="E3209" t="n">
+        <v>30445.3515625</v>
+      </c>
+      <c r="F3209" t="n">
+        <v>30445.3515625</v>
+      </c>
+      <c r="G3209" t="n">
+        <v>13180860821</v>
+      </c>
+    </row>
+    <row r="3210">
+      <c r="A3210" s="2" t="n">
+        <v>45107</v>
+      </c>
+      <c r="B3210" t="n">
+        <v>30441.353515625</v>
+      </c>
+      <c r="C3210" t="n">
+        <v>31256.86328125</v>
+      </c>
+      <c r="D3210" t="n">
+        <v>29600.275390625</v>
+      </c>
+      <c r="E3210" t="n">
+        <v>30477.251953125</v>
+      </c>
+      <c r="F3210" t="n">
+        <v>30477.251953125</v>
+      </c>
+      <c r="G3210" t="n">
+        <v>26387306197</v>
+      </c>
+    </row>
+    <row r="3211">
+      <c r="A3211" s="2" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B3211" t="n">
+        <v>30471.84765625</v>
+      </c>
+      <c r="C3211" t="n">
+        <v>30641.2890625</v>
+      </c>
+      <c r="D3211" t="n">
+        <v>30328.865234375</v>
+      </c>
+      <c r="E3211" t="n">
+        <v>30590.078125</v>
+      </c>
+      <c r="F3211" t="n">
+        <v>30590.078125</v>
+      </c>
+      <c r="G3211" t="n">
+        <v>9086606733</v>
+      </c>
+    </row>
+    <row r="3212">
+      <c r="A3212" s="2" t="n">
+        <v>45109</v>
+      </c>
+      <c r="B3212" t="n">
+        <v>30587.26953125</v>
+      </c>
+      <c r="C3212" t="n">
+        <v>30766.140625</v>
+      </c>
+      <c r="D3212" t="n">
+        <v>30264.01953125</v>
+      </c>
+      <c r="E3212" t="n">
+        <v>30620.76953125</v>
+      </c>
+      <c r="F3212" t="n">
+        <v>30620.76953125</v>
+      </c>
+      <c r="G3212" t="n">
+        <v>10533418042</v>
+      </c>
+    </row>
+    <row r="3213">
+      <c r="A3213" s="2" t="n">
+        <v>45110</v>
+      </c>
+      <c r="B3213" t="n">
+        <v>30624.515625</v>
+      </c>
+      <c r="C3213" t="n">
+        <v>31375.61328125</v>
+      </c>
+      <c r="D3213" t="n">
+        <v>30586.513671875</v>
+      </c>
+      <c r="E3213" t="n">
+        <v>31156.439453125</v>
+      </c>
+      <c r="F3213" t="n">
+        <v>31156.439453125</v>
+      </c>
+      <c r="G3213" t="n">
+        <v>15271884873</v>
+      </c>
+    </row>
+    <row r="3214">
+      <c r="A3214" s="2" t="n">
+        <v>45111</v>
+      </c>
+      <c r="B3214" t="n">
+        <v>31156.865234375</v>
+      </c>
+      <c r="C3214" t="n">
+        <v>31325.197265625</v>
+      </c>
+      <c r="D3214" t="n">
+        <v>30659.35546875</v>
+      </c>
+      <c r="E3214" t="n">
+        <v>30777.58203125</v>
+      </c>
+      <c r="F3214" t="n">
+        <v>30777.58203125</v>
+      </c>
+      <c r="G3214" t="n">
+        <v>12810828427</v>
+      </c>
+    </row>
+    <row r="3215">
+      <c r="A3215" s="2" t="n">
+        <v>45112</v>
+      </c>
+      <c r="B3215" t="n">
+        <v>30778.724609375</v>
+      </c>
+      <c r="C3215" t="n">
+        <v>30877.330078125</v>
+      </c>
+      <c r="D3215" t="n">
+        <v>30225.61328125</v>
+      </c>
+      <c r="E3215" t="n">
+        <v>30514.166015625</v>
+      </c>
+      <c r="F3215" t="n">
+        <v>30514.166015625</v>
+      </c>
+      <c r="G3215" t="n">
+        <v>12481622280</v>
+      </c>
+    </row>
+    <row r="3216">
+      <c r="A3216" s="2" t="n">
+        <v>45113</v>
+      </c>
+      <c r="B3216" t="n">
+        <v>30507.150390625</v>
+      </c>
+      <c r="C3216" t="n">
+        <v>31460.052734375</v>
+      </c>
+      <c r="D3216" t="n">
+        <v>29892.2265625</v>
+      </c>
+      <c r="E3216" t="n">
+        <v>29909.337890625</v>
+      </c>
+      <c r="F3216" t="n">
+        <v>29909.337890625</v>
+      </c>
+      <c r="G3216" t="n">
+        <v>21129219509</v>
+      </c>
+    </row>
+    <row r="3217">
+      <c r="A3217" s="2" t="n">
+        <v>45114</v>
+      </c>
+      <c r="B3217" t="n">
+        <v>29907.998046875</v>
+      </c>
+      <c r="C3217" t="n">
+        <v>30434.64453125</v>
+      </c>
+      <c r="D3217" t="n">
+        <v>29777.28515625</v>
+      </c>
+      <c r="E3217" t="n">
+        <v>30342.265625</v>
+      </c>
+      <c r="F3217" t="n">
+        <v>30342.265625</v>
+      </c>
+      <c r="G3217" t="n">
+        <v>13384770155</v>
+      </c>
+    </row>
+    <row r="3218">
+      <c r="A3218" s="2" t="n">
+        <v>45115</v>
+      </c>
+      <c r="B3218" t="n">
+        <v>30346.921875</v>
+      </c>
+      <c r="C3218" t="n">
+        <v>30374.4375</v>
+      </c>
+      <c r="D3218" t="n">
+        <v>30080.16015625</v>
+      </c>
+      <c r="E3218" t="n">
+        <v>30292.541015625</v>
+      </c>
+      <c r="F3218" t="n">
+        <v>30292.541015625</v>
+      </c>
+      <c r="G3218" t="n">
+        <v>7509378699</v>
+      </c>
+    </row>
+    <row r="3219">
+      <c r="A3219" s="2" t="n">
+        <v>45116</v>
+      </c>
+      <c r="B3219" t="n">
+        <v>30291.611328125</v>
+      </c>
+      <c r="C3219" t="n">
+        <v>30427.58984375</v>
+      </c>
+      <c r="D3219" t="n">
+        <v>30085.591796875</v>
+      </c>
+      <c r="E3219" t="n">
+        <v>30171.234375</v>
+      </c>
+      <c r="F3219" t="n">
+        <v>30171.234375</v>
+      </c>
+      <c r="G3219" t="n">
+        <v>7903327692</v>
+      </c>
+    </row>
+    <row r="3220">
+      <c r="A3220" s="2" t="n">
+        <v>45117</v>
+      </c>
+      <c r="B3220" t="n">
+        <v>30172.423828125</v>
+      </c>
+      <c r="C3220" t="n">
+        <v>31026.083984375</v>
+      </c>
+      <c r="D3220" t="n">
+        <v>29985.39453125</v>
+      </c>
+      <c r="E3220" t="n">
+        <v>30414.470703125</v>
+      </c>
+      <c r="F3220" t="n">
+        <v>30414.470703125</v>
+      </c>
+      <c r="G3220" t="n">
+        <v>14828209155</v>
+      </c>
+    </row>
+    <row r="3221">
+      <c r="A3221" s="2" t="n">
+        <v>45118</v>
+      </c>
+      <c r="B3221" t="n">
+        <v>30417.6328125</v>
+      </c>
+      <c r="C3221" t="n">
+        <v>30788.314453125</v>
+      </c>
+      <c r="D3221" t="n">
+        <v>30358.09765625</v>
+      </c>
+      <c r="E3221" t="n">
+        <v>30620.951171875</v>
+      </c>
+      <c r="F3221" t="n">
+        <v>30620.951171875</v>
+      </c>
+      <c r="G3221" t="n">
+        <v>12151839152</v>
+      </c>
+    </row>
+    <row r="3222">
+      <c r="A3222" s="2" t="n">
+        <v>45119</v>
+      </c>
+      <c r="B3222" t="n">
+        <v>30622.24609375</v>
+      </c>
+      <c r="C3222" t="n">
+        <v>30959.96484375</v>
+      </c>
+      <c r="D3222" t="n">
+        <v>30228.8359375</v>
+      </c>
+      <c r="E3222" t="n">
+        <v>30391.646484375</v>
+      </c>
+      <c r="F3222" t="n">
+        <v>30391.646484375</v>
+      </c>
+      <c r="G3222" t="n">
+        <v>14805659717</v>
+      </c>
+    </row>
+    <row r="3223">
+      <c r="A3223" s="2" t="n">
+        <v>45120</v>
+      </c>
+      <c r="B3223" t="n">
+        <v>30387.48828125</v>
+      </c>
+      <c r="C3223" t="n">
+        <v>31814.515625</v>
+      </c>
+      <c r="D3223" t="n">
+        <v>30268.3515625</v>
+      </c>
+      <c r="E3223" t="n">
+        <v>31476.048828125</v>
+      </c>
+      <c r="F3223" t="n">
+        <v>31476.048828125</v>
+      </c>
+      <c r="G3223" t="n">
+        <v>23686079548</v>
+      </c>
+    </row>
+    <row r="3224">
+      <c r="A3224" s="2" t="n">
+        <v>45121</v>
+      </c>
+      <c r="B3224" t="n">
+        <v>31474.720703125</v>
+      </c>
+      <c r="C3224" t="n">
+        <v>31582.25390625</v>
+      </c>
+      <c r="D3224" t="n">
+        <v>29966.38671875</v>
+      </c>
+      <c r="E3224" t="n">
+        <v>30334.068359375</v>
+      </c>
+      <c r="F3224" t="n">
+        <v>30334.068359375</v>
+      </c>
+      <c r="G3224" t="n">
+        <v>20917902660</v>
+      </c>
+    </row>
+    <row r="3225">
+      <c r="A3225" s="2" t="n">
+        <v>45122</v>
+      </c>
+      <c r="B3225" t="n">
+        <v>30331.783203125</v>
+      </c>
+      <c r="C3225" t="n">
+        <v>30407.78125</v>
+      </c>
+      <c r="D3225" t="n">
+        <v>30263.462890625</v>
+      </c>
+      <c r="E3225" t="n">
+        <v>30295.806640625</v>
+      </c>
+      <c r="F3225" t="n">
+        <v>30295.806640625</v>
+      </c>
+      <c r="G3225" t="n">
+        <v>8011667756</v>
+      </c>
+    </row>
+    <row r="3226">
+      <c r="A3226" s="2" t="n">
+        <v>45123</v>
+      </c>
+      <c r="B3226" t="n">
+        <v>30297.47265625</v>
+      </c>
+      <c r="C3226" t="n">
+        <v>30437.560546875</v>
+      </c>
+      <c r="D3226" t="n">
+        <v>30089.669921875</v>
+      </c>
+      <c r="E3226" t="n">
+        <v>30249.1328125</v>
+      </c>
+      <c r="F3226" t="n">
+        <v>30249.1328125</v>
+      </c>
+      <c r="G3226" t="n">
+        <v>8516564470</v>
+      </c>
+    </row>
+    <row r="3227">
+      <c r="A3227" s="2" t="n">
+        <v>45124</v>
+      </c>
+      <c r="B3227" t="n">
+        <v>30249.626953125</v>
+      </c>
+      <c r="C3227" t="n">
+        <v>30336.400390625</v>
+      </c>
+      <c r="D3227" t="n">
+        <v>29685.783203125</v>
+      </c>
+      <c r="E3227" t="n">
+        <v>30145.888671875</v>
+      </c>
+      <c r="F3227" t="n">
+        <v>30145.888671875</v>
+      </c>
+      <c r="G3227" t="n">
+        <v>13240156074</v>
+      </c>
+    </row>
+    <row r="3228">
+      <c r="A3228" s="2" t="n">
+        <v>45125</v>
+      </c>
+      <c r="B3228" t="n">
+        <v>30147.0703125</v>
+      </c>
+      <c r="C3228" t="n">
+        <v>30233.65625</v>
+      </c>
+      <c r="D3228" t="n">
+        <v>29556.427734375</v>
+      </c>
+      <c r="E3228" t="n">
+        <v>29856.5625</v>
+      </c>
+      <c r="F3228" t="n">
+        <v>29856.5625</v>
+      </c>
+      <c r="G3228" t="n">
+        <v>13138897269</v>
+      </c>
+    </row>
+    <row r="3229">
+      <c r="A3229" s="2" t="n">
+        <v>45126</v>
+      </c>
+      <c r="B3229" t="n">
+        <v>29862.046875</v>
+      </c>
+      <c r="C3229" t="n">
+        <v>30184.181640625</v>
+      </c>
+      <c r="D3229" t="n">
+        <v>29794.26953125</v>
+      </c>
+      <c r="E3229" t="n">
+        <v>29913.923828125</v>
+      </c>
+      <c r="F3229" t="n">
+        <v>29913.923828125</v>
+      </c>
+      <c r="G3229" t="n">
+        <v>12128602812</v>
+      </c>
+    </row>
+    <row r="3230">
+      <c r="A3230" s="2" t="n">
+        <v>45127</v>
+      </c>
+      <c r="B3230" t="n">
+        <v>29915.25</v>
+      </c>
+      <c r="C3230" t="n">
+        <v>30195.53125</v>
+      </c>
+      <c r="D3230" t="n">
+        <v>29638.095703125</v>
+      </c>
+      <c r="E3230" t="n">
+        <v>29792.015625</v>
+      </c>
+      <c r="F3230" t="n">
+        <v>29792.015625</v>
+      </c>
+      <c r="G3230" t="n">
+        <v>14655207121</v>
+      </c>
+    </row>
+    <row r="3231">
+      <c r="A3231" s="2" t="n">
+        <v>45128</v>
+      </c>
+      <c r="B3231" t="n">
+        <v>29805.111328125</v>
+      </c>
+      <c r="C3231" t="n">
+        <v>30045.998046875</v>
+      </c>
+      <c r="D3231" t="n">
+        <v>29733.8515625</v>
+      </c>
+      <c r="E3231" t="n">
+        <v>29908.744140625</v>
+      </c>
+      <c r="F3231" t="n">
+        <v>29908.744140625</v>
+      </c>
+      <c r="G3231" t="n">
+        <v>10972789818</v>
+      </c>
+    </row>
+    <row r="3232">
+      <c r="A3232" s="2" t="n">
+        <v>45129</v>
+      </c>
+      <c r="B3232" t="n">
+        <v>29908.697265625</v>
+      </c>
+      <c r="C3232" t="n">
+        <v>29991.615234375</v>
+      </c>
+      <c r="D3232" t="n">
+        <v>29664.12109375</v>
+      </c>
+      <c r="E3232" t="n">
+        <v>29771.802734375</v>
+      </c>
+      <c r="F3232" t="n">
+        <v>29771.802734375</v>
+      </c>
+      <c r="G3232" t="n">
+        <v>7873300598</v>
+      </c>
+    </row>
+    <row r="3233">
+      <c r="A3233" s="2" t="n">
+        <v>45130</v>
+      </c>
+      <c r="B3233" t="n">
+        <v>29790.111328125</v>
+      </c>
+      <c r="C3233" t="n">
+        <v>30330.640625</v>
+      </c>
+      <c r="D3233" t="n">
+        <v>29741.52734375</v>
+      </c>
+      <c r="E3233" t="n">
+        <v>30084.5390625</v>
+      </c>
+      <c r="F3233" t="n">
+        <v>30084.5390625</v>
+      </c>
+      <c r="G3233" t="n">
+        <v>9220145050</v>
+      </c>
+    </row>
+    <row r="3234">
+      <c r="A3234" s="2" t="n">
+        <v>45131</v>
+      </c>
+      <c r="B3234" t="n">
+        <v>30081.662109375</v>
+      </c>
+      <c r="C3234" t="n">
+        <v>30093.39453125</v>
+      </c>
+      <c r="D3234" t="n">
+        <v>28934.294921875</v>
+      </c>
+      <c r="E3234" t="n">
+        <v>29176.916015625</v>
+      </c>
+      <c r="F3234" t="n">
+        <v>29176.916015625</v>
+      </c>
+      <c r="G3234" t="n">
+        <v>15395817395</v>
+      </c>
+    </row>
+    <row r="3235">
+      <c r="A3235" s="2" t="n">
+        <v>45132</v>
+      </c>
+      <c r="B3235" t="n">
+        <v>29178.970703125</v>
+      </c>
+      <c r="C3235" t="n">
+        <v>29353.16015625</v>
+      </c>
+      <c r="D3235" t="n">
+        <v>29062.43359375</v>
+      </c>
+      <c r="E3235" t="n">
+        <v>29227.390625</v>
+      </c>
+      <c r="F3235" t="n">
+        <v>29227.390625</v>
+      </c>
+      <c r="G3235" t="n">
+        <v>10266772793</v>
+      </c>
+    </row>
+    <row r="3236">
+      <c r="A3236" s="2" t="n">
+        <v>45133</v>
+      </c>
+      <c r="B3236" t="n">
+        <v>29225.759765625</v>
+      </c>
+      <c r="C3236" t="n">
+        <v>29675.552734375</v>
+      </c>
+      <c r="D3236" t="n">
+        <v>29113.912109375</v>
+      </c>
+      <c r="E3236" t="n">
+        <v>29354.97265625</v>
+      </c>
+      <c r="F3236" t="n">
+        <v>29354.97265625</v>
+      </c>
+      <c r="G3236" t="n">
+        <v>13497554655</v>
+      </c>
+    </row>
+    <row r="3237">
+      <c r="A3237" s="2" t="n">
+        <v>45134</v>
+      </c>
+      <c r="B3237" t="n">
+        <v>29353.798828125</v>
+      </c>
+      <c r="C3237" t="n">
+        <v>29560.966796875</v>
+      </c>
+      <c r="D3237" t="n">
+        <v>29099.3515625</v>
+      </c>
+      <c r="E3237" t="n">
+        <v>29210.689453125</v>
+      </c>
+      <c r="F3237" t="n">
+        <v>29210.689453125</v>
+      </c>
+      <c r="G3237" t="n">
+        <v>10770779217</v>
+      </c>
+    </row>
+    <row r="3238">
+      <c r="A3238" s="2" t="n">
+        <v>45135</v>
+      </c>
+      <c r="B3238" t="n">
+        <v>29212.1640625</v>
+      </c>
+      <c r="C3238" t="n">
+        <v>29521.513671875</v>
+      </c>
+      <c r="D3238" t="n">
+        <v>29125.845703125</v>
+      </c>
+      <c r="E3238" t="n">
+        <v>29319.24609375</v>
+      </c>
+      <c r="F3238" t="n">
+        <v>29319.24609375</v>
+      </c>
+      <c r="G3238" t="n">
+        <v>11218474952</v>
+      </c>
+    </row>
+    <row r="3239">
+      <c r="A3239" s="2" t="n">
+        <v>45136</v>
+      </c>
+      <c r="B3239" t="n">
+        <v>29319.4453125</v>
+      </c>
+      <c r="C3239" t="n">
+        <v>29396.84375</v>
+      </c>
+      <c r="D3239" t="n">
+        <v>29264.166015625</v>
+      </c>
+      <c r="E3239" t="n">
+        <v>29356.91796875</v>
+      </c>
+      <c r="F3239" t="n">
+        <v>29356.91796875</v>
+      </c>
+      <c r="G3239" t="n">
+        <v>6481775959</v>
+      </c>
+    </row>
+    <row r="3240">
+      <c r="A3240" s="2" t="n">
+        <v>45137</v>
+      </c>
+      <c r="B3240" t="n">
+        <v>29357.09375</v>
+      </c>
+      <c r="C3240" t="n">
+        <v>29443.169921875</v>
+      </c>
+      <c r="D3240" t="n">
+        <v>29059.501953125</v>
+      </c>
+      <c r="E3240" t="n">
+        <v>29275.30859375</v>
+      </c>
+      <c r="F3240" t="n">
+        <v>29275.30859375</v>
+      </c>
+      <c r="G3240" t="n">
+        <v>8678454527</v>
+      </c>
+    </row>
+    <row r="3241">
+      <c r="A3241" s="2" t="n">
+        <v>45138</v>
+      </c>
+      <c r="B3241" t="n">
+        <v>29278.314453125</v>
+      </c>
+      <c r="C3241" t="n">
+        <v>29489.873046875</v>
+      </c>
+      <c r="D3241" t="n">
+        <v>29131.578125</v>
+      </c>
+      <c r="E3241" t="n">
+        <v>29230.111328125</v>
+      </c>
+      <c r="F3241" t="n">
+        <v>29230.111328125</v>
+      </c>
+      <c r="G3241" t="n">
+        <v>11656781982</v>
+      </c>
+    </row>
+    <row r="3242">
+      <c r="A3242" s="2" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B3242" t="n">
+        <v>29230.873046875</v>
+      </c>
+      <c r="C3242" t="n">
+        <v>29675.732421875</v>
+      </c>
+      <c r="D3242" t="n">
+        <v>28657.0234375</v>
+      </c>
+      <c r="E3242" t="n">
+        <v>29675.732421875</v>
+      </c>
+      <c r="F3242" t="n">
+        <v>29675.732421875</v>
+      </c>
+      <c r="G3242" t="n">
+        <v>18272392391</v>
+      </c>
+    </row>
+    <row r="3243">
+      <c r="A3243" s="2" t="n">
+        <v>45140</v>
+      </c>
+      <c r="B3243" t="n">
+        <v>29704.146484375</v>
+      </c>
+      <c r="C3243" t="n">
+        <v>29987.998046875</v>
+      </c>
+      <c r="D3243" t="n">
+        <v>28946.509765625</v>
+      </c>
+      <c r="E3243" t="n">
+        <v>29151.958984375</v>
+      </c>
+      <c r="F3243" t="n">
+        <v>29151.958984375</v>
+      </c>
+      <c r="G3243" t="n">
+        <v>19212655598</v>
+      </c>
+    </row>
+    <row r="3244">
+      <c r="A3244" s="2" t="n">
+        <v>45141</v>
+      </c>
+      <c r="B3244" t="n">
+        <v>29161.8125</v>
+      </c>
+      <c r="C3244" t="n">
+        <v>29375.70703125</v>
+      </c>
+      <c r="D3244" t="n">
+        <v>28959.48828125</v>
+      </c>
+      <c r="E3244" t="n">
+        <v>29178.6796875</v>
+      </c>
+      <c r="F3244" t="n">
+        <v>29178.6796875</v>
+      </c>
+      <c r="G3244" t="n">
+        <v>12780357746</v>
+      </c>
+    </row>
+    <row r="3245">
+      <c r="A3245" s="2" t="n">
+        <v>45142</v>
+      </c>
+      <c r="B3245" t="n">
+        <v>29174.3828125</v>
+      </c>
+      <c r="C3245" t="n">
+        <v>29302.078125</v>
+      </c>
+      <c r="D3245" t="n">
+        <v>28885.3359375</v>
+      </c>
+      <c r="E3245" t="n">
+        <v>29074.091796875</v>
+      </c>
+      <c r="F3245" t="n">
+        <v>29074.091796875</v>
+      </c>
+      <c r="G3245" t="n">
+        <v>12036639988</v>
+      </c>
+    </row>
+    <row r="3246">
+      <c r="A3246" s="2" t="n">
+        <v>45143</v>
+      </c>
+      <c r="B3246" t="n">
+        <v>29075.388671875</v>
+      </c>
+      <c r="C3246" t="n">
+        <v>29102.46484375</v>
+      </c>
+      <c r="D3246" t="n">
+        <v>28957.796875</v>
+      </c>
+      <c r="E3246" t="n">
+        <v>29042.126953125</v>
+      </c>
+      <c r="F3246" t="n">
+        <v>29042.126953125</v>
+      </c>
+      <c r="G3246" t="n">
+        <v>6598366353</v>
+      </c>
+    </row>
+    <row r="3247">
+      <c r="A3247" s="2" t="n">
+        <v>45144</v>
+      </c>
+      <c r="B3247" t="n">
+        <v>29043.701171875</v>
+      </c>
+      <c r="C3247" t="n">
+        <v>29160.822265625</v>
+      </c>
+      <c r="D3247" t="n">
+        <v>28963.833984375</v>
+      </c>
+      <c r="E3247" t="n">
+        <v>29041.85546875</v>
+      </c>
+      <c r="F3247" t="n">
+        <v>29041.85546875</v>
+      </c>
+      <c r="G3247" t="n">
+        <v>7269806994</v>
+      </c>
+    </row>
+    <row r="3248">
+      <c r="A3248" s="2" t="n">
+        <v>45145</v>
+      </c>
+      <c r="B3248" t="n">
+        <v>29038.513671875</v>
+      </c>
+      <c r="C3248" t="n">
+        <v>29244.28125</v>
+      </c>
+      <c r="D3248" t="n">
+        <v>28724.140625</v>
+      </c>
+      <c r="E3248" t="n">
+        <v>29180.578125</v>
+      </c>
+      <c r="F3248" t="n">
+        <v>29180.578125</v>
+      </c>
+      <c r="G3248" t="n">
+        <v>13618163710</v>
+      </c>
+    </row>
+    <row r="3249">
+      <c r="A3249" s="2" t="n">
+        <v>45146</v>
+      </c>
+      <c r="B3249" t="n">
+        <v>29180.01953125</v>
+      </c>
+      <c r="C3249" t="n">
+        <v>30176.796875</v>
+      </c>
+      <c r="D3249" t="n">
+        <v>29113.814453125</v>
+      </c>
+      <c r="E3249" t="n">
+        <v>29765.4921875</v>
+      </c>
+      <c r="F3249" t="n">
+        <v>29765.4921875</v>
+      </c>
+      <c r="G3249" t="n">
+        <v>17570561357</v>
+      </c>
+    </row>
+    <row r="3250">
+      <c r="A3250" s="2" t="n">
+        <v>45147</v>
+      </c>
+      <c r="B3250" t="n">
+        <v>29766.6953125</v>
+      </c>
+      <c r="C3250" t="n">
+        <v>30093.435546875</v>
+      </c>
+      <c r="D3250" t="n">
+        <v>29376.80078125</v>
+      </c>
+      <c r="E3250" t="n">
+        <v>29561.494140625</v>
+      </c>
+      <c r="F3250" t="n">
+        <v>29561.494140625</v>
+      </c>
+      <c r="G3250" t="n">
+        <v>18379521213</v>
+      </c>
+    </row>
+    <row r="3251">
+      <c r="A3251" s="2" t="n">
+        <v>45148</v>
+      </c>
+      <c r="B3251" t="n">
+        <v>29563.97265625</v>
+      </c>
+      <c r="C3251" t="n">
+        <v>29688.564453125</v>
+      </c>
+      <c r="D3251" t="n">
+        <v>29354.447265625</v>
+      </c>
+      <c r="E3251" t="n">
+        <v>29429.591796875</v>
+      </c>
+      <c r="F3251" t="n">
+        <v>29429.591796875</v>
+      </c>
+      <c r="G3251" t="n">
+        <v>11865344789</v>
+      </c>
+    </row>
+    <row r="3252">
+      <c r="A3252" s="2" t="n">
+        <v>45149</v>
+      </c>
+      <c r="B3252" t="n">
+        <v>29424.90234375</v>
+      </c>
+      <c r="C3252" t="n">
+        <v>29517.7734375</v>
+      </c>
+      <c r="D3252" t="n">
+        <v>29253.517578125</v>
+      </c>
+      <c r="E3252" t="n">
+        <v>29397.71484375</v>
+      </c>
+      <c r="F3252" t="n">
+        <v>29397.71484375</v>
+      </c>
+      <c r="G3252" t="n">
+        <v>10195168197</v>
+      </c>
+    </row>
+    <row r="3253">
+      <c r="A3253" s="2" t="n">
+        <v>45150</v>
+      </c>
+      <c r="B3253" t="n">
+        <v>29399.787109375</v>
+      </c>
+      <c r="C3253" t="n">
+        <v>29465.11328125</v>
+      </c>
+      <c r="D3253" t="n">
+        <v>29357.587890625</v>
+      </c>
+      <c r="E3253" t="n">
+        <v>29415.96484375</v>
+      </c>
+      <c r="F3253" t="n">
+        <v>29415.96484375</v>
+      </c>
+      <c r="G3253" t="n">
+        <v>6194358008</v>
+      </c>
+    </row>
+    <row r="3254">
+      <c r="A3254" s="2" t="n">
+        <v>45151</v>
+      </c>
+      <c r="B3254" t="n">
+        <v>29416.59375</v>
+      </c>
+      <c r="C3254" t="n">
+        <v>29441.43359375</v>
+      </c>
+      <c r="D3254" t="n">
+        <v>29265.806640625</v>
+      </c>
+      <c r="E3254" t="n">
+        <v>29282.9140625</v>
+      </c>
+      <c r="F3254" t="n">
+        <v>29282.9140625</v>
+      </c>
+      <c r="G3254" t="n">
+        <v>7329897180</v>
+      </c>
+    </row>
+    <row r="3255">
+      <c r="A3255" s="2" t="n">
+        <v>45152</v>
+      </c>
+      <c r="B3255" t="n">
+        <v>29283.263671875</v>
+      </c>
+      <c r="C3255" t="n">
+        <v>29660.25390625</v>
+      </c>
+      <c r="D3255" t="n">
+        <v>29124.10546875</v>
+      </c>
+      <c r="E3255" t="n">
+        <v>29408.443359375</v>
+      </c>
+      <c r="F3255" t="n">
+        <v>29408.443359375</v>
+      </c>
+      <c r="G3255" t="n">
+        <v>14013695304</v>
+      </c>
+    </row>
+    <row r="3256">
+      <c r="A3256" s="2" t="n">
+        <v>45153</v>
+      </c>
+      <c r="B3256" t="n">
+        <v>29408.048828125</v>
+      </c>
+      <c r="C3256" t="n">
+        <v>29439.12109375</v>
+      </c>
+      <c r="D3256" t="n">
+        <v>29088.853515625</v>
+      </c>
+      <c r="E3256" t="n">
+        <v>29170.34765625</v>
+      </c>
+      <c r="F3256" t="n">
+        <v>29170.34765625</v>
+      </c>
+      <c r="G3256" t="n">
+        <v>12640195779</v>
+      </c>
+    </row>
+    <row r="3257">
+      <c r="A3257" s="2" t="n">
+        <v>45154</v>
+      </c>
+      <c r="B3257" t="n">
+        <v>29169.07421875</v>
+      </c>
+      <c r="C3257" t="n">
+        <v>29221.9765625</v>
+      </c>
+      <c r="D3257" t="n">
+        <v>28701.779296875</v>
+      </c>
+      <c r="E3257" t="n">
+        <v>28701.779296875</v>
+      </c>
+      <c r="F3257" t="n">
+        <v>28701.779296875</v>
+      </c>
+      <c r="G3257" t="n">
+        <v>14949271904</v>
+      </c>
+    </row>
+    <row r="3258">
+      <c r="A3258" s="2" t="n">
+        <v>45155</v>
+      </c>
+      <c r="B3258" t="n">
+        <v>28699.802734375</v>
+      </c>
+      <c r="C3258" t="n">
+        <v>28745.947265625</v>
+      </c>
+      <c r="D3258" t="n">
+        <v>25409.111328125</v>
+      </c>
+      <c r="E3258" t="n">
+        <v>26664.55078125</v>
+      </c>
+      <c r="F3258" t="n">
+        <v>26664.55078125</v>
+      </c>
+      <c r="G3258" t="n">
+        <v>31120851211</v>
+      </c>
+    </row>
+    <row r="3259">
+      <c r="A3259" s="2" t="n">
+        <v>45156</v>
+      </c>
+      <c r="B3259" t="n">
+        <v>26636.078125</v>
+      </c>
+      <c r="C3259" t="n">
+        <v>26808.1953125</v>
+      </c>
+      <c r="D3259" t="n">
+        <v>25668.921875</v>
+      </c>
+      <c r="E3259" t="n">
+        <v>26049.556640625</v>
+      </c>
+      <c r="F3259" t="n">
+        <v>26049.556640625</v>
+      </c>
+      <c r="G3259" t="n">
+        <v>24026236529</v>
+      </c>
+    </row>
+    <row r="3260">
+      <c r="A3260" s="2" t="n">
+        <v>45157</v>
+      </c>
+      <c r="B3260" t="n">
+        <v>26047.83203125</v>
+      </c>
+      <c r="C3260" t="n">
+        <v>26249.44921875</v>
+      </c>
+      <c r="D3260" t="n">
+        <v>25802.408203125</v>
+      </c>
+      <c r="E3260" t="n">
+        <v>26096.205078125</v>
+      </c>
+      <c r="F3260" t="n">
+        <v>26096.205078125</v>
+      </c>
+      <c r="G3260" t="n">
+        <v>10631443812</v>
+      </c>
+    </row>
+    <row r="3261">
+      <c r="A3261" s="2" t="n">
+        <v>45158</v>
+      </c>
+      <c r="B3261" t="n">
+        <v>26096.861328125</v>
+      </c>
+      <c r="C3261" t="n">
+        <v>26260.681640625</v>
+      </c>
+      <c r="D3261" t="n">
+        <v>26004.314453125</v>
+      </c>
+      <c r="E3261" t="n">
+        <v>26189.583984375</v>
+      </c>
+      <c r="F3261" t="n">
+        <v>26189.583984375</v>
+      </c>
+      <c r="G3261" t="n">
+        <v>9036580420</v>
+      </c>
+    </row>
+    <row r="3262">
+      <c r="A3262" s="2" t="n">
+        <v>45159</v>
+      </c>
+      <c r="B3262" t="n">
+        <v>26188.69140625</v>
+      </c>
+      <c r="C3262" t="n">
+        <v>26220.201171875</v>
+      </c>
+      <c r="D3262" t="n">
+        <v>25846.087890625</v>
+      </c>
+      <c r="E3262" t="n">
+        <v>26124.140625</v>
+      </c>
+      <c r="F3262" t="n">
+        <v>26124.140625</v>
+      </c>
+      <c r="G3262" t="n">
+        <v>13371557893</v>
+      </c>
+    </row>
+    <row r="3263">
+      <c r="A3263" s="2" t="n">
+        <v>45160</v>
+      </c>
+      <c r="B3263" t="n">
+        <v>26130.748046875</v>
+      </c>
+      <c r="C3263" t="n">
+        <v>26135.5078125</v>
+      </c>
+      <c r="D3263" t="n">
+        <v>25520.728515625</v>
+      </c>
+      <c r="E3263" t="n">
+        <v>26031.65625</v>
+      </c>
+      <c r="F3263" t="n">
+        <v>26031.65625</v>
+      </c>
+      <c r="G3263" t="n">
+        <v>14503820706</v>
+      </c>
+    </row>
+    <row r="3264">
+      <c r="A3264" s="2" t="n">
+        <v>45161</v>
+      </c>
+      <c r="B3264" t="n">
+        <v>26040.474609375</v>
+      </c>
+      <c r="C3264" t="n">
+        <v>26786.8984375</v>
+      </c>
+      <c r="D3264" t="n">
+        <v>25804.998046875</v>
+      </c>
+      <c r="E3264" t="n">
+        <v>26431.640625</v>
+      </c>
+      <c r="F3264" t="n">
+        <v>26431.640625</v>
+      </c>
+      <c r="G3264" t="n">
+        <v>16985265785</v>
+      </c>
+    </row>
+    <row r="3265">
+      <c r="A3265" s="2" t="n">
+        <v>45162</v>
+      </c>
+      <c r="B3265" t="n">
+        <v>26431.51953125</v>
+      </c>
+      <c r="C3265" t="n">
+        <v>26554.91015625</v>
+      </c>
+      <c r="D3265" t="n">
+        <v>25914.92578125</v>
+      </c>
+      <c r="E3265" t="n">
+        <v>26162.373046875</v>
+      </c>
+      <c r="F3265" t="n">
+        <v>26162.373046875</v>
+      </c>
+      <c r="G3265" t="n">
+        <v>12871532023</v>
+      </c>
+    </row>
+    <row r="3266">
+      <c r="A3266" s="2" t="n">
+        <v>45163</v>
+      </c>
+      <c r="B3266" t="n">
+        <v>26163.6796875</v>
+      </c>
+      <c r="C3266" t="n">
+        <v>26248.103515625</v>
+      </c>
+      <c r="D3266" t="n">
+        <v>25786.8125</v>
+      </c>
+      <c r="E3266" t="n">
+        <v>26047.66796875</v>
+      </c>
+      <c r="F3266" t="n">
+        <v>26047.66796875</v>
+      </c>
+      <c r="G3266" t="n">
+        <v>12406045118</v>
+      </c>
+    </row>
+    <row r="3267">
+      <c r="A3267" s="2" t="n">
+        <v>45164</v>
+      </c>
+      <c r="B3267" t="n">
+        <v>26047.234375</v>
+      </c>
+      <c r="C3267" t="n">
+        <v>26107.384765625</v>
+      </c>
+      <c r="D3267" t="n">
+        <v>25983.87890625</v>
+      </c>
+      <c r="E3267" t="n">
+        <v>26008.462890625</v>
+      </c>
+      <c r="F3267" t="n">
+        <v>26008.462890625</v>
+      </c>
+      <c r="G3267" t="n">
+        <v>6034817316</v>
+      </c>
+    </row>
+    <row r="3268">
+      <c r="A3268" s="2" t="n">
+        <v>45165</v>
+      </c>
+      <c r="B3268" t="n">
+        <v>26008.2421875</v>
+      </c>
+      <c r="C3268" t="n">
+        <v>26165.373046875</v>
+      </c>
+      <c r="D3268" t="n">
+        <v>25965.09765625</v>
+      </c>
+      <c r="E3268" t="n">
+        <v>26089.693359375</v>
+      </c>
+      <c r="F3268" t="n">
+        <v>26089.693359375</v>
+      </c>
+      <c r="G3268" t="n">
+        <v>6913768611</v>
+      </c>
+    </row>
+    <row r="3269">
+      <c r="A3269" s="2" t="n">
+        <v>45166</v>
+      </c>
+      <c r="B3269" t="n">
+        <v>26089.615234375</v>
+      </c>
+      <c r="C3269" t="n">
+        <v>26198.578125</v>
+      </c>
+      <c r="D3269" t="n">
+        <v>25880.599609375</v>
+      </c>
+      <c r="E3269" t="n">
+        <v>26106.150390625</v>
+      </c>
+      <c r="F3269" t="n">
+        <v>26106.150390625</v>
+      </c>
+      <c r="G3269" t="n">
+        <v>11002805166</v>
+      </c>
+    </row>
+    <row r="3270">
+      <c r="A3270" s="2" t="n">
+        <v>45167</v>
+      </c>
+      <c r="B3270" t="n">
+        <v>26102.486328125</v>
+      </c>
+      <c r="C3270" t="n">
+        <v>28089.337890625</v>
+      </c>
+      <c r="D3270" t="n">
+        <v>25912.62890625</v>
+      </c>
+      <c r="E3270" t="n">
+        <v>27727.392578125</v>
+      </c>
+      <c r="F3270" t="n">
+        <v>27727.392578125</v>
+      </c>
+      <c r="G3270" t="n">
+        <v>29368391712</v>
+      </c>
+    </row>
+    <row r="3271">
+      <c r="A3271" s="2" t="n">
+        <v>45168</v>
+      </c>
+      <c r="B3271" t="n">
+        <v>27726.083984375</v>
+      </c>
+      <c r="C3271" t="n">
+        <v>27760.16015625</v>
+      </c>
+      <c r="D3271" t="n">
+        <v>27069.20703125</v>
+      </c>
+      <c r="E3271" t="n">
+        <v>27297.265625</v>
+      </c>
+      <c r="F3271" t="n">
+        <v>27297.265625</v>
+      </c>
+      <c r="G3271" t="n">
+        <v>16343655235</v>
+      </c>
+    </row>
+    <row r="3272">
+      <c r="A3272" s="2" t="n">
+        <v>45169</v>
+      </c>
+      <c r="B3272" t="n">
+        <v>27301.9296875</v>
+      </c>
+      <c r="C3272" t="n">
+        <v>27456.078125</v>
+      </c>
+      <c r="D3272" t="n">
+        <v>25752.9296875</v>
+      </c>
+      <c r="E3272" t="n">
+        <v>25931.47265625</v>
+      </c>
+      <c r="F3272" t="n">
+        <v>25931.47265625</v>
+      </c>
+      <c r="G3272" t="n">
+        <v>20181001451</v>
+      </c>
+    </row>
+    <row r="3273">
+      <c r="A3273" s="2" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B3273" t="n">
+        <v>25934.021484375</v>
+      </c>
+      <c r="C3273" t="n">
+        <v>26125.869140625</v>
+      </c>
+      <c r="D3273" t="n">
+        <v>25362.609375</v>
+      </c>
+      <c r="E3273" t="n">
+        <v>25800.724609375</v>
+      </c>
+      <c r="F3273" t="n">
+        <v>25800.724609375</v>
+      </c>
+      <c r="G3273" t="n">
+        <v>17202862221</v>
+      </c>
+    </row>
+    <row r="3274">
+      <c r="A3274" s="2" t="n">
+        <v>45171</v>
+      </c>
+      <c r="B3274" t="n">
+        <v>25800.91015625</v>
+      </c>
+      <c r="C3274" t="n">
+        <v>25970.28515625</v>
+      </c>
+      <c r="D3274" t="n">
+        <v>25753.09375</v>
+      </c>
+      <c r="E3274" t="n">
+        <v>25868.798828125</v>
+      </c>
+      <c r="F3274" t="n">
+        <v>25868.798828125</v>
+      </c>
+      <c r="G3274" t="n">
+        <v>10100387473</v>
+      </c>
+    </row>
+    <row r="3275">
+      <c r="A3275" s="2" t="n">
+        <v>45172</v>
+      </c>
+      <c r="B3275" t="n">
+        <v>25869.47265625</v>
+      </c>
+      <c r="C3275" t="n">
+        <v>26087.1484375</v>
+      </c>
+      <c r="D3275" t="n">
+        <v>25817.03125</v>
+      </c>
+      <c r="E3275" t="n">
+        <v>25969.56640625</v>
+      </c>
+      <c r="F3275" t="n">
+        <v>25969.56640625</v>
+      </c>
+      <c r="G3275" t="n">
+        <v>8962524523</v>
+      </c>
+    </row>
+    <row r="3276">
+      <c r="A3276" s="2" t="n">
+        <v>45173</v>
+      </c>
+      <c r="B3276" t="n">
+        <v>25968.169921875</v>
+      </c>
+      <c r="C3276" t="n">
+        <v>26081.525390625</v>
+      </c>
+      <c r="D3276" t="n">
+        <v>25657.025390625</v>
+      </c>
+      <c r="E3276" t="n">
+        <v>25812.416015625</v>
+      </c>
+      <c r="F3276" t="n">
+        <v>25812.416015625</v>
+      </c>
+      <c r="G3276" t="n">
+        <v>10680635106</v>
+      </c>
+    </row>
+    <row r="3277">
+      <c r="A3277" s="2" t="n">
+        <v>45174</v>
+      </c>
+      <c r="B3277" t="n">
+        <v>25814.95703125</v>
+      </c>
+      <c r="C3277" t="n">
+        <v>25858.375</v>
+      </c>
+      <c r="D3277" t="n">
+        <v>25589.98828125</v>
+      </c>
+      <c r="E3277" t="n">
+        <v>25779.982421875</v>
+      </c>
+      <c r="F3277" t="n">
+        <v>25779.982421875</v>
+      </c>
+      <c r="G3277" t="n">
+        <v>11094740040</v>
+      </c>
+    </row>
+    <row r="3278">
+      <c r="A3278" s="2" t="n">
+        <v>45175</v>
+      </c>
+      <c r="B3278" t="n">
+        <v>25783.931640625</v>
+      </c>
+      <c r="C3278" t="n">
+        <v>25953.015625</v>
+      </c>
+      <c r="D3278" t="n">
+        <v>25404.359375</v>
+      </c>
+      <c r="E3278" t="n">
+        <v>25753.236328125</v>
+      </c>
+      <c r="F3278" t="n">
+        <v>25753.236328125</v>
+      </c>
+      <c r="G3278" t="n">
+        <v>12752705327</v>
+      </c>
+    </row>
+    <row r="3279">
+      <c r="A3279" s="2" t="n">
+        <v>45176</v>
+      </c>
+      <c r="B3279" t="n">
+        <v>25748.3125</v>
+      </c>
+      <c r="C3279" t="n">
+        <v>26409.302734375</v>
+      </c>
+      <c r="D3279" t="n">
+        <v>25608.201171875</v>
+      </c>
+      <c r="E3279" t="n">
+        <v>26240.1953125</v>
+      </c>
+      <c r="F3279" t="n">
+        <v>26240.1953125</v>
+      </c>
+      <c r="G3279" t="n">
+        <v>11088307100</v>
+      </c>
+    </row>
+    <row r="3280">
+      <c r="A3280" s="2" t="n">
+        <v>45177</v>
+      </c>
+      <c r="B3280" t="n">
+        <v>26245.208984375</v>
+      </c>
+      <c r="C3280" t="n">
+        <v>26414.005859375</v>
+      </c>
+      <c r="D3280" t="n">
+        <v>25677.48046875</v>
+      </c>
+      <c r="E3280" t="n">
+        <v>25905.654296875</v>
+      </c>
+      <c r="F3280" t="n">
+        <v>25905.654296875</v>
+      </c>
+      <c r="G3280" t="n">
+        <v>10817356400</v>
+      </c>
+    </row>
+    <row r="3281">
+      <c r="A3281" s="2" t="n">
+        <v>45178</v>
+      </c>
+      <c r="B3281" t="n">
+        <v>25905.42578125</v>
+      </c>
+      <c r="C3281" t="n">
+        <v>25921.9765625</v>
+      </c>
+      <c r="D3281" t="n">
+        <v>25810.494140625</v>
+      </c>
+      <c r="E3281" t="n">
+        <v>25895.677734375</v>
+      </c>
+      <c r="F3281" t="n">
+        <v>25895.677734375</v>
+      </c>
+      <c r="G3281" t="n">
+        <v>5481314132</v>
+      </c>
+    </row>
+    <row r="3282">
+      <c r="A3282" s="2" t="n">
+        <v>45179</v>
+      </c>
+      <c r="B3282" t="n">
+        <v>25895.2109375</v>
+      </c>
+      <c r="C3282" t="n">
+        <v>25978.130859375</v>
+      </c>
+      <c r="D3282" t="n">
+        <v>25640.26171875</v>
+      </c>
+      <c r="E3282" t="n">
+        <v>25832.2265625</v>
+      </c>
+      <c r="F3282" t="n">
+        <v>25832.2265625</v>
+      </c>
+      <c r="G3282" t="n">
+        <v>7899553047</v>
+      </c>
+    </row>
+    <row r="3283">
+      <c r="A3283" s="2" t="n">
+        <v>45180</v>
+      </c>
+      <c r="B3283" t="n">
+        <v>25831.71484375</v>
+      </c>
+      <c r="C3283" t="n">
+        <v>25883.947265625</v>
+      </c>
+      <c r="D3283" t="n">
+        <v>24930.296875</v>
+      </c>
+      <c r="E3283" t="n">
+        <v>25162.654296875</v>
+      </c>
+      <c r="F3283" t="n">
+        <v>25162.654296875</v>
+      </c>
+      <c r="G3283" t="n">
+        <v>14600006467</v>
+      </c>
+    </row>
+    <row r="3284">
+      <c r="A3284" s="2" t="n">
+        <v>45181</v>
+      </c>
+      <c r="B3284" t="n">
+        <v>25160.658203125</v>
+      </c>
+      <c r="C3284" t="n">
+        <v>26451.939453125</v>
+      </c>
+      <c r="D3284" t="n">
+        <v>25133.078125</v>
+      </c>
+      <c r="E3284" t="n">
+        <v>25833.34375</v>
+      </c>
+      <c r="F3284" t="n">
+        <v>25833.34375</v>
+      </c>
+      <c r="G3284" t="n">
+        <v>18657279324</v>
+      </c>
+    </row>
+    <row r="3285">
+      <c r="A3285" s="2" t="n">
+        <v>45182</v>
+      </c>
+      <c r="B3285" t="n">
+        <v>25837.5546875</v>
+      </c>
+      <c r="C3285" t="n">
+        <v>26376.11328125</v>
+      </c>
+      <c r="D3285" t="n">
+        <v>25781.123046875</v>
+      </c>
+      <c r="E3285" t="n">
+        <v>26228.32421875</v>
+      </c>
+      <c r="F3285" t="n">
+        <v>26228.32421875</v>
+      </c>
+      <c r="G3285" t="n">
+        <v>13072077070</v>
+      </c>
+    </row>
+    <row r="3286">
+      <c r="A3286" s="2" t="n">
+        <v>45183</v>
+      </c>
+      <c r="B3286" t="n">
+        <v>26228.27734375</v>
+      </c>
+      <c r="C3286" t="n">
+        <v>26774.623046875</v>
+      </c>
+      <c r="D3286" t="n">
+        <v>26171.451171875</v>
+      </c>
+      <c r="E3286" t="n">
+        <v>26539.673828125</v>
+      </c>
+      <c r="F3286" t="n">
+        <v>26539.673828125</v>
+      </c>
+      <c r="G3286" t="n">
+        <v>13811359124</v>
+      </c>
+    </row>
+    <row r="3287">
+      <c r="A3287" s="2" t="n">
+        <v>45184</v>
+      </c>
+      <c r="B3287" t="n">
+        <v>26533.818359375</v>
+      </c>
+      <c r="C3287" t="n">
+        <v>26840.498046875</v>
+      </c>
+      <c r="D3287" t="n">
+        <v>26240.701171875</v>
+      </c>
+      <c r="E3287" t="n">
+        <v>26608.693359375</v>
+      </c>
+      <c r="F3287" t="n">
+        <v>26608.693359375</v>
+      </c>
+      <c r="G3287" t="n">
+        <v>11479735788</v>
+      </c>
+    </row>
+    <row r="3288">
+      <c r="A3288" s="2" t="n">
+        <v>45185</v>
+      </c>
+      <c r="B3288" t="n">
+        <v>26606.19921875</v>
+      </c>
+      <c r="C3288" t="n">
+        <v>26754.76953125</v>
+      </c>
+      <c r="D3288" t="n">
+        <v>26473.890625</v>
+      </c>
+      <c r="E3288" t="n">
+        <v>26568.28125</v>
+      </c>
+      <c r="F3288" t="n">
+        <v>26568.28125</v>
+      </c>
+      <c r="G3288" t="n">
+        <v>7402031417</v>
+      </c>
+    </row>
+    <row r="3289">
+      <c r="A3289" s="2" t="n">
+        <v>45186</v>
+      </c>
+      <c r="B3289" t="n">
+        <v>26567.927734375</v>
+      </c>
+      <c r="C3289" t="n">
+        <v>26617.998046875</v>
+      </c>
+      <c r="D3289" t="n">
+        <v>26445.07421875</v>
+      </c>
+      <c r="E3289" t="n">
+        <v>26534.1875</v>
+      </c>
+      <c r="F3289" t="n">
+        <v>26534.1875</v>
+      </c>
+      <c r="G3289" t="n">
+        <v>6774210670</v>
+      </c>
+    </row>
+    <row r="3290">
+      <c r="A3290" s="2" t="n">
+        <v>45187</v>
+      </c>
+      <c r="B3290" t="n">
+        <v>26532.994140625</v>
+      </c>
+      <c r="C3290" t="n">
+        <v>27414.734375</v>
+      </c>
+      <c r="D3290" t="n">
+        <v>26415.515625</v>
+      </c>
+      <c r="E3290" t="n">
+        <v>26754.28125</v>
+      </c>
+      <c r="F3290" t="n">
+        <v>26754.28125</v>
+      </c>
+      <c r="G3290" t="n">
+        <v>15615339655</v>
+      </c>
+    </row>
+    <row r="3291">
+      <c r="A3291" s="2" t="n">
+        <v>45188</v>
+      </c>
+      <c r="B3291" t="n">
+        <v>26760.8515625</v>
+      </c>
+      <c r="C3291" t="n">
+        <v>27488.763671875</v>
+      </c>
+      <c r="D3291" t="n">
+        <v>26681.60546875</v>
+      </c>
+      <c r="E3291" t="n">
+        <v>27211.1171875</v>
+      </c>
+      <c r="F3291" t="n">
+        <v>27211.1171875</v>
+      </c>
+      <c r="G3291" t="n">
+        <v>13807690550</v>
+      </c>
+    </row>
+    <row r="3292">
+      <c r="A3292" s="2" t="n">
+        <v>45189</v>
+      </c>
+      <c r="B3292" t="n">
+        <v>27210.228515625</v>
+      </c>
+      <c r="C3292" t="n">
+        <v>27379.505859375</v>
+      </c>
+      <c r="D3292" t="n">
+        <v>26864.08203125</v>
+      </c>
+      <c r="E3292" t="n">
+        <v>27132.0078125</v>
+      </c>
+      <c r="F3292" t="n">
+        <v>27132.0078125</v>
+      </c>
+      <c r="G3292" t="n">
+        <v>13281116604</v>
+      </c>
+    </row>
+    <row r="3293">
+      <c r="A3293" s="2" t="n">
+        <v>45190</v>
+      </c>
+      <c r="B3293" t="n">
+        <v>27129.83984375</v>
+      </c>
+      <c r="C3293" t="n">
+        <v>27152.939453125</v>
+      </c>
+      <c r="D3293" t="n">
+        <v>26389.30078125</v>
+      </c>
+      <c r="E3293" t="n">
+        <v>26567.6328125</v>
+      </c>
+      <c r="F3293" t="n">
+        <v>26567.6328125</v>
+      </c>
+      <c r="G3293" t="n">
+        <v>13371443708</v>
+      </c>
+    </row>
+    <row r="3294">
+      <c r="A3294" s="2" t="n">
+        <v>45191</v>
+      </c>
+      <c r="B3294" t="n">
+        <v>26564.056640625</v>
+      </c>
+      <c r="C3294" t="n">
+        <v>26726.078125</v>
+      </c>
+      <c r="D3294" t="n">
+        <v>26495.533203125</v>
+      </c>
+      <c r="E3294" t="n">
+        <v>26579.568359375</v>
+      </c>
+      <c r="F3294" t="n">
+        <v>26579.568359375</v>
+      </c>
+      <c r="G3294" t="n">
+        <v>10578746709</v>
+      </c>
+    </row>
+    <row r="3295">
+      <c r="A3295" s="2" t="n">
+        <v>45192</v>
+      </c>
+      <c r="B3295" t="n">
+        <v>26578.556640625</v>
+      </c>
+      <c r="C3295" t="n">
+        <v>26634.185546875</v>
+      </c>
+      <c r="D3295" t="n">
+        <v>26520.51953125</v>
+      </c>
+      <c r="E3295" t="n">
+        <v>26579.390625</v>
+      </c>
+      <c r="F3295" t="n">
+        <v>26579.390625</v>
+      </c>
+      <c r="G3295" t="n">
+        <v>7404700301</v>
+      </c>
+    </row>
+    <row r="3296">
+      <c r="A3296" s="2" t="n">
+        <v>45193</v>
+      </c>
+      <c r="B3296" t="n">
+        <v>26579.373046875</v>
+      </c>
+      <c r="C3296" t="n">
+        <v>26716.05859375</v>
+      </c>
+      <c r="D3296" t="n">
+        <v>26221.05078125</v>
+      </c>
+      <c r="E3296" t="n">
+        <v>26256.826171875</v>
+      </c>
+      <c r="F3296" t="n">
+        <v>26256.826171875</v>
+      </c>
+      <c r="G3296" t="n">
+        <v>8192867686</v>
+      </c>
+    </row>
+    <row r="3297">
+      <c r="A3297" s="2" t="n">
+        <v>45194</v>
+      </c>
+      <c r="B3297" t="n">
+        <v>26253.775390625</v>
+      </c>
+      <c r="C3297" t="n">
+        <v>26421.5078125</v>
+      </c>
+      <c r="D3297" t="n">
+        <v>26011.46875</v>
+      </c>
+      <c r="E3297" t="n">
+        <v>26298.48046875</v>
+      </c>
+      <c r="F3297" t="n">
+        <v>26298.48046875</v>
+      </c>
+      <c r="G3297" t="n">
+        <v>11997833257</v>
+      </c>
+    </row>
+    <row r="3298">
+      <c r="A3298" s="2" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3298" t="n">
+        <v>26294.7578125</v>
+      </c>
+      <c r="C3298" t="n">
+        <v>26389.884765625</v>
+      </c>
+      <c r="D3298" t="n">
+        <v>26090.712890625</v>
+      </c>
+      <c r="E3298" t="n">
+        <v>26217.25</v>
+      </c>
+      <c r="F3298" t="n">
+        <v>26217.25</v>
+      </c>
+      <c r="G3298" t="n">
+        <v>9985498161</v>
+      </c>
+    </row>
+    <row r="3299">
+      <c r="A3299" s="2" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B3299" t="n">
+        <v>26209.498046875</v>
+      </c>
+      <c r="C3299" t="n">
+        <v>26817.841796875</v>
+      </c>
+      <c r="D3299" t="n">
+        <v>26111.46484375</v>
+      </c>
+      <c r="E3299" t="n">
+        <v>26352.716796875</v>
+      </c>
+      <c r="F3299" t="n">
+        <v>26352.716796875</v>
+      </c>
+      <c r="G3299" t="n">
+        <v>11718380997</v>
+      </c>
+    </row>
+    <row r="3300">
+      <c r="A3300" s="2" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B3300" t="n">
+        <v>26355.8125</v>
+      </c>
+      <c r="C3300" t="n">
+        <v>27259.5</v>
+      </c>
+      <c r="D3300" t="n">
+        <v>26327.322265625</v>
+      </c>
+      <c r="E3300" t="n">
+        <v>27021.546875</v>
+      </c>
+      <c r="F3300" t="n">
+        <v>27021.546875</v>
+      </c>
+      <c r="G3300" t="n">
+        <v>14079002707</v>
+      </c>
+    </row>
+    <row r="3301">
+      <c r="A3301" s="2" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B3301" t="n">
+        <v>27024.841796875</v>
+      </c>
+      <c r="C3301" t="n">
+        <v>27225.9375</v>
+      </c>
+      <c r="D3301" t="n">
+        <v>26721.763671875</v>
+      </c>
+      <c r="E3301" t="n">
+        <v>26911.720703125</v>
+      </c>
+      <c r="F3301" t="n">
+        <v>26911.720703125</v>
+      </c>
+      <c r="G3301" t="n">
+        <v>10396435377</v>
+      </c>
+    </row>
+    <row r="3302">
+      <c r="A3302" s="2" t="n">
+        <v>45199</v>
+      </c>
+      <c r="B3302" t="n">
+        <v>26911.689453125</v>
+      </c>
+      <c r="C3302" t="n">
+        <v>27091.794921875</v>
+      </c>
+      <c r="D3302" t="n">
+        <v>26888.96875</v>
+      </c>
+      <c r="E3302" t="n">
+        <v>26967.916015625</v>
+      </c>
+      <c r="F3302" t="n">
+        <v>26967.916015625</v>
+      </c>
+      <c r="G3302" t="n">
+        <v>5331172801</v>
+      </c>
+    </row>
+    <row r="3303">
+      <c r="A3303" s="2" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B3303" t="n">
+        <v>26967.396484375</v>
+      </c>
+      <c r="C3303" t="n">
+        <v>28047.23828125</v>
+      </c>
+      <c r="D3303" t="n">
+        <v>26965.09375</v>
+      </c>
+      <c r="E3303" t="n">
+        <v>27983.75</v>
+      </c>
+      <c r="F3303" t="n">
+        <v>27983.75</v>
+      </c>
+      <c r="G3303" t="n">
+        <v>9503917434</v>
+      </c>
+    </row>
+    <row r="3304">
+      <c r="A3304" s="2" t="n">
+        <v>45201</v>
+      </c>
+      <c r="B3304" t="n">
+        <v>27976.798828125</v>
+      </c>
+      <c r="C3304" t="n">
+        <v>28494.458984375</v>
+      </c>
+      <c r="D3304" t="n">
+        <v>27347.787109375</v>
+      </c>
+      <c r="E3304" t="n">
+        <v>27530.78515625</v>
+      </c>
+      <c r="F3304" t="n">
+        <v>27530.78515625</v>
+      </c>
+      <c r="G3304" t="n">
+        <v>19793041322</v>
+      </c>
+    </row>
+    <row r="3305">
+      <c r="A3305" s="2" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B3305" t="n">
+        <v>27508.251953125</v>
+      </c>
+      <c r="C3305" t="n">
+        <v>27667.19140625</v>
+      </c>
+      <c r="D3305" t="n">
+        <v>27216.001953125</v>
+      </c>
+      <c r="E3305" t="n">
+        <v>27429.978515625</v>
+      </c>
+      <c r="F3305" t="n">
+        <v>27429.978515625</v>
+      </c>
+      <c r="G3305" t="n">
+        <v>11407814187</v>
+      </c>
+    </row>
+    <row r="3306">
+      <c r="A3306" s="2" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B3306" t="n">
+        <v>27429.07421875</v>
+      </c>
+      <c r="C3306" t="n">
+        <v>27826.658203125</v>
+      </c>
+      <c r="D3306" t="n">
+        <v>27248.10546875</v>
+      </c>
+      <c r="E3306" t="n">
+        <v>27799.39453125</v>
+      </c>
+      <c r="F3306" t="n">
+        <v>27799.39453125</v>
+      </c>
+      <c r="G3306" t="n">
+        <v>11143355314</v>
+      </c>
+    </row>
+    <row r="3307">
+      <c r="A3307" s="2" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B3307" t="n">
+        <v>27798.646484375</v>
+      </c>
+      <c r="C3307" t="n">
+        <v>28091.861328125</v>
+      </c>
+      <c r="D3307" t="n">
+        <v>27375.6015625</v>
+      </c>
+      <c r="E3307" t="n">
+        <v>27415.912109375</v>
+      </c>
+      <c r="F3307" t="n">
+        <v>27415.912109375</v>
+      </c>
+      <c r="G3307" t="n">
+        <v>11877253670</v>
+      </c>
+    </row>
+    <row r="3308">
+      <c r="A3308" s="2" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B3308" t="n">
+        <v>27412.123046875</v>
+      </c>
+      <c r="C3308" t="n">
+        <v>28252.537109375</v>
+      </c>
+      <c r="D3308" t="n">
+        <v>27215.552734375</v>
+      </c>
+      <c r="E3308" t="n">
+        <v>27946.59765625</v>
+      </c>
+      <c r="F3308" t="n">
+        <v>27946.59765625</v>
+      </c>
+      <c r="G3308" t="n">
+        <v>13492391599</v>
+      </c>
+    </row>
+    <row r="3309">
+      <c r="A3309" s="2" t="n">
+        <v>45206</v>
+      </c>
+      <c r="B3309" t="n">
+        <v>27946.78125</v>
+      </c>
+      <c r="C3309" t="n">
+        <v>28028.091796875</v>
+      </c>
+      <c r="D3309" t="n">
+        <v>27870.423828125</v>
+      </c>
+      <c r="E3309" t="n">
+        <v>27968.83984375</v>
+      </c>
+      <c r="F3309" t="n">
+        <v>27968.83984375</v>
+      </c>
+      <c r="G3309" t="n">
+        <v>6553044316</v>
+      </c>
+    </row>
+    <row r="3310">
+      <c r="A3310" s="2" t="n">
+        <v>45207</v>
+      </c>
+      <c r="B3310" t="n">
+        <v>27971.677734375</v>
+      </c>
+      <c r="C3310" t="n">
+        <v>28102.169921875</v>
+      </c>
+      <c r="D3310" t="n">
+        <v>27740.662109375</v>
+      </c>
+      <c r="E3310" t="n">
+        <v>27935.08984375</v>
+      </c>
+      <c r="F3310" t="n">
+        <v>27935.08984375</v>
+      </c>
+      <c r="G3310" t="n">
+        <v>7916875290</v>
+      </c>
+    </row>
+    <row r="3311">
+      <c r="A3311" s="2" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B3311" t="n">
+        <v>27934.47265625</v>
+      </c>
+      <c r="C3311" t="n">
+        <v>27989.470703125</v>
+      </c>
+      <c r="D3311" t="n">
+        <v>27302.5625</v>
+      </c>
+      <c r="E3311" t="n">
+        <v>27583.677734375</v>
+      </c>
+      <c r="F3311" t="n">
+        <v>27583.677734375</v>
+      </c>
+      <c r="G3311" t="n">
+        <v>12007668568</v>
+      </c>
+    </row>
+    <row r="3312">
+      <c r="A3312" s="2" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B3312" t="n">
+        <v>27589.201171875</v>
+      </c>
+      <c r="C3312" t="n">
+        <v>27715.84765625</v>
+      </c>
+      <c r="D3312" t="n">
+        <v>27301.654296875</v>
+      </c>
+      <c r="E3312" t="n">
+        <v>27391.01953125</v>
+      </c>
+      <c r="F3312" t="n">
+        <v>27391.01953125</v>
+      </c>
+      <c r="G3312" t="n">
+        <v>9973350678</v>
+      </c>
+    </row>
+    <row r="3313">
+      <c r="A3313" s="2" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B3313" t="n">
+        <v>27392.076171875</v>
+      </c>
+      <c r="C3313" t="n">
+        <v>27474.115234375</v>
+      </c>
+      <c r="D3313" t="n">
+        <v>26561.099609375</v>
+      </c>
+      <c r="E3313" t="n">
+        <v>26873.3203125</v>
+      </c>
+      <c r="F3313" t="n">
+        <v>26873.3203125</v>
+      </c>
+      <c r="G3313" t="n">
+        <v>13648094333</v>
+      </c>
+    </row>
+    <row r="3314">
+      <c r="A3314" s="2" t="n">
+        <v>45211</v>
+      </c>
+      <c r="B3314" t="n">
+        <v>26873.29296875</v>
+      </c>
+      <c r="C3314" t="n">
+        <v>26921.439453125</v>
+      </c>
+      <c r="D3314" t="n">
+        <v>26558.3203125</v>
+      </c>
+      <c r="E3314" t="n">
+        <v>26756.798828125</v>
+      </c>
+      <c r="F3314" t="n">
+        <v>26756.798828125</v>
+      </c>
+      <c r="G3314" t="n">
+        <v>9392909295</v>
+      </c>
+    </row>
+    <row r="3315">
+      <c r="A3315" s="2" t="n">
+        <v>45212</v>
+      </c>
+      <c r="B3315" t="n">
+        <v>26752.87890625</v>
+      </c>
+      <c r="C3315" t="n">
+        <v>27092.697265625</v>
+      </c>
+      <c r="D3315" t="n">
+        <v>26686.322265625</v>
+      </c>
+      <c r="E3315" t="n">
+        <v>26862.375</v>
+      </c>
+      <c r="F3315" t="n">
+        <v>26862.375</v>
+      </c>
+      <c r="G3315" t="n">
+        <v>15165312851</v>
+      </c>
+    </row>
+    <row r="3316">
+      <c r="A3316" s="2" t="n">
+        <v>45213</v>
+      </c>
+      <c r="B3316" t="n">
+        <v>26866.203125</v>
+      </c>
+      <c r="C3316" t="n">
+        <v>26969</v>
+      </c>
+      <c r="D3316" t="n">
+        <v>26814.5859375</v>
+      </c>
+      <c r="E3316" t="n">
+        <v>26861.70703125</v>
+      </c>
+      <c r="F3316" t="n">
+        <v>26861.70703125</v>
+      </c>
+      <c r="G3316" t="n">
+        <v>5388116782</v>
+      </c>
+    </row>
+    <row r="3317">
+      <c r="A3317" s="2" t="n">
+        <v>45214</v>
+      </c>
+      <c r="B3317" t="n">
+        <v>26858.01171875</v>
+      </c>
+      <c r="C3317" t="n">
+        <v>27289.169921875</v>
+      </c>
+      <c r="D3317" t="n">
+        <v>26817.89453125</v>
+      </c>
+      <c r="E3317" t="n">
+        <v>27159.65234375</v>
+      </c>
+      <c r="F3317" t="n">
+        <v>27159.65234375</v>
+      </c>
+      <c r="G3317" t="n">
+        <v>7098201980</v>
+      </c>
+    </row>
+    <row r="3318">
+      <c r="A3318" s="2" t="n">
+        <v>45215</v>
+      </c>
+      <c r="B3318" t="n">
+        <v>27162.62890625</v>
+      </c>
+      <c r="C3318" t="n">
+        <v>29448.138671875</v>
+      </c>
+      <c r="D3318" t="n">
+        <v>27130.47265625</v>
+      </c>
+      <c r="E3318" t="n">
+        <v>28519.466796875</v>
+      </c>
+      <c r="F3318" t="n">
+        <v>28519.466796875</v>
+      </c>
+      <c r="G3318" t="n">
+        <v>27833876539</v>
+      </c>
+    </row>
+    <row r="3319">
+      <c r="A3319" s="2" t="n">
+        <v>45216</v>
+      </c>
+      <c r="B3319" t="n">
+        <v>28522.09765625</v>
+      </c>
+      <c r="C3319" t="n">
+        <v>28618.751953125</v>
+      </c>
+      <c r="D3319" t="n">
+        <v>28110.185546875</v>
+      </c>
+      <c r="E3319" t="n">
+        <v>28415.748046875</v>
+      </c>
+      <c r="F3319" t="n">
+        <v>28415.748046875</v>
+      </c>
+      <c r="G3319" t="n">
+        <v>14872527508</v>
+      </c>
+    </row>
+    <row r="3320">
+      <c r="A3320" s="2" t="n">
+        <v>45217</v>
+      </c>
+      <c r="B3320" t="n">
+        <v>28413.53125</v>
+      </c>
+      <c r="C3320" t="n">
+        <v>28889.009765625</v>
+      </c>
+      <c r="D3320" t="n">
+        <v>28174.251953125</v>
+      </c>
+      <c r="E3320" t="n">
+        <v>28328.341796875</v>
+      </c>
+      <c r="F3320" t="n">
+        <v>28328.341796875</v>
+      </c>
+      <c r="G3320" t="n">
+        <v>12724128586</v>
+      </c>
+    </row>
+    <row r="3321">
+      <c r="A3321" s="2" t="n">
+        <v>45218</v>
+      </c>
+      <c r="B3321" t="n">
+        <v>28332.416015625</v>
+      </c>
+      <c r="C3321" t="n">
+        <v>28892.474609375</v>
+      </c>
+      <c r="D3321" t="n">
+        <v>28177.98828125</v>
+      </c>
+      <c r="E3321" t="n">
+        <v>28719.806640625</v>
+      </c>
+      <c r="F3321" t="n">
+        <v>28719.806640625</v>
+      </c>
+      <c r="G3321" t="n">
+        <v>14448058195</v>
+      </c>
+    </row>
+    <row r="3322">
+      <c r="A3322" s="2" t="n">
+        <v>45219</v>
+      </c>
+      <c r="B3322" t="n">
+        <v>28732.8125</v>
+      </c>
+      <c r="C3322" t="n">
+        <v>30104.0859375</v>
+      </c>
+      <c r="D3322" t="n">
+        <v>28601.669921875</v>
+      </c>
+      <c r="E3322" t="n">
+        <v>29682.94921875</v>
+      </c>
+      <c r="F3322" t="n">
+        <v>29682.94921875</v>
+      </c>
+      <c r="G3322" t="n">
+        <v>21536125230</v>
+      </c>
+    </row>
+    <row r="3323">
+      <c r="A3323" s="2" t="n">
+        <v>45220</v>
+      </c>
+      <c r="B3323" t="n">
+        <v>29683.380859375</v>
+      </c>
+      <c r="C3323" t="n">
+        <v>30287.482421875</v>
+      </c>
+      <c r="D3323" t="n">
+        <v>29481.751953125</v>
+      </c>
+      <c r="E3323" t="n">
+        <v>29918.412109375</v>
+      </c>
+      <c r="F3323" t="n">
+        <v>29918.412109375</v>
+      </c>
+      <c r="G3323" t="n">
+        <v>11541146996</v>
+      </c>
+    </row>
+    <row r="3324">
+      <c r="A3324" s="2" t="n">
+        <v>45221</v>
+      </c>
+      <c r="B3324" t="n">
+        <v>29918.654296875</v>
+      </c>
+      <c r="C3324" t="n">
+        <v>30199.43359375</v>
+      </c>
+      <c r="D3324" t="n">
+        <v>29720.3125</v>
+      </c>
+      <c r="E3324" t="n">
+        <v>29993.896484375</v>
+      </c>
+      <c r="F3324" t="n">
+        <v>29993.896484375</v>
+      </c>
+      <c r="G3324" t="n">
+        <v>10446520040</v>
+      </c>
+    </row>
+    <row r="3325">
+      <c r="A3325" s="2" t="n">
+        <v>45222</v>
+      </c>
+      <c r="B3325" t="n">
+        <v>30140.685546875</v>
+      </c>
+      <c r="C3325" t="n">
+        <v>34370.4375</v>
+      </c>
+      <c r="D3325" t="n">
+        <v>30097.828125</v>
+      </c>
+      <c r="E3325" t="n">
+        <v>33086.234375</v>
+      </c>
+      <c r="F3325" t="n">
+        <v>33086.234375</v>
+      </c>
+      <c r="G3325" t="n">
+        <v>38363572311</v>
+      </c>
+    </row>
+    <row r="3326">
+      <c r="A3326" s="2" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B3326" t="n">
+        <v>33077.3046875</v>
+      </c>
+      <c r="C3326" t="n">
+        <v>35150.43359375</v>
+      </c>
+      <c r="D3326" t="n">
+        <v>32880.76171875</v>
+      </c>
+      <c r="E3326" t="n">
+        <v>33901.52734375</v>
+      </c>
+      <c r="F3326" t="n">
+        <v>33901.52734375</v>
+      </c>
+      <c r="G3326" t="n">
+        <v>44934999645</v>
+      </c>
+    </row>
+    <row r="3327">
+      <c r="A3327" s="2" t="n">
+        <v>45224</v>
+      </c>
+      <c r="B3327" t="n">
+        <v>33916.04296875</v>
+      </c>
+      <c r="C3327" t="n">
+        <v>35133.7578125</v>
+      </c>
+      <c r="D3327" t="n">
+        <v>33709.109375</v>
+      </c>
+      <c r="E3327" t="n">
+        <v>34502.8203125</v>
+      </c>
+      <c r="F3327" t="n">
+        <v>34502.8203125</v>
+      </c>
+      <c r="G3327" t="n">
+        <v>25254318008</v>
+      </c>
+    </row>
+    <row r="3328">
+      <c r="A3328" s="2" t="n">
+        <v>45225</v>
+      </c>
+      <c r="B3328" t="n">
+        <v>34504.2890625</v>
+      </c>
+      <c r="C3328" t="n">
+        <v>34832.91015625</v>
+      </c>
+      <c r="D3328" t="n">
+        <v>33762.32421875</v>
+      </c>
+      <c r="E3328" t="n">
+        <v>34156.6484375</v>
+      </c>
+      <c r="F3328" t="n">
+        <v>34156.6484375</v>
+      </c>
+      <c r="G3328" t="n">
+        <v>19427195376</v>
+      </c>
+    </row>
+    <row r="3329">
+      <c r="A3329" s="2" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B3329" t="n">
+        <v>34156.5</v>
+      </c>
+      <c r="C3329" t="n">
+        <v>34238.2109375</v>
+      </c>
+      <c r="D3329" t="n">
+        <v>33416.88671875</v>
+      </c>
+      <c r="E3329" t="n">
+        <v>33909.80078125</v>
+      </c>
+      <c r="F3329" t="n">
+        <v>33909.80078125</v>
+      </c>
+      <c r="G3329" t="n">
+        <v>16418032871</v>
+      </c>
+    </row>
+    <row r="3330">
+      <c r="A3330" s="2" t="n">
+        <v>45227</v>
+      </c>
+      <c r="B3330" t="n">
+        <v>33907.72265625</v>
+      </c>
+      <c r="C3330" t="n">
+        <v>34399.390625</v>
+      </c>
+      <c r="D3330" t="n">
+        <v>33874.8046875</v>
+      </c>
+      <c r="E3330" t="n">
+        <v>34089.57421875</v>
+      </c>
+      <c r="F3330" t="n">
+        <v>34089.57421875</v>
+      </c>
+      <c r="G3330" t="n">
+        <v>10160330825</v>
+      </c>
+    </row>
+    <row r="3331">
+      <c r="A3331" s="2" t="n">
+        <v>45228</v>
+      </c>
+      <c r="B3331" t="n">
+        <v>34089.37109375</v>
+      </c>
+      <c r="C3331" t="n">
+        <v>34743.26171875</v>
+      </c>
+      <c r="D3331" t="n">
+        <v>33947.56640625</v>
+      </c>
+      <c r="E3331" t="n">
+        <v>34538.48046875</v>
+      </c>
+      <c r="F3331" t="n">
+        <v>34538.48046875</v>
+      </c>
+      <c r="G3331" t="n">
+        <v>11160323986</v>
+      </c>
+    </row>
+    <row r="3332">
+      <c r="A3332" s="2" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B3332" t="n">
+        <v>34531.7421875</v>
+      </c>
+      <c r="C3332" t="n">
+        <v>34843.93359375</v>
+      </c>
+      <c r="D3332" t="n">
+        <v>34110.97265625</v>
+      </c>
+      <c r="E3332" t="n">
+        <v>34502.36328125</v>
+      </c>
+      <c r="F3332" t="n">
+        <v>34502.36328125</v>
+      </c>
+      <c r="G3332" t="n">
+        <v>17184860315</v>
+      </c>
+    </row>
+    <row r="3333">
+      <c r="A3333" s="2" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B3333" t="n">
+        <v>34500.078125</v>
+      </c>
+      <c r="C3333" t="n">
+        <v>34719.25390625</v>
+      </c>
+      <c r="D3333" t="n">
+        <v>34083.30859375</v>
+      </c>
+      <c r="E3333" t="n">
+        <v>34667.78125</v>
+      </c>
+      <c r="F3333" t="n">
+        <v>34667.78125</v>
+      </c>
+      <c r="G3333" t="n">
+        <v>15758270810</v>
+      </c>
+    </row>
+    <row r="3334">
+      <c r="A3334" s="2" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B3334" t="n">
+        <v>34657.2734375</v>
+      </c>
+      <c r="C3334" t="n">
+        <v>35527.9296875</v>
+      </c>
+      <c r="D3334" t="n">
+        <v>34170.69140625</v>
+      </c>
+      <c r="E3334" t="n">
+        <v>35437.25390625</v>
+      </c>
+      <c r="F3334" t="n">
+        <v>35437.25390625</v>
+      </c>
+      <c r="G3334" t="n">
+        <v>22446272005</v>
+      </c>
+    </row>
+    <row r="3335">
+      <c r="A3335" s="2" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B3335" t="n">
+        <v>35441.578125</v>
+      </c>
+      <c r="C3335" t="n">
+        <v>35919.84375</v>
+      </c>
+      <c r="D3335" t="n">
+        <v>34401.57421875</v>
+      </c>
+      <c r="E3335" t="n">
+        <v>34938.2421875</v>
+      </c>
+      <c r="F3335" t="n">
+        <v>34938.2421875</v>
+      </c>
+      <c r="G3335" t="n">
+        <v>20998158544</v>
+      </c>
+    </row>
+    <row r="3336">
+      <c r="A3336" s="2" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B3336" t="n">
+        <v>34942.47265625</v>
+      </c>
+      <c r="C3336" t="n">
+        <v>34942.47265625</v>
+      </c>
+      <c r="D3336" t="n">
+        <v>34133.44140625</v>
+      </c>
+      <c r="E3336" t="n">
+        <v>34732.32421875</v>
+      </c>
+      <c r="F3336" t="n">
+        <v>34732.32421875</v>
+      </c>
+      <c r="G3336" t="n">
+        <v>17158456701</v>
+      </c>
+    </row>
+    <row r="3337">
+      <c r="A3337" s="2" t="n">
+        <v>45234</v>
+      </c>
+      <c r="B3337" t="n">
+        <v>34736.32421875</v>
+      </c>
+      <c r="C3337" t="n">
+        <v>35256.03125</v>
+      </c>
+      <c r="D3337" t="n">
+        <v>34616.69140625</v>
+      </c>
+      <c r="E3337" t="n">
+        <v>35082.1953125</v>
+      </c>
+      <c r="F3337" t="n">
+        <v>35082.1953125</v>
+      </c>
+      <c r="G3337" t="n">
+        <v>9561294264</v>
+      </c>
+    </row>
+    <row r="3338">
+      <c r="A3338" s="2" t="n">
+        <v>45235</v>
+      </c>
+      <c r="B3338" t="n">
+        <v>35090.01171875</v>
+      </c>
+      <c r="C3338" t="n">
+        <v>35340.33984375</v>
+      </c>
+      <c r="D3338" t="n">
+        <v>34594.2421875</v>
+      </c>
+      <c r="E3338" t="n">
+        <v>35049.35546875</v>
+      </c>
+      <c r="F3338" t="n">
+        <v>35049.35546875</v>
+      </c>
+      <c r="G3338" t="n">
+        <v>12412743996</v>
+      </c>
+    </row>
+    <row r="3339">
+      <c r="A3339" s="2" t="n">
+        <v>45236</v>
+      </c>
+      <c r="B3339" t="n">
+        <v>35044.7890625</v>
+      </c>
+      <c r="C3339" t="n">
+        <v>35286.02734375</v>
+      </c>
+      <c r="D3339" t="n">
+        <v>34765.36328125</v>
+      </c>
+      <c r="E3339" t="n">
+        <v>35037.37109375</v>
+      </c>
+      <c r="F3339" t="n">
+        <v>35037.37109375</v>
+      </c>
+      <c r="G3339" t="n">
+        <v>12693436420</v>
+      </c>
+    </row>
+    <row r="3340">
+      <c r="A3340" s="2" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B3340" t="n">
+        <v>35047.79296875</v>
+      </c>
+      <c r="C3340" t="n">
+        <v>35892.41796875</v>
+      </c>
+      <c r="D3340" t="n">
+        <v>34545.81640625</v>
+      </c>
+      <c r="E3340" t="n">
+        <v>35443.5625</v>
+      </c>
+      <c r="F3340" t="n">
+        <v>35443.5625</v>
+      </c>
+      <c r="G3340" t="n">
+        <v>18834737789</v>
+      </c>
+    </row>
+    <row r="3341">
+      <c r="A3341" s="2" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B3341" t="n">
+        <v>35419.4765625</v>
+      </c>
+      <c r="C3341" t="n">
+        <v>35994.41796875</v>
+      </c>
+      <c r="D3341" t="n">
+        <v>35147.80078125</v>
+      </c>
+      <c r="E3341" t="n">
+        <v>35655.27734375</v>
+      </c>
+      <c r="F3341" t="n">
+        <v>35655.27734375</v>
+      </c>
+      <c r="G3341" t="n">
+        <v>17295394918</v>
+      </c>
+    </row>
+    <row r="3342">
+      <c r="A3342" s="2" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B3342" t="n">
+        <v>35633.6328125</v>
+      </c>
+      <c r="C3342" t="n">
+        <v>37926.2578125</v>
+      </c>
+      <c r="D3342" t="n">
+        <v>35592.1015625</v>
+      </c>
+      <c r="E3342" t="n">
+        <v>36693.125</v>
+      </c>
+      <c r="F3342" t="n">
+        <v>36693.125</v>
+      </c>
+      <c r="G3342" t="n">
+        <v>37762672382</v>
+      </c>
+    </row>
+    <row r="3343">
+      <c r="A3343" s="2" t="n">
+        <v>45240</v>
+      </c>
+      <c r="B3343" t="n">
+        <v>36702.25</v>
+      </c>
+      <c r="C3343" t="n">
+        <v>37493.80078125</v>
+      </c>
+      <c r="D3343" t="n">
+        <v>36362.75390625</v>
+      </c>
+      <c r="E3343" t="n">
+        <v>37313.96875</v>
+      </c>
+      <c r="F3343" t="n">
+        <v>37313.96875</v>
+      </c>
+      <c r="G3343" t="n">
+        <v>22711265155</v>
+      </c>
+    </row>
+    <row r="3344">
+      <c r="A3344" s="2" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B3344" t="n">
+        <v>37310.0703125</v>
+      </c>
+      <c r="C3344" t="n">
+        <v>37407.09375</v>
+      </c>
+      <c r="D3344" t="n">
+        <v>36773.66796875</v>
+      </c>
+      <c r="E3344" t="n">
+        <v>37138.05078125</v>
+      </c>
+      <c r="F3344" t="n">
+        <v>37138.05078125</v>
+      </c>
+      <c r="G3344" t="n">
+        <v>13924272142</v>
+      </c>
+    </row>
+    <row r="3345">
+      <c r="A3345" s="2" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B3345" t="n">
+        <v>37133.9921875</v>
+      </c>
+      <c r="C3345" t="n">
+        <v>37227.69140625</v>
+      </c>
+      <c r="D3345" t="n">
+        <v>36779.1171875</v>
+      </c>
+      <c r="E3345" t="n">
+        <v>37054.51953125</v>
+      </c>
+      <c r="F3345" t="n">
+        <v>37054.51953125</v>
+      </c>
+      <c r="G3345" t="n">
+        <v>11545715999</v>
+      </c>
+    </row>
+    <row r="3346">
+      <c r="A3346" s="2" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B3346" t="n">
+        <v>37070.3046875</v>
+      </c>
+      <c r="C3346" t="n">
+        <v>37405.1171875</v>
+      </c>
+      <c r="D3346" t="n">
+        <v>36399.60546875</v>
+      </c>
+      <c r="E3346" t="n">
+        <v>36502.35546875</v>
+      </c>
+      <c r="F3346" t="n">
+        <v>36502.35546875</v>
+      </c>
+      <c r="G3346" t="n">
+        <v>19057712790</v>
+      </c>
+    </row>
+    <row r="3347">
+      <c r="A3347" s="2" t="n">
+        <v>45244</v>
+      </c>
+      <c r="B3347" t="n">
+        <v>36491.7890625</v>
+      </c>
+      <c r="C3347" t="n">
+        <v>36753.3515625</v>
+      </c>
+      <c r="D3347" t="n">
+        <v>34948.5</v>
+      </c>
+      <c r="E3347" t="n">
+        <v>35537.640625</v>
+      </c>
+      <c r="F3347" t="n">
+        <v>35537.640625</v>
+      </c>
+      <c r="G3347" t="n">
+        <v>23857403554</v>
+      </c>
+    </row>
+    <row r="3348">
+      <c r="A3348" s="2" t="n">
+        <v>45245</v>
+      </c>
+      <c r="B3348" t="n">
+        <v>35548.11328125</v>
+      </c>
+      <c r="C3348" t="n">
+        <v>37964.89453125</v>
+      </c>
+      <c r="D3348" t="n">
+        <v>35383.78125</v>
+      </c>
+      <c r="E3348" t="n">
+        <v>37880.58203125</v>
+      </c>
+      <c r="F3348" t="n">
+        <v>37880.58203125</v>
+      </c>
+      <c r="G3348" t="n">
+        <v>27365821679</v>
+      </c>
+    </row>
+    <row r="3349">
+      <c r="A3349" s="2" t="n">
+        <v>45246</v>
+      </c>
+      <c r="B3349" t="n">
+        <v>37879.98046875</v>
+      </c>
+      <c r="C3349" t="n">
+        <v>37934.625</v>
+      </c>
+      <c r="D3349" t="n">
+        <v>35545.47265625</v>
+      </c>
+      <c r="E3349" t="n">
+        <v>36154.76953125</v>
+      </c>
+      <c r="F3349" t="n">
+        <v>36154.76953125</v>
+      </c>
+      <c r="G3349" t="n">
+        <v>26007385366</v>
+      </c>
+    </row>
+    <row r="3350">
+      <c r="A3350" s="2" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B3350" t="n">
+        <v>36164.82421875</v>
+      </c>
+      <c r="C3350" t="n">
+        <v>36704.484375</v>
+      </c>
+      <c r="D3350" t="n">
+        <v>35901.234375</v>
+      </c>
+      <c r="E3350" t="n">
+        <v>36596.68359375</v>
+      </c>
+      <c r="F3350" t="n">
+        <v>36596.68359375</v>
+      </c>
+      <c r="G3350" t="n">
+        <v>22445028430</v>
+      </c>
+    </row>
+    <row r="3351">
+      <c r="A3351" s="2" t="n">
+        <v>45248</v>
+      </c>
+      <c r="B3351" t="n">
+        <v>36625.37109375</v>
+      </c>
+      <c r="C3351" t="n">
+        <v>36839.28125</v>
+      </c>
+      <c r="D3351" t="n">
+        <v>36233.3125</v>
+      </c>
+      <c r="E3351" t="n">
+        <v>36585.703125</v>
+      </c>
+      <c r="F3351" t="n">
+        <v>36585.703125</v>
+      </c>
+      <c r="G3351" t="n">
+        <v>11886022717</v>
+      </c>
+    </row>
+    <row r="3352">
+      <c r="A3352" s="2" t="n">
+        <v>45249</v>
+      </c>
+      <c r="B3352" t="n">
+        <v>36585.765625</v>
+      </c>
+      <c r="C3352" t="n">
+        <v>37509.35546875</v>
+      </c>
+      <c r="D3352" t="n">
+        <v>36414.59765625</v>
+      </c>
+      <c r="E3352" t="n">
+        <v>37386.546875</v>
+      </c>
+      <c r="F3352" t="n">
+        <v>37386.546875</v>
+      </c>
+      <c r="G3352" t="n">
+        <v>12915986553</v>
+      </c>
+    </row>
+    <row r="3353">
+      <c r="A3353" s="2" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B3353" t="n">
+        <v>37374.07421875</v>
+      </c>
+      <c r="C3353" t="n">
+        <v>37756.8203125</v>
+      </c>
+      <c r="D3353" t="n">
+        <v>36882.53125</v>
+      </c>
+      <c r="E3353" t="n">
+        <v>37476.95703125</v>
+      </c>
+      <c r="F3353" t="n">
+        <v>37476.95703125</v>
+      </c>
+      <c r="G3353" t="n">
+        <v>20888209068</v>
+      </c>
+    </row>
+    <row r="3354">
+      <c r="A3354" s="2" t="n">
+        <v>45251</v>
+      </c>
+      <c r="B3354" t="n">
+        <v>37469.16015625</v>
+      </c>
+      <c r="C3354" t="n">
+        <v>37631.140625</v>
+      </c>
+      <c r="D3354" t="n">
+        <v>35813.8125</v>
+      </c>
+      <c r="E3354" t="n">
+        <v>35813.8125</v>
+      </c>
+      <c r="F3354" t="n">
+        <v>35813.8125</v>
+      </c>
+      <c r="G3354" t="n">
+        <v>25172163756</v>
+      </c>
+    </row>
+    <row r="3355">
+      <c r="A3355" s="2" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B3355" t="n">
+        <v>35756.5546875</v>
+      </c>
+      <c r="C3355" t="n">
+        <v>37856.98046875</v>
+      </c>
+      <c r="D3355" t="n">
+        <v>35670.97265625</v>
+      </c>
+      <c r="E3355" t="n">
+        <v>37432.33984375</v>
+      </c>
+      <c r="F3355" t="n">
+        <v>37432.33984375</v>
+      </c>
+      <c r="G3355" t="n">
+        <v>24397247860</v>
+      </c>
+    </row>
+    <row r="3356">
+      <c r="A3356" s="2" t="n">
+        <v>45253</v>
+      </c>
+      <c r="B3356" t="n">
+        <v>37420.43359375</v>
+      </c>
+      <c r="C3356" t="n">
+        <v>37643.91796875</v>
+      </c>
+      <c r="D3356" t="n">
+        <v>36923.86328125</v>
+      </c>
+      <c r="E3356" t="n">
+        <v>37289.62109375</v>
+      </c>
+      <c r="F3356" t="n">
+        <v>37289.62109375</v>
+      </c>
+      <c r="G3356" t="n">
+        <v>14214948217</v>
+      </c>
+    </row>
+    <row r="3357">
+      <c r="A3357" s="2" t="n">
+        <v>45254</v>
+      </c>
+      <c r="B3357" t="n">
+        <v>37296.31640625</v>
+      </c>
+      <c r="C3357" t="n">
+        <v>38415.33984375</v>
+      </c>
+      <c r="D3357" t="n">
+        <v>37261.60546875</v>
+      </c>
+      <c r="E3357" t="n">
+        <v>37720.28125</v>
+      </c>
+      <c r="F3357" t="n">
+        <v>37720.28125</v>
+      </c>
+      <c r="G3357" t="n">
+        <v>22922957823</v>
+      </c>
+    </row>
+    <row r="3358">
+      <c r="A3358" s="2" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B3358" t="n">
+        <v>37721.4140625</v>
+      </c>
+      <c r="C3358" t="n">
+        <v>37892.4296875</v>
+      </c>
+      <c r="D3358" t="n">
+        <v>37617.41796875</v>
+      </c>
+      <c r="E3358" t="n">
+        <v>37796.79296875</v>
+      </c>
+      <c r="F3358" t="n">
+        <v>37796.79296875</v>
+      </c>
+      <c r="G3358" t="n">
+        <v>9099571165</v>
+      </c>
+    </row>
+    <row r="3359">
+      <c r="A3359" s="2" t="n">
+        <v>45256</v>
+      </c>
+      <c r="B3359" t="n">
+        <v>37796.828125</v>
+      </c>
+      <c r="C3359" t="n">
+        <v>37820.30078125</v>
+      </c>
+      <c r="D3359" t="n">
+        <v>37162.75</v>
+      </c>
+      <c r="E3359" t="n">
+        <v>37479.12109375</v>
+      </c>
+      <c r="F3359" t="n">
+        <v>37479.12109375</v>
+      </c>
+      <c r="G3359" t="n">
+        <v>13744796068</v>
+      </c>
+    </row>
+    <row r="3360">
+      <c r="A3360" s="2" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B3360" t="n">
+        <v>37454.19140625</v>
+      </c>
+      <c r="C3360" t="n">
+        <v>37559.35546875</v>
+      </c>
+      <c r="D3360" t="n">
+        <v>36750.12890625</v>
+      </c>
+      <c r="E3360" t="n">
+        <v>37254.16796875</v>
+      </c>
+      <c r="F3360" t="n">
+        <v>37254.16796875</v>
+      </c>
+      <c r="G3360" t="n">
+        <v>19002925720</v>
+      </c>
+    </row>
+    <row r="3361">
+      <c r="A3361" s="2" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B3361" t="n">
+        <v>37247.9921875</v>
+      </c>
+      <c r="C3361" t="n">
+        <v>38368.48046875</v>
+      </c>
+      <c r="D3361" t="n">
+        <v>36891.08984375</v>
+      </c>
+      <c r="E3361" t="n">
+        <v>37831.0859375</v>
+      </c>
+      <c r="F3361" t="n">
+        <v>37831.0859375</v>
+      </c>
+      <c r="G3361" t="n">
+        <v>21696137014</v>
+      </c>
+    </row>
+    <row r="3362">
+      <c r="A3362" s="2" t="n">
+        <v>45259</v>
+      </c>
+      <c r="B3362" t="n">
+        <v>37826.10546875</v>
+      </c>
+      <c r="C3362" t="n">
+        <v>38366.11328125</v>
+      </c>
+      <c r="D3362" t="n">
+        <v>37612.6328125</v>
+      </c>
+      <c r="E3362" t="n">
+        <v>37858.4921875</v>
+      </c>
+      <c r="F3362" t="n">
+        <v>37858.4921875</v>
+      </c>
+      <c r="G3362" t="n">
+        <v>20728546658</v>
+      </c>
+    </row>
+    <row r="3363">
+      <c r="A3363" s="2" t="n">
+        <v>45260</v>
+      </c>
+      <c r="B3363" t="n">
+        <v>37861.1171875</v>
+      </c>
+      <c r="C3363" t="n">
+        <v>38141.75390625</v>
+      </c>
+      <c r="D3363" t="n">
+        <v>37531.140625</v>
+      </c>
+      <c r="E3363" t="n">
+        <v>37712.74609375</v>
+      </c>
+      <c r="F3363" t="n">
+        <v>37712.74609375</v>
+      </c>
+      <c r="G3363" t="n">
+        <v>18115982627</v>
+      </c>
+    </row>
+    <row r="3364">
+      <c r="A3364" s="2" t="n">
+        <v>45261</v>
+      </c>
+      <c r="B3364" t="n">
+        <v>37718.0078125</v>
+      </c>
+      <c r="C3364" t="n">
+        <v>38954.109375</v>
+      </c>
+      <c r="D3364" t="n">
+        <v>37629.359375</v>
+      </c>
+      <c r="E3364" t="n">
+        <v>38688.75</v>
+      </c>
+      <c r="F3364" t="n">
+        <v>38688.75</v>
+      </c>
+      <c r="G3364" t="n">
+        <v>23512784002</v>
+      </c>
+    </row>
+    <row r="3365">
+      <c r="A3365" s="2" t="n">
+        <v>45262</v>
+      </c>
+      <c r="B3365" t="n">
+        <v>38689.27734375</v>
+      </c>
+      <c r="C3365" t="n">
+        <v>39678.9375</v>
+      </c>
+      <c r="D3365" t="n">
+        <v>38652.59375</v>
+      </c>
+      <c r="E3365" t="n">
+        <v>39476.33203125</v>
+      </c>
+      <c r="F3365" t="n">
+        <v>39476.33203125</v>
+      </c>
+      <c r="G3365" t="n">
+        <v>15534035612</v>
+      </c>
+    </row>
+    <row r="3366">
+      <c r="A3366" s="2" t="n">
+        <v>45263</v>
+      </c>
+      <c r="B3366" t="n">
+        <v>39472.20703125</v>
+      </c>
+      <c r="C3366" t="n">
+        <v>40135.60546875</v>
+      </c>
+      <c r="D3366" t="n">
+        <v>39298.1640625</v>
+      </c>
+      <c r="E3366" t="n">
+        <v>39978.390625</v>
+      </c>
+      <c r="F3366" t="n">
+        <v>39978.390625</v>
+      </c>
+      <c r="G3366" t="n">
+        <v>15769696322</v>
+      </c>
+    </row>
+    <row r="3367">
+      <c r="A3367" s="2" t="n">
+        <v>45264</v>
+      </c>
+      <c r="B3367" t="n">
+        <v>39978.62890625</v>
+      </c>
+      <c r="C3367" t="n">
+        <v>42371.75</v>
+      </c>
+      <c r="D3367" t="n">
+        <v>39978.62890625</v>
+      </c>
+      <c r="E3367" t="n">
+        <v>41980.09765625</v>
+      </c>
+      <c r="F3367" t="n">
+        <v>41980.09765625</v>
+      </c>
+      <c r="G3367" t="n">
+        <v>39856129827</v>
+      </c>
+    </row>
+    <row r="3368">
+      <c r="A3368" s="2" t="n">
+        <v>45265</v>
+      </c>
+      <c r="B3368" t="n">
+        <v>41986.265625</v>
+      </c>
+      <c r="C3368" t="n">
+        <v>44408.6640625</v>
+      </c>
+      <c r="D3368" t="n">
+        <v>41421.1484375</v>
+      </c>
+      <c r="E3368" t="n">
+        <v>44080.6484375</v>
+      </c>
+      <c r="F3368" t="n">
+        <v>44080.6484375</v>
+      </c>
+      <c r="G3368" t="n">
+        <v>36312154535</v>
+      </c>
+    </row>
+    <row r="3369">
+      <c r="A3369" s="2" t="n">
+        <v>45266</v>
+      </c>
+      <c r="B3369" t="n">
+        <v>44080.0234375</v>
+      </c>
+      <c r="C3369" t="n">
+        <v>44265.76953125</v>
+      </c>
+      <c r="D3369" t="n">
+        <v>43478.08203125</v>
+      </c>
+      <c r="E3369" t="n">
+        <v>43746.4453125</v>
+      </c>
+      <c r="F3369" t="n">
+        <v>43746.4453125</v>
+      </c>
+      <c r="G3369" t="n">
+        <v>29909761586</v>
+      </c>
+    </row>
+    <row r="3370">
+      <c r="A3370" s="2" t="n">
+        <v>45267</v>
+      </c>
+      <c r="B3370" t="n">
+        <v>43769.1328125</v>
+      </c>
+      <c r="C3370" t="n">
+        <v>44042.58984375</v>
+      </c>
+      <c r="D3370" t="n">
+        <v>42880.6484375</v>
+      </c>
+      <c r="E3370" t="n">
+        <v>43292.6640625</v>
+      </c>
+      <c r="F3370" t="n">
+        <v>43292.6640625</v>
+      </c>
+      <c r="G3370" t="n">
+        <v>27635760671</v>
+      </c>
+    </row>
+    <row r="3371">
+      <c r="A3371" s="2" t="n">
+        <v>45268</v>
+      </c>
+      <c r="B3371" t="n">
+        <v>43293.13671875</v>
+      </c>
+      <c r="C3371" t="n">
+        <v>44705.515625</v>
+      </c>
+      <c r="D3371" t="n">
+        <v>43125.296875</v>
+      </c>
+      <c r="E3371" t="n">
+        <v>44166.6015625</v>
+      </c>
+      <c r="F3371" t="n">
+        <v>44166.6015625</v>
+      </c>
+      <c r="G3371" t="n">
+        <v>24421116687</v>
+      </c>
+    </row>
+    <row r="3372">
+      <c r="A3372" s="2" t="n">
+        <v>45269</v>
+      </c>
+      <c r="B3372" t="n">
+        <v>44180.01953125</v>
+      </c>
+      <c r="C3372" t="n">
+        <v>44361.2578125</v>
+      </c>
+      <c r="D3372" t="n">
+        <v>43627.59765625</v>
+      </c>
+      <c r="E3372" t="n">
+        <v>43725.984375</v>
+      </c>
+      <c r="F3372" t="n">
+        <v>43725.984375</v>
+      </c>
+      <c r="G3372" t="n">
+        <v>17368210171</v>
+      </c>
+    </row>
+    <row r="3373">
+      <c r="A3373" s="2" t="n">
+        <v>45270</v>
+      </c>
+      <c r="B3373" t="n">
+        <v>43728.3828125</v>
+      </c>
+      <c r="C3373" t="n">
+        <v>44034.625</v>
+      </c>
+      <c r="D3373" t="n">
+        <v>43593.28515625</v>
+      </c>
+      <c r="E3373" t="n">
+        <v>43779.69921875</v>
+      </c>
+      <c r="F3373" t="n">
+        <v>43779.69921875</v>
+      </c>
+      <c r="G3373" t="n">
+        <v>13000481418</v>
+      </c>
+    </row>
+    <row r="3374">
+      <c r="A3374" s="2" t="n">
+        <v>45271</v>
+      </c>
+      <c r="B3374" t="n">
+        <v>43792.01953125</v>
+      </c>
+      <c r="C3374" t="n">
+        <v>43808.375</v>
+      </c>
+      <c r="D3374" t="n">
+        <v>40234.578125</v>
+      </c>
+      <c r="E3374" t="n">
+        <v>41243.83203125</v>
+      </c>
+      <c r="F3374" t="n">
+        <v>41243.83203125</v>
+      </c>
+      <c r="G3374" t="n">
+        <v>40632672038</v>
+      </c>
+    </row>
+    <row r="3375">
+      <c r="A3375" s="2" t="n">
+        <v>45272</v>
+      </c>
+      <c r="B3375" t="n">
+        <v>41238.734375</v>
+      </c>
+      <c r="C3375" t="n">
+        <v>42048.3046875</v>
+      </c>
+      <c r="D3375" t="n">
+        <v>40667.5625</v>
+      </c>
+      <c r="E3375" t="n">
+        <v>41450.22265625</v>
+      </c>
+      <c r="F3375" t="n">
+        <v>41450.22265625</v>
+      </c>
+      <c r="G3375" t="n">
+        <v>24779520132</v>
+      </c>
+    </row>
+    <row r="3376">
+      <c r="A3376" s="2" t="n">
+        <v>45273</v>
+      </c>
+      <c r="B3376" t="n">
+        <v>41468.46484375</v>
+      </c>
+      <c r="C3376" t="n">
+        <v>43429.78125</v>
+      </c>
+      <c r="D3376" t="n">
+        <v>40676.8671875</v>
+      </c>
+      <c r="E3376" t="n">
+        <v>42890.7421875</v>
+      </c>
+      <c r="F3376" t="n">
+        <v>42890.7421875</v>
+      </c>
+      <c r="G3376" t="n">
+        <v>26797884674</v>
+      </c>
+    </row>
+    <row r="3377">
+      <c r="A3377" s="2" t="n">
+        <v>45274</v>
+      </c>
+      <c r="B3377" t="n">
+        <v>42884.26171875</v>
+      </c>
+      <c r="C3377" t="n">
+        <v>43390.859375</v>
+      </c>
+      <c r="D3377" t="n">
+        <v>41767.08984375</v>
+      </c>
+      <c r="E3377" t="n">
+        <v>43023.97265625</v>
+      </c>
+      <c r="F3377" t="n">
+        <v>43023.97265625</v>
+      </c>
+      <c r="G3377" t="n">
+        <v>25578530178</v>
+      </c>
+    </row>
+    <row r="3378">
+      <c r="A3378" s="2" t="n">
+        <v>45275</v>
+      </c>
+      <c r="B3378" t="n">
+        <v>43028.25</v>
+      </c>
+      <c r="C3378" t="n">
+        <v>43087.82421875</v>
+      </c>
+      <c r="D3378" t="n">
+        <v>41692.96875</v>
+      </c>
+      <c r="E3378" t="n">
+        <v>41929.7578125</v>
+      </c>
+      <c r="F3378" t="n">
+        <v>41929.7578125</v>
+      </c>
+      <c r="G3378" t="n">
+        <v>19639442462</v>
+      </c>
+    </row>
+    <row r="3379">
+      <c r="A3379" s="2" t="n">
+        <v>45276</v>
+      </c>
+      <c r="B3379" t="n">
+        <v>41937.7421875</v>
+      </c>
+      <c r="C3379" t="n">
+        <v>42664.9453125</v>
+      </c>
+      <c r="D3379" t="n">
+        <v>41723.11328125</v>
+      </c>
+      <c r="E3379" t="n">
+        <v>42240.1171875</v>
+      </c>
+      <c r="F3379" t="n">
+        <v>42240.1171875</v>
+      </c>
+      <c r="G3379" t="n">
+        <v>14386729590</v>
+      </c>
+    </row>
+    <row r="3380">
+      <c r="A3380" s="2" t="n">
+        <v>45277</v>
+      </c>
+      <c r="B3380" t="n">
+        <v>42236.109375</v>
+      </c>
+      <c r="C3380" t="n">
+        <v>42359.49609375</v>
+      </c>
+      <c r="D3380" t="n">
+        <v>41274.54296875</v>
+      </c>
+      <c r="E3380" t="n">
+        <v>41364.6640625</v>
+      </c>
+      <c r="F3380" t="n">
+        <v>41364.6640625</v>
+      </c>
+      <c r="G3380" t="n">
+        <v>16678702876</v>
+      </c>
+    </row>
+    <row r="3381">
+      <c r="A3381" s="2" t="n">
+        <v>45278</v>
+      </c>
+      <c r="B3381" t="n">
+        <v>41348.203125</v>
+      </c>
+      <c r="C3381" t="n">
+        <v>42720.296875</v>
+      </c>
+      <c r="D3381" t="n">
+        <v>40530.2578125</v>
+      </c>
+      <c r="E3381" t="n">
+        <v>42623.5390625</v>
+      </c>
+      <c r="F3381" t="n">
+        <v>42623.5390625</v>
+      </c>
+      <c r="G3381" t="n">
+        <v>25224642008</v>
+      </c>
+    </row>
+    <row r="3382">
+      <c r="A3382" s="2" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B3382" t="n">
+        <v>42641.51171875</v>
+      </c>
+      <c r="C3382" t="n">
+        <v>43354.296875</v>
+      </c>
+      <c r="D3382" t="n">
+        <v>41826.3359375</v>
+      </c>
+      <c r="E3382" t="n">
+        <v>42270.52734375</v>
+      </c>
+      <c r="F3382" t="n">
+        <v>42270.52734375</v>
+      </c>
+      <c r="G3382" t="n">
+        <v>23171001281</v>
+      </c>
+    </row>
+    <row r="3383">
+      <c r="A3383" s="2" t="n">
+        <v>45280</v>
+      </c>
+      <c r="B3383" t="n">
+        <v>42261.30078125</v>
+      </c>
+      <c r="C3383" t="n">
+        <v>44275.5859375</v>
+      </c>
+      <c r="D3383" t="n">
+        <v>42223.81640625</v>
+      </c>
+      <c r="E3383" t="n">
+        <v>43652.25</v>
+      </c>
+      <c r="F3383" t="n">
+        <v>43652.25</v>
+      </c>
+      <c r="G3383" t="n">
+        <v>27868908174</v>
+      </c>
+    </row>
+    <row r="3384">
+      <c r="A3384" s="2" t="n">
+        <v>45281</v>
+      </c>
+      <c r="B3384" t="n">
+        <v>43648.125</v>
+      </c>
+      <c r="C3384" t="n">
+        <v>44240.66796875</v>
+      </c>
+      <c r="D3384" t="n">
+        <v>43330.05078125</v>
+      </c>
+      <c r="E3384" t="n">
+        <v>43869.15234375</v>
+      </c>
+      <c r="F3384" t="n">
+        <v>43869.15234375</v>
+      </c>
+      <c r="G3384" t="n">
+        <v>22452766169</v>
+      </c>
+    </row>
+    <row r="3385">
+      <c r="A3385" s="2" t="n">
+        <v>45282</v>
+      </c>
+      <c r="B3385" t="n">
+        <v>43868.98828125</v>
+      </c>
+      <c r="C3385" t="n">
+        <v>44367.95703125</v>
+      </c>
+      <c r="D3385" t="n">
+        <v>43441.96875</v>
+      </c>
+      <c r="E3385" t="n">
+        <v>43997.90234375</v>
+      </c>
+      <c r="F3385" t="n">
+        <v>43997.90234375</v>
+      </c>
+      <c r="G3385" t="n">
+        <v>21028503216</v>
+      </c>
+    </row>
+    <row r="3386">
+      <c r="A3386" s="2" t="n">
+        <v>45283</v>
+      </c>
+      <c r="B3386" t="n">
+        <v>44012.19921875</v>
+      </c>
+      <c r="C3386" t="n">
+        <v>44015.69921875</v>
+      </c>
+      <c r="D3386" t="n">
+        <v>43351.35546875</v>
+      </c>
+      <c r="E3386" t="n">
+        <v>43739.54296875</v>
+      </c>
+      <c r="F3386" t="n">
+        <v>43739.54296875</v>
+      </c>
+      <c r="G3386" t="n">
+        <v>13507796558</v>
+      </c>
+    </row>
+    <row r="3387">
+      <c r="A3387" s="2" t="n">
+        <v>45284</v>
+      </c>
+      <c r="B3387" t="n">
+        <v>43728.3671875</v>
+      </c>
+      <c r="C3387" t="n">
+        <v>43945.5234375</v>
+      </c>
+      <c r="D3387" t="n">
+        <v>42786.91796875</v>
+      </c>
+      <c r="E3387" t="n">
+        <v>43016.1171875</v>
+      </c>
+      <c r="F3387" t="n">
+        <v>43016.1171875</v>
+      </c>
+      <c r="G3387" t="n">
+        <v>18830554085</v>
+      </c>
+    </row>
+    <row r="3388">
+      <c r="A3388" s="2" t="n">
+        <v>45285</v>
+      </c>
+      <c r="B3388" t="n">
+        <v>43010.57421875</v>
+      </c>
+      <c r="C3388" t="n">
+        <v>43757.15234375</v>
+      </c>
+      <c r="D3388" t="n">
+        <v>42785.6796875</v>
+      </c>
+      <c r="E3388" t="n">
+        <v>43686.7578125</v>
+      </c>
+      <c r="F3388" t="n">
+        <v>43686.7578125</v>
+      </c>
+      <c r="G3388" t="n">
+        <v>21846523904</v>
       </c>
     </row>
   </sheetData>

</xml_diff>